<commit_message>
Perreuil et publi beaucourt
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Calendrier" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="220">
   <si>
     <t>Date</t>
   </si>
@@ -418,250 +418,262 @@
     <t>Dim 16 Juin</t>
   </si>
   <si>
+    <t>Dim 23 Juin</t>
+  </si>
+  <si>
+    <t>Munster Bike Tour à Muhlbach sur Munster</t>
+  </si>
+  <si>
+    <t>Sam 29 Juin</t>
+  </si>
+  <si>
+    <t>12ème Nuit des Gros Mollets à Flaxlanden</t>
+  </si>
+  <si>
+    <t>10ème Nuit des Gros Mollets jeunes à Flaxlanden (poussins à minimes)</t>
+  </si>
+  <si>
+    <t>29 et 30 Juin</t>
+  </si>
+  <si>
+    <t>Championnat Fédéral route à Bouquehault dans le Pas de Calais (62)</t>
+  </si>
+  <si>
+    <t>Dim 30 Juin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTT du Champ du Feu       VeSPA = Vélo et Sport de Plein Air  </t>
+  </si>
+  <si>
+    <t>6 et 7 Juillet</t>
+  </si>
+  <si>
+    <t>Championnat Fédéral à Retzwiller</t>
+  </si>
+  <si>
+    <t>Dim 4 Août</t>
+  </si>
+  <si>
+    <t>Sam 24 Août</t>
+  </si>
+  <si>
+    <t>3ème VTT Peugeot  (dans l'usine Peugeot)</t>
+  </si>
+  <si>
+    <t>Sam 31 Août</t>
+  </si>
+  <si>
+    <t>L'Urbaine VTT - Cernay</t>
+  </si>
+  <si>
+    <t>Dim 1 Septembre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23ème Montée du Floridor, col du Hundsruck à Thann  </t>
+  </si>
+  <si>
+    <t>Dim 8 Septembre</t>
+  </si>
+  <si>
+    <t>11ème Prix de Boron</t>
+  </si>
+  <si>
+    <t>boron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15ème Grimpée du Col Amic à Soultz  </t>
+  </si>
+  <si>
+    <t>Sam 14 Septembre</t>
+  </si>
+  <si>
+    <t>Dim 15 Septembre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19ème Grand Prix Gestimmo à Magstatt le Bas  </t>
+  </si>
+  <si>
+    <t>Championnat Régional de CLM Individuel à Frotey les Lure</t>
+  </si>
+  <si>
+    <t>frotey_clm</t>
+  </si>
+  <si>
+    <t>21 et 22 Septembre</t>
+  </si>
+  <si>
+    <t>Sam 28 Septembre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4ème VTT MS Automobile Rixheim  </t>
+  </si>
+  <si>
+    <t>Dim 29 Septembre</t>
+  </si>
+  <si>
+    <t>Sam 5 Octobre</t>
+  </si>
+  <si>
+    <t>Sam 12 Octobre</t>
+  </si>
+  <si>
+    <t>Dim 13 Octobre</t>
+  </si>
+  <si>
+    <t>2ème Cyclo-cross de Giromagny épreuve FFC ouvetre aux FSGT</t>
+  </si>
+  <si>
+    <t>US Giromagny VTT</t>
+  </si>
+  <si>
+    <t>giromagny</t>
+  </si>
+  <si>
+    <t>Sam 19 Octobre</t>
+  </si>
+  <si>
+    <t>Sam 26 Octobre</t>
+  </si>
+  <si>
+    <t>Sam 9 Novembre</t>
+  </si>
+  <si>
+    <t>Sam 16 Novembre</t>
+  </si>
+  <si>
+    <t>Sam 30 Novembre</t>
+  </si>
+  <si>
+    <t>Dim 8 Décembre</t>
+  </si>
+  <si>
+    <t>Sam 14 Décembre</t>
+  </si>
+  <si>
+    <t>Dim 21 Décembre</t>
+  </si>
+  <si>
+    <t>2ème Cyclo-cross du Gloeckelsberg</t>
+  </si>
+  <si>
+    <t>Dim 31 Mars</t>
+  </si>
+  <si>
+    <t>Sam 13 Avril</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27ème Grand Prix Gestimmo à Magstatt le bas  </t>
+  </si>
+  <si>
+    <t>Montreux-Vieux à Vélo</t>
+  </si>
+  <si>
+    <t>Lun 10 Juin</t>
+  </si>
+  <si>
+    <t>La Staff à Staffelfelden</t>
+  </si>
+  <si>
+    <t>Grimpée de St Alexis à Riquewihr</t>
+  </si>
+  <si>
+    <t>riquewihr</t>
+  </si>
+  <si>
+    <t>2ème Nuit des Gros Mollets Marathon solo à Flaxlanden</t>
+  </si>
+  <si>
+    <t>2ème Nuit des Gros Mollets pour VTT avec assistance électrique</t>
+  </si>
+  <si>
+    <t>danjoutin</t>
+  </si>
+  <si>
+    <t>seppois</t>
+  </si>
+  <si>
+    <t>fontaine</t>
+  </si>
+  <si>
+    <t>kruth</t>
+  </si>
+  <si>
+    <t>eteimbes</t>
+  </si>
+  <si>
+    <t>vauthiermont</t>
+  </si>
+  <si>
+    <t>lure</t>
+  </si>
+  <si>
+    <t>frotey</t>
+  </si>
+  <si>
+    <t>bourogne</t>
+  </si>
+  <si>
+    <t>rougemont</t>
+  </si>
+  <si>
+    <t>nommay</t>
+  </si>
+  <si>
+    <t>19 et 20 Janvier</t>
+  </si>
+  <si>
+    <t>Dim 7 Juillet</t>
+  </si>
+  <si>
+    <t>Dim 21 Juillet</t>
+  </si>
+  <si>
+    <t>Sam 23 Novembre</t>
+  </si>
+  <si>
+    <t>Sam 7 Septembre</t>
+  </si>
+  <si>
+    <t>Prix du Garage Wadel</t>
+  </si>
+  <si>
+    <t>VTT du Centenaire de la SSOL</t>
+  </si>
+  <si>
+    <t>Les 3h VTT du VSCA</t>
+  </si>
+  <si>
+    <t>AS de L'Allan</t>
+  </si>
+  <si>
+    <t>Championnat Fédéral 2019</t>
+  </si>
+  <si>
+    <t>31 Mai et 1 Juin</t>
+  </si>
+  <si>
+    <t>Trophée National des Finances</t>
+  </si>
+  <si>
+    <t>finances</t>
+  </si>
+  <si>
+    <t>Sam 13 Juillet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perreuil (71) </t>
+  </si>
+  <si>
+    <t>Cycling Eco Team</t>
+  </si>
+  <si>
+    <t>perreuil</t>
+  </si>
+  <si>
+    <t>Championnat régional Bourgogne Franche-Comté</t>
+  </si>
+  <si>
     <t>Championnat régional</t>
-  </si>
-  <si>
-    <t>Dim 23 Juin</t>
-  </si>
-  <si>
-    <t>Munster Bike Tour à Muhlbach sur Munster</t>
-  </si>
-  <si>
-    <t>Sam 29 Juin</t>
-  </si>
-  <si>
-    <t>12ème Nuit des Gros Mollets à Flaxlanden</t>
-  </si>
-  <si>
-    <t>10ème Nuit des Gros Mollets jeunes à Flaxlanden (poussins à minimes)</t>
-  </si>
-  <si>
-    <t>29 et 30 Juin</t>
-  </si>
-  <si>
-    <t>Championnat Fédéral route à Bouquehault dans le Pas de Calais (62)</t>
-  </si>
-  <si>
-    <t>Dim 30 Juin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VTT du Champ du Feu       VeSPA = Vélo et Sport de Plein Air  </t>
-  </si>
-  <si>
-    <t>6 et 7 Juillet</t>
-  </si>
-  <si>
-    <t>Championnat Fédéral à Retzwiller</t>
-  </si>
-  <si>
-    <t>Dim 4 Août</t>
-  </si>
-  <si>
-    <t>Sam 24 Août</t>
-  </si>
-  <si>
-    <t>3ème VTT Peugeot  (dans l'usine Peugeot)</t>
-  </si>
-  <si>
-    <t>Sam 31 Août</t>
-  </si>
-  <si>
-    <t>L'Urbaine VTT - Cernay</t>
-  </si>
-  <si>
-    <t>Dim 1 Septembre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23ème Montée du Floridor, col du Hundsruck à Thann  </t>
-  </si>
-  <si>
-    <t>Dim 8 Septembre</t>
-  </si>
-  <si>
-    <t>11ème Prix de Boron</t>
-  </si>
-  <si>
-    <t>boron</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15ème Grimpée du Col Amic à Soultz  </t>
-  </si>
-  <si>
-    <t>Sam 14 Septembre</t>
-  </si>
-  <si>
-    <t>Dim 15 Septembre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19ème Grand Prix Gestimmo à Magstatt le Bas  </t>
-  </si>
-  <si>
-    <t>Championnat Régional de CLM Individuel à Frotey les Lure</t>
-  </si>
-  <si>
-    <t>frotey_clm</t>
-  </si>
-  <si>
-    <t>21 et 22 Septembre</t>
-  </si>
-  <si>
-    <t>Sam 28 Septembre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4ème VTT MS Automobile Rixheim  </t>
-  </si>
-  <si>
-    <t>Dim 29 Septembre</t>
-  </si>
-  <si>
-    <t>Sam 5 Octobre</t>
-  </si>
-  <si>
-    <t>Sam 12 Octobre</t>
-  </si>
-  <si>
-    <t>Dim 13 Octobre</t>
-  </si>
-  <si>
-    <t>2ème Cyclo-cross de Giromagny épreuve FFC ouvetre aux FSGT</t>
-  </si>
-  <si>
-    <t>US Giromagny VTT</t>
-  </si>
-  <si>
-    <t>giromagny</t>
-  </si>
-  <si>
-    <t>Sam 19 Octobre</t>
-  </si>
-  <si>
-    <t>Sam 26 Octobre</t>
-  </si>
-  <si>
-    <t>Sam 9 Novembre</t>
-  </si>
-  <si>
-    <t>Sam 16 Novembre</t>
-  </si>
-  <si>
-    <t>Sam 30 Novembre</t>
-  </si>
-  <si>
-    <t>Dim 8 Décembre</t>
-  </si>
-  <si>
-    <t>Sam 14 Décembre</t>
-  </si>
-  <si>
-    <t>Dim 21 Décembre</t>
-  </si>
-  <si>
-    <t>2ème Cyclo-cross du Gloeckelsberg</t>
-  </si>
-  <si>
-    <t>Dim 31 Mars</t>
-  </si>
-  <si>
-    <t>Sam 13 Avril</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27ème Grand Prix Gestimmo à Magstatt le bas  </t>
-  </si>
-  <si>
-    <t>Montreux-Vieux à Vélo</t>
-  </si>
-  <si>
-    <t>Lun 10 Juin</t>
-  </si>
-  <si>
-    <t>La Staff à Staffelfelden</t>
-  </si>
-  <si>
-    <t>Grimpée de St Alexis à Riquewihr</t>
-  </si>
-  <si>
-    <t>riquewihr</t>
-  </si>
-  <si>
-    <t>2ème Nuit des Gros Mollets Marathon solo à Flaxlanden</t>
-  </si>
-  <si>
-    <t>2ème Nuit des Gros Mollets pour VTT avec assistance électrique</t>
-  </si>
-  <si>
-    <t>danjoutin</t>
-  </si>
-  <si>
-    <t>seppois</t>
-  </si>
-  <si>
-    <t>fontaine</t>
-  </si>
-  <si>
-    <t>kruth</t>
-  </si>
-  <si>
-    <t>eteimbes</t>
-  </si>
-  <si>
-    <t>vauthiermont</t>
-  </si>
-  <si>
-    <t>lure</t>
-  </si>
-  <si>
-    <t>frotey</t>
-  </si>
-  <si>
-    <t>bourogne</t>
-  </si>
-  <si>
-    <t>rougemont</t>
-  </si>
-  <si>
-    <t>nommay</t>
-  </si>
-  <si>
-    <t>19 et 20 Janvier</t>
-  </si>
-  <si>
-    <t>Dim 7 Juillet</t>
-  </si>
-  <si>
-    <t>Dim 21 Juillet</t>
-  </si>
-  <si>
-    <t>Sam 23 Novembre</t>
-  </si>
-  <si>
-    <t>Sam 7 Septembre</t>
-  </si>
-  <si>
-    <t>Prix du Garage Wadel</t>
-  </si>
-  <si>
-    <t>VTT du Centenaire de la SSOL</t>
-  </si>
-  <si>
-    <t>Les 3h VTT du VSCA</t>
-  </si>
-  <si>
-    <t>AS de L'Allan</t>
-  </si>
-  <si>
-    <t>Championnat Fédéral 2019</t>
-  </si>
-  <si>
-    <t>31 Mai et 1 Juin</t>
-  </si>
-  <si>
-    <t>Trophée National des Finances</t>
-  </si>
-  <si>
-    <t>finances</t>
-  </si>
-  <si>
-    <t>Sam 13 Juillet</t>
   </si>
 </sst>
 </file>
@@ -1524,10 +1536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+    <sheetView tabSelected="1" topLeftCell="C12" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1561,10 +1573,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D2" t="s">
         <v>46</v>
@@ -1595,7 +1607,7 @@
         <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -1621,12 +1633,12 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -1638,7 +1650,7 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1655,12 +1667,12 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B8" t="s">
         <v>113</v>
@@ -1689,7 +1701,7 @@
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1731,7 +1743,7 @@
         <v>117</v>
       </c>
       <c r="B12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
@@ -1757,7 +1769,7 @@
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1774,7 +1786,7 @@
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1791,7 +1803,7 @@
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1813,61 +1825,64 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B17" t="s">
-        <v>183</v>
+        <v>215</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>216</v>
       </c>
       <c r="D17" t="s">
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
+        <v>217</v>
+      </c>
+      <c r="F17" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>182</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>104</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>212</v>
+        <v>126</v>
       </c>
       <c r="B19" t="s">
-        <v>213</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D19" t="s">
         <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>214</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>127</v>
+        <v>211</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>212</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -1876,7 +1891,7 @@
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>199</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1884,70 +1899,67 @@
         <v>127</v>
       </c>
       <c r="B21" t="s">
-        <v>184</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>64</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B22" t="s">
-        <v>209</v>
+        <v>183</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E22" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>185</v>
+        <v>129</v>
       </c>
       <c r="B23" t="s">
-        <v>130</v>
+        <v>208</v>
       </c>
       <c r="C23" t="s">
-        <v>131</v>
+        <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>133</v>
+        <v>184</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>130</v>
       </c>
       <c r="C24" t="s">
-        <v>5</v>
+        <v>131</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>66</v>
-      </c>
-      <c r="F24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1955,75 +1967,78 @@
         <v>133</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>89</v>
+        <v>66</v>
+      </c>
+      <c r="F25" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E26" t="s">
-        <v>191</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B27" t="s">
-        <v>136</v>
+        <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>90</v>
+        <v>6</v>
+      </c>
+      <c r="E27" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B28" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C28" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D28" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" t="s">
-        <v>70</v>
+        <v>16</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
+        <v>136</v>
+      </c>
+      <c r="B29" t="s">
         <v>137</v>
-      </c>
-      <c r="B29" t="s">
-        <v>139</v>
       </c>
       <c r="C29" t="s">
         <v>28</v>
@@ -2032,15 +2047,15 @@
         <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>189</v>
+      <c r="A30" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" t="s">
+        <v>138</v>
       </c>
       <c r="C30" t="s">
         <v>28</v>
@@ -2049,15 +2064,15 @@
         <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C31" t="s">
         <v>28</v>
@@ -2066,570 +2081,587 @@
         <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>141</v>
+        <v>189</v>
+      </c>
+      <c r="C32" t="s">
+        <v>28</v>
       </c>
       <c r="D32" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" t="s">
-        <v>14</v>
+        <v>139</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>140</v>
       </c>
       <c r="D33" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E33" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>143</v>
+        <v>29</v>
       </c>
       <c r="C34" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D34" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E34" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="C35" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D35" t="s">
         <v>3</v>
       </c>
       <c r="E35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C36" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" t="s">
-        <v>203</v>
-      </c>
-      <c r="B36" t="s">
-        <v>186</v>
-      </c>
-      <c r="C36" t="s">
-        <v>34</v>
-      </c>
-      <c r="D36" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>215</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>31</v>
+        <v>202</v>
+      </c>
+      <c r="B37" t="s">
+        <v>185</v>
       </c>
       <c r="C37" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D37" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="E37" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>204</v>
-      </c>
-      <c r="B38" t="s">
-        <v>187</v>
+        <v>214</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="C38" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D38" t="s">
         <v>33</v>
       </c>
       <c r="E38" t="s">
-        <v>188</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>146</v>
+        <v>203</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>186</v>
       </c>
       <c r="C39" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D39" t="s">
         <v>33</v>
       </c>
       <c r="E39" t="s">
-        <v>84</v>
+        <v>187</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B40" t="s">
-        <v>148</v>
+        <v>35</v>
       </c>
       <c r="C40" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="D40" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="E40" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B41" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C41" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D41" t="s">
         <v>3</v>
       </c>
       <c r="E41" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>149</v>
       </c>
       <c r="C42" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D42" t="s">
         <v>3</v>
       </c>
       <c r="E42" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C43" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D43" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E43" t="s">
-        <v>200</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>206</v>
+        <v>150</v>
       </c>
       <c r="B44" t="s">
-        <v>152</v>
+        <v>41</v>
       </c>
       <c r="C44" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="E44" t="s">
-        <v>99</v>
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>153</v>
+        <v>205</v>
       </c>
       <c r="B45" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C45" t="s">
-        <v>210</v>
+        <v>39</v>
       </c>
       <c r="D45" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="E45" t="s">
-        <v>155</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
+        <v>152</v>
+      </c>
+      <c r="B46" t="s">
         <v>153</v>
       </c>
-      <c r="B46" t="s">
-        <v>42</v>
-      </c>
       <c r="C46" t="s">
-        <v>10</v>
+        <v>209</v>
       </c>
       <c r="D46" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E46" t="s">
-        <v>81</v>
+        <v>154</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B47" t="s">
-        <v>156</v>
+        <v>42</v>
       </c>
       <c r="C47" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="D47" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="E47" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B48" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C48" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D48" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="E48" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
+        <v>157</v>
+      </c>
+      <c r="B49" t="s">
         <v>158</v>
       </c>
-      <c r="B49" t="s">
-        <v>160</v>
-      </c>
       <c r="C49" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D49" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E49" t="s">
-        <v>161</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B50" t="s">
-        <v>44</v>
+        <v>159</v>
       </c>
       <c r="C50" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="D50" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="E50" t="s">
-        <v>82</v>
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B51" t="s">
-        <v>164</v>
+        <v>44</v>
       </c>
       <c r="C51" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="D51" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="E51" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B52" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
       <c r="C52" t="s">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E52" t="s">
-        <v>201</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B53" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C53" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="D53" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="E53" t="s">
-        <v>86</v>
+        <v>200</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C54" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="D54" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="E54" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B55" t="s">
-        <v>169</v>
+        <v>50</v>
       </c>
       <c r="C55" t="s">
-        <v>170</v>
+        <v>51</v>
       </c>
       <c r="D55" t="s">
         <v>46</v>
       </c>
       <c r="E55" t="s">
-        <v>171</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B56" t="s">
-        <v>52</v>
+        <v>168</v>
       </c>
       <c r="C56" t="s">
-        <v>28</v>
+        <v>169</v>
       </c>
       <c r="D56" t="s">
         <v>46</v>
       </c>
       <c r="E56" t="s">
-        <v>74</v>
+        <v>170</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C57" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D57" t="s">
         <v>46</v>
       </c>
       <c r="E57" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B58" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C58" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="D58" t="s">
         <v>46</v>
       </c>
       <c r="E58" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C59" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="D59" t="s">
         <v>46</v>
       </c>
       <c r="E59" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>205</v>
+        <v>174</v>
       </c>
       <c r="B60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C60" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D60" t="s">
         <v>46</v>
       </c>
       <c r="E60" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
       <c r="B61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C61" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D61" t="s">
         <v>46</v>
       </c>
       <c r="E61" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B62" t="s">
-        <v>103</v>
+        <v>59</v>
       </c>
       <c r="C62" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="D62" t="s">
         <v>46</v>
       </c>
       <c r="E62" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B63" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="C63" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D63" t="s">
         <v>46</v>
       </c>
       <c r="E63" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B64" t="s">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="C64" t="s">
-        <v>96</v>
+        <v>34</v>
       </c>
       <c r="D64" t="s">
         <v>46</v>
       </c>
       <c r="E64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>178</v>
+      </c>
+      <c r="B65" t="s">
+        <v>179</v>
+      </c>
+      <c r="C65" t="s">
+        <v>96</v>
+      </c>
+      <c r="D65" t="s">
+        <v>46</v>
+      </c>
+      <c r="E65" t="s">
         <v>97</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E27" r:id="rId1"/>
+    <hyperlink ref="E28" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
naming championnats et typo
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -640,9 +640,6 @@
     <t>VTT du Centenaire de la SSOL</t>
   </si>
   <si>
-    <t>Les 3h VTT du VSCA</t>
-  </si>
-  <si>
     <t>AS de L'Allan</t>
   </si>
   <si>
@@ -670,10 +667,13 @@
     <t>perreuil</t>
   </si>
   <si>
-    <t>Championnat régional Bourgogne Franche-Comté</t>
-  </si>
-  <si>
-    <t>Championnat régional</t>
+    <t>Championnat d'Alsace FSGT</t>
+  </si>
+  <si>
+    <t>Championnat Bourgogne Franche-Comté FSGT</t>
+  </si>
+  <si>
+    <t>Les 3h VTT du VCSA</t>
   </si>
 </sst>
 </file>
@@ -1528,7 +1528,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1538,8 +1538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C12" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1576,7 +1576,7 @@
         <v>201</v>
       </c>
       <c r="B2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D2" t="s">
         <v>46</v>
@@ -1828,16 +1828,16 @@
         <v>122</v>
       </c>
       <c r="B17" t="s">
+        <v>214</v>
+      </c>
+      <c r="C17" t="s">
         <v>215</v>
-      </c>
-      <c r="C17" t="s">
-        <v>216</v>
       </c>
       <c r="D17" t="s">
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F17" t="s">
         <v>218</v>
@@ -1879,10 +1879,10 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
+        <v>210</v>
+      </c>
+      <c r="B20" t="s">
         <v>211</v>
-      </c>
-      <c r="B20" t="s">
-        <v>212</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -1891,7 +1891,7 @@
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1933,7 +1933,7 @@
         <v>129</v>
       </c>
       <c r="B23" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
@@ -1979,7 +1979,7 @@
         <v>66</v>
       </c>
       <c r="F25" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2185,7 +2185,7 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>31</v>
@@ -2327,7 +2327,7 @@
         <v>153</v>
       </c>
       <c r="C46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D46" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Calendrier correspondants et geko bikes
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="224">
   <si>
     <t>Date</t>
   </si>
@@ -674,6 +674,18 @@
   </si>
   <si>
     <t>Les 3h VTT du VCSA</t>
+  </si>
+  <si>
+    <t>Dim 6 Octobre</t>
+  </si>
+  <si>
+    <t>La Geko Bikes</t>
+  </si>
+  <si>
+    <t>UC Lutterbach VTT</t>
+  </si>
+  <si>
+    <t>gekobikes</t>
   </si>
 </sst>
 </file>
@@ -1528,7 +1540,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1536,10 +1548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2474,188 +2486,205 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>166</v>
+        <v>220</v>
       </c>
       <c r="B55" t="s">
-        <v>50</v>
+        <v>221</v>
       </c>
       <c r="C55" t="s">
-        <v>51</v>
+        <v>222</v>
       </c>
       <c r="D55" t="s">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="E55" t="s">
-        <v>75</v>
+        <v>223</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B56" t="s">
-        <v>168</v>
+        <v>50</v>
       </c>
       <c r="C56" t="s">
-        <v>169</v>
+        <v>51</v>
       </c>
       <c r="D56" t="s">
         <v>46</v>
       </c>
       <c r="E56" t="s">
-        <v>170</v>
+        <v>75</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B57" t="s">
-        <v>52</v>
+        <v>168</v>
       </c>
       <c r="C57" t="s">
-        <v>28</v>
+        <v>169</v>
       </c>
       <c r="D57" t="s">
         <v>46</v>
       </c>
       <c r="E57" t="s">
-        <v>74</v>
+        <v>170</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B58" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C58" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D58" t="s">
         <v>46</v>
       </c>
       <c r="E58" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B59" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C59" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="D59" t="s">
         <v>46</v>
       </c>
       <c r="E59" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C60" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="D60" t="s">
         <v>46</v>
       </c>
       <c r="E60" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>204</v>
+        <v>174</v>
       </c>
       <c r="B61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C61" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D61" t="s">
         <v>46</v>
       </c>
       <c r="E61" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>175</v>
+        <v>204</v>
       </c>
       <c r="B62" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C62" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D62" t="s">
         <v>46</v>
       </c>
       <c r="E62" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B63" t="s">
-        <v>103</v>
+        <v>59</v>
       </c>
       <c r="C63" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="D63" t="s">
         <v>46</v>
       </c>
       <c r="E63" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B64" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="C64" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D64" t="s">
         <v>46</v>
       </c>
       <c r="E64" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B65" t="s">
-        <v>179</v>
+        <v>60</v>
       </c>
       <c r="C65" t="s">
-        <v>96</v>
+        <v>34</v>
       </c>
       <c r="D65" t="s">
         <v>46</v>
       </c>
       <c r="E65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>178</v>
+      </c>
+      <c r="B66" t="s">
+        <v>179</v>
+      </c>
+      <c r="C66" t="s">
+        <v>96</v>
+      </c>
+      <c r="D66" t="s">
+        <v>46</v>
+      </c>
+      <c r="E66" t="s">
         <v>97</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new date for fontaine
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="225">
   <si>
     <t>Date</t>
   </si>
@@ -556,136 +556,139 @@
     <t>2ème Cyclo-cross du Gloeckelsberg</t>
   </si>
   <si>
+    <t>Sam 13 Avril</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27ème Grand Prix Gestimmo à Magstatt le bas  </t>
+  </si>
+  <si>
+    <t>Montreux-Vieux à Vélo</t>
+  </si>
+  <si>
+    <t>Lun 10 Juin</t>
+  </si>
+  <si>
+    <t>La Staff à Staffelfelden</t>
+  </si>
+  <si>
+    <t>Grimpée de St Alexis à Riquewihr</t>
+  </si>
+  <si>
+    <t>riquewihr</t>
+  </si>
+  <si>
+    <t>2ème Nuit des Gros Mollets Marathon solo à Flaxlanden</t>
+  </si>
+  <si>
+    <t>2ème Nuit des Gros Mollets pour VTT avec assistance électrique</t>
+  </si>
+  <si>
+    <t>danjoutin</t>
+  </si>
+  <si>
+    <t>seppois</t>
+  </si>
+  <si>
+    <t>fontaine</t>
+  </si>
+  <si>
+    <t>kruth</t>
+  </si>
+  <si>
+    <t>eteimbes</t>
+  </si>
+  <si>
+    <t>vauthiermont</t>
+  </si>
+  <si>
+    <t>lure</t>
+  </si>
+  <si>
+    <t>frotey</t>
+  </si>
+  <si>
+    <t>bourogne</t>
+  </si>
+  <si>
+    <t>rougemont</t>
+  </si>
+  <si>
+    <t>nommay</t>
+  </si>
+  <si>
+    <t>19 et 20 Janvier</t>
+  </si>
+  <si>
+    <t>Dim 7 Juillet</t>
+  </si>
+  <si>
+    <t>Dim 21 Juillet</t>
+  </si>
+  <si>
+    <t>Sam 23 Novembre</t>
+  </si>
+  <si>
+    <t>Sam 7 Septembre</t>
+  </si>
+  <si>
+    <t>Prix du Garage Wadel</t>
+  </si>
+  <si>
+    <t>VTT du Centenaire de la SSOL</t>
+  </si>
+  <si>
+    <t>AS de L'Allan</t>
+  </si>
+  <si>
+    <t>Championnat Fédéral 2019</t>
+  </si>
+  <si>
+    <t>31 Mai et 1 Juin</t>
+  </si>
+  <si>
+    <t>Trophée National des Finances</t>
+  </si>
+  <si>
+    <t>finances</t>
+  </si>
+  <si>
+    <t>Sam 13 Juillet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perreuil (71) </t>
+  </si>
+  <si>
+    <t>Cycling Eco Team</t>
+  </si>
+  <si>
+    <t>perreuil</t>
+  </si>
+  <si>
+    <t>Championnat d'Alsace FSGT</t>
+  </si>
+  <si>
+    <t>Championnat Bourgogne Franche-Comté FSGT</t>
+  </si>
+  <si>
+    <t>Les 3h VTT du VCSA</t>
+  </si>
+  <si>
+    <t>Dim 6 Octobre</t>
+  </si>
+  <si>
+    <t>La Geko Bikes</t>
+  </si>
+  <si>
+    <t>UC Lutterbach VTT</t>
+  </si>
+  <si>
+    <t>gekobikes</t>
+  </si>
+  <si>
+    <t>Nouvelle date !</t>
+  </si>
+  <si>
     <t>Dim 31 Mars</t>
-  </si>
-  <si>
-    <t>Sam 13 Avril</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27ème Grand Prix Gestimmo à Magstatt le bas  </t>
-  </si>
-  <si>
-    <t>Montreux-Vieux à Vélo</t>
-  </si>
-  <si>
-    <t>Lun 10 Juin</t>
-  </si>
-  <si>
-    <t>La Staff à Staffelfelden</t>
-  </si>
-  <si>
-    <t>Grimpée de St Alexis à Riquewihr</t>
-  </si>
-  <si>
-    <t>riquewihr</t>
-  </si>
-  <si>
-    <t>2ème Nuit des Gros Mollets Marathon solo à Flaxlanden</t>
-  </si>
-  <si>
-    <t>2ème Nuit des Gros Mollets pour VTT avec assistance électrique</t>
-  </si>
-  <si>
-    <t>danjoutin</t>
-  </si>
-  <si>
-    <t>seppois</t>
-  </si>
-  <si>
-    <t>fontaine</t>
-  </si>
-  <si>
-    <t>kruth</t>
-  </si>
-  <si>
-    <t>eteimbes</t>
-  </si>
-  <si>
-    <t>vauthiermont</t>
-  </si>
-  <si>
-    <t>lure</t>
-  </si>
-  <si>
-    <t>frotey</t>
-  </si>
-  <si>
-    <t>bourogne</t>
-  </si>
-  <si>
-    <t>rougemont</t>
-  </si>
-  <si>
-    <t>nommay</t>
-  </si>
-  <si>
-    <t>19 et 20 Janvier</t>
-  </si>
-  <si>
-    <t>Dim 7 Juillet</t>
-  </si>
-  <si>
-    <t>Dim 21 Juillet</t>
-  </si>
-  <si>
-    <t>Sam 23 Novembre</t>
-  </si>
-  <si>
-    <t>Sam 7 Septembre</t>
-  </si>
-  <si>
-    <t>Prix du Garage Wadel</t>
-  </si>
-  <si>
-    <t>VTT du Centenaire de la SSOL</t>
-  </si>
-  <si>
-    <t>AS de L'Allan</t>
-  </si>
-  <si>
-    <t>Championnat Fédéral 2019</t>
-  </si>
-  <si>
-    <t>31 Mai et 1 Juin</t>
-  </si>
-  <si>
-    <t>Trophée National des Finances</t>
-  </si>
-  <si>
-    <t>finances</t>
-  </si>
-  <si>
-    <t>Sam 13 Juillet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Perreuil (71) </t>
-  </si>
-  <si>
-    <t>Cycling Eco Team</t>
-  </si>
-  <si>
-    <t>perreuil</t>
-  </si>
-  <si>
-    <t>Championnat d'Alsace FSGT</t>
-  </si>
-  <si>
-    <t>Championnat Bourgogne Franche-Comté FSGT</t>
-  </si>
-  <si>
-    <t>Les 3h VTT du VCSA</t>
-  </si>
-  <si>
-    <t>Dim 6 Octobre</t>
-  </si>
-  <si>
-    <t>La Geko Bikes</t>
-  </si>
-  <si>
-    <t>UC Lutterbach VTT</t>
-  </si>
-  <si>
-    <t>gekobikes</t>
   </si>
 </sst>
 </file>
@@ -1550,8 +1553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1585,10 +1588,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D2" t="s">
         <v>46</v>
@@ -1615,54 +1618,57 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
+        <v>224</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B4" t="s">
-        <v>207</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>180</v>
+        <v>110</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1679,12 +1685,12 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B8" t="s">
         <v>113</v>
@@ -1713,7 +1719,7 @@
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1755,7 +1761,7 @@
         <v>117</v>
       </c>
       <c r="B12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
@@ -1781,7 +1787,7 @@
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1798,7 +1804,7 @@
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1815,7 +1821,7 @@
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1840,19 +1846,19 @@
         <v>122</v>
       </c>
       <c r="B17" t="s">
+        <v>213</v>
+      </c>
+      <c r="C17" t="s">
         <v>214</v>
-      </c>
-      <c r="C17" t="s">
-        <v>215</v>
       </c>
       <c r="D17" t="s">
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1860,7 +1866,7 @@
         <v>125</v>
       </c>
       <c r="B18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C18" t="s">
         <v>21</v>
@@ -1891,10 +1897,10 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
+        <v>209</v>
+      </c>
+      <c r="B20" t="s">
         <v>210</v>
-      </c>
-      <c r="B20" t="s">
-        <v>211</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -1903,7 +1909,7 @@
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1920,7 +1926,7 @@
         <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1928,7 +1934,7 @@
         <v>127</v>
       </c>
       <c r="B22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
@@ -1945,7 +1951,7 @@
         <v>129</v>
       </c>
       <c r="B23" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
@@ -1959,7 +1965,7 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B24" t="s">
         <v>130</v>
@@ -1991,7 +1997,7 @@
         <v>66</v>
       </c>
       <c r="F25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2025,7 +2031,7 @@
         <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2084,7 +2090,7 @@
         <v>136</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C31" t="s">
         <v>28</v>
@@ -2101,7 +2107,7 @@
         <v>136</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C32" t="s">
         <v>28</v>
@@ -2180,10 +2186,10 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B37" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C37" t="s">
         <v>34</v>
@@ -2197,7 +2203,7 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>31</v>
@@ -2214,10 +2220,10 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B39" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C39" t="s">
         <v>26</v>
@@ -2226,7 +2232,7 @@
         <v>33</v>
       </c>
       <c r="E39" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -2311,12 +2317,12 @@
         <v>6</v>
       </c>
       <c r="E44" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B45" t="s">
         <v>151</v>
@@ -2339,7 +2345,7 @@
         <v>153</v>
       </c>
       <c r="C46" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D46" t="s">
         <v>6</v>
@@ -2464,7 +2470,7 @@
         <v>6</v>
       </c>
       <c r="E53" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2486,19 +2492,19 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
+        <v>219</v>
+      </c>
+      <c r="B55" t="s">
         <v>220</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>221</v>
-      </c>
-      <c r="C55" t="s">
-        <v>222</v>
       </c>
       <c r="D55" t="s">
         <v>3</v>
       </c>
       <c r="E55" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2605,7 +2611,7 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B62" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
remove - nouvelle date -
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="225">
   <si>
     <t>Date</t>
   </si>
@@ -671,9 +671,6 @@
   </si>
   <si>
     <t>gekobikes</t>
-  </si>
-  <si>
-    <t>Nouvelle date !</t>
   </si>
   <si>
     <t>Dim 17 Mars</t>
@@ -1556,8 +1553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1622,7 +1619,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1635,9 +1632,6 @@
       </c>
       <c r="E4" t="s">
         <v>188</v>
-      </c>
-      <c r="F4" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1691,7 +1685,7 @@
         <v>189</v>
       </c>
       <c r="F7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1847,7 +1841,7 @@
         <v>122</v>
       </c>
       <c r="F16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2062,7 +2056,7 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B29" t="s">
         <v>134</v>
@@ -2079,7 +2073,7 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B30" t="s">
         <v>135</v>
@@ -2096,7 +2090,7 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>184</v>
@@ -2111,12 +2105,12 @@
         <v>99</v>
       </c>
       <c r="F31" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>185</v>
@@ -2232,7 +2226,7 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B39" t="s">
         <v>182</v>
@@ -2371,7 +2365,7 @@
         <v>149</v>
       </c>
       <c r="B47" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C47" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
ordre grimpee et gentlemen
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7548"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
   </bookViews>
   <sheets>
     <sheet name="Calendrier" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -1573,7 +1573,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1583,18 +1583,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:XFD55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="66.88671875" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" customWidth="1"/>
-    <col min="5" max="5" width="28.5546875" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" customWidth="1"/>
-    <col min="7" max="7" width="65.88671875" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="66.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="65.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2554,36 +2554,36 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>229</v>
+        <v>158</v>
       </c>
       <c r="B55" t="s">
-        <v>221</v>
+        <v>45</v>
       </c>
       <c r="C55" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="D55" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E55" t="s">
-        <v>189</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>158</v>
+        <v>229</v>
       </c>
       <c r="B56" t="s">
-        <v>45</v>
+        <v>221</v>
       </c>
       <c r="C56" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="D56" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="E56" t="s">
-        <v>82</v>
+        <v>189</v>
       </c>
     </row>
     <row r="57" spans="1:7">

</xml_diff>

<commit_message>
post reunion changements de date
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7548"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
   </bookViews>
   <sheets>
     <sheet name="Calendrier" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="214">
   <si>
     <t>Date</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Beaucourt OS</t>
   </si>
   <si>
-    <t>Les Mordus</t>
-  </si>
-  <si>
     <t>Randonnée</t>
   </si>
   <si>
@@ -277,391 +274,388 @@
     <t>danjoutin</t>
   </si>
   <si>
+    <t>fontaine</t>
+  </si>
+  <si>
+    <t>eteimbes</t>
+  </si>
+  <si>
+    <t>vauthiermont</t>
+  </si>
+  <si>
+    <t>lure</t>
+  </si>
+  <si>
+    <t>frotey</t>
+  </si>
+  <si>
+    <t>rougemont</t>
+  </si>
+  <si>
+    <t>nommay</t>
+  </si>
+  <si>
+    <t>UC Lutterbach VTT</t>
+  </si>
+  <si>
+    <t>champduf</t>
+  </si>
+  <si>
+    <t>FileNameResults</t>
+  </si>
+  <si>
+    <t>Championnat Fédéral 2020 à Nogent sur Seine, Aube Grand Est</t>
+  </si>
+  <si>
+    <t>UC Nogentaise</t>
+  </si>
+  <si>
+    <t>Sam 21 Mars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTT des Transports Portmann  </t>
+  </si>
+  <si>
+    <t>Dim 22 Mars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28ème Prix Agri-Center à Jettingen  </t>
+  </si>
+  <si>
+    <t>jettingen</t>
+  </si>
+  <si>
+    <t>Sam 28 Mars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grand Prix du Grand Hamster  </t>
+  </si>
+  <si>
+    <t>Dim 5 Avril</t>
+  </si>
+  <si>
+    <t>Dim 12 Avril</t>
+  </si>
+  <si>
+    <t>Circuit du Vallon en 2 étapes, à Eteimbes</t>
+  </si>
+  <si>
+    <t>Dim 26 Avril</t>
+  </si>
+  <si>
+    <t>Dim 3 Mai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prix du Garage Wadel à Retzwiller  </t>
+  </si>
+  <si>
+    <t>Ven 8 Mai</t>
+  </si>
+  <si>
+    <t>Dim 10 Mai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grand Prix Dépannage 70 à Frotey les Lure  </t>
+  </si>
+  <si>
+    <t>Ven 15 Mai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nocturne de Lure (ouvert aux cadets)  </t>
+  </si>
+  <si>
+    <t>Sam 23 Mai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29ème Grand Prix Gestimmo à Magstatt le bas  </t>
+  </si>
+  <si>
+    <t>Dim 24 Mai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyclosportive les Marcaires  </t>
+  </si>
+  <si>
+    <t>Sam 6 Juin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les 3h VTT du VCSA  </t>
+  </si>
+  <si>
+    <t>Dim 21 Juin</t>
+  </si>
+  <si>
+    <t>La Rando Tour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Munster Bike Tour à Muhlbach sur Munster  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTT à Retzwiller  </t>
+  </si>
+  <si>
+    <t>retzwillerbis</t>
+  </si>
+  <si>
+    <t>Sam 27 Juin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Randonnée du Champ du Feu  </t>
+  </si>
+  <si>
+    <t>Dim 28 Juin</t>
+  </si>
+  <si>
+    <t>Journée Sport et Détente à Beaucourt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTT du Champ du Feu       VeSPA = Vélo et Sport de Plein Air  </t>
+  </si>
+  <si>
+    <t>4 et 5 Juillet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Championnat Fédéral  à Saint Chinian et Prades sur Vernazobre (Hérault)  </t>
+  </si>
+  <si>
+    <t>Sam 4 Juillet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12ème Nuit des Gros Mollets à Flaxlanden  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10ème Nuit des Gros Mollets jeunes à Flaxlanden (poussins à minimes)  </t>
+  </si>
+  <si>
+    <t>goros_mollets_jeunes</t>
+  </si>
+  <si>
+    <t>Dim 5 Juillet</t>
+  </si>
+  <si>
+    <t>Petit Ballon Rando Tour</t>
+  </si>
+  <si>
+    <t>rando_tour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1er Grand Prix du Petit Meublard à Bréchaumont  </t>
+  </si>
+  <si>
+    <t>brechaumont</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fédéraux de VTT à La Chapelle St Aubin (Sarthe)  </t>
+  </si>
+  <si>
+    <t>federaux</t>
+  </si>
+  <si>
+    <t>Sam 11 Juillet</t>
+  </si>
+  <si>
+    <t>Grimpée des Bagenelles</t>
+  </si>
+  <si>
+    <t>Dim 12 Juillet</t>
+  </si>
+  <si>
+    <t>Dim 2 Août</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grimpée Le Waldbach, d'Ammerschwihr à Labaroche   </t>
+  </si>
+  <si>
+    <t>Dim 23 Août</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grand Prix d'Ampfersbach  </t>
+  </si>
+  <si>
+    <t>ampfersbach</t>
+  </si>
+  <si>
+    <t>Sam 29 Août</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3ème VTT Peugeot  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">24ème Montée du Floridor, col du Hundsruck à Thann  </t>
+  </si>
+  <si>
+    <t>Dim 30 Août</t>
+  </si>
+  <si>
+    <t>Sam 5 Septembre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'Urbaine VTT - Cernay  </t>
+  </si>
+  <si>
+    <t>Dim 6 Septembre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTT des Bords de l'Ill (mixte sous l'égide de la FFC)  </t>
+  </si>
+  <si>
+    <t>ste_croix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11ème Prix de Boron  </t>
+  </si>
+  <si>
+    <t>AS de l'Allan</t>
+  </si>
+  <si>
+    <t>Sam 12 Septembre</t>
+  </si>
+  <si>
+    <t>15ème Grimpée du Col Amic à Soultz</t>
+  </si>
+  <si>
+    <t>Dim 13 Septembre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grand Prix VTT de Mollau  </t>
+  </si>
+  <si>
+    <t>Cyclo-cross de la Ville de Wittenheim</t>
+  </si>
+  <si>
+    <t>Sam 26 Septembre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5ème VTT MS Automobile Rixheim  </t>
+  </si>
+  <si>
+    <t>Dim 27 Septembre</t>
+  </si>
+  <si>
+    <t>La Geko-Bikes à Didenheim</t>
+  </si>
+  <si>
+    <t>didenheim</t>
+  </si>
+  <si>
+    <t>Sam 3 Octobre</t>
+  </si>
+  <si>
+    <t>Sam 10 Octobre</t>
+  </si>
+  <si>
+    <t>Cyclo-cross de Morschwiller le bas</t>
+  </si>
+  <si>
+    <t>Dim 11 Octobre</t>
+  </si>
+  <si>
+    <t>2ème Cyclo-cross de Giromagny. Epreuve FFC ouverte aux FSGT</t>
+  </si>
+  <si>
+    <t>Sam 17 Octobre</t>
+  </si>
+  <si>
+    <t>Cyclo-cross de Heimsbrunn</t>
+  </si>
+  <si>
+    <t>Sam 24 Octobre</t>
+  </si>
+  <si>
+    <t>Sam 7 Novembre</t>
+  </si>
+  <si>
+    <t>Sam 14 Novembre</t>
+  </si>
+  <si>
+    <t>Sam 21 Novembre</t>
+  </si>
+  <si>
+    <t>Sam 28 Novembre</t>
+  </si>
+  <si>
+    <t>Dim 6 Décembre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyclo-cross du Bief de Niffer, Prix Vélotop Kembs  </t>
+  </si>
+  <si>
+    <t>Sam 12 Décembre</t>
+  </si>
+  <si>
+    <t>Grand Prix Landwerlin</t>
+  </si>
+  <si>
+    <t>Dim 20 Décembre</t>
+  </si>
+  <si>
+    <t>2ème cyclo-cross du Gloeckelsberg</t>
+  </si>
+  <si>
+    <t>19 et 20 Septembre</t>
+  </si>
+  <si>
+    <t>Championnat d'Alsace FSGT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20ème Grand Prix Gestimmo à Magstatt-le-Bas  </t>
+  </si>
+  <si>
+    <t>25 et 26 Janvier</t>
+  </si>
+  <si>
+    <t>Sam 9 Mai</t>
+  </si>
+  <si>
+    <t>11 et 12 Juillet</t>
+  </si>
+  <si>
+    <t>La Super cUp VTT (mixte sous l'égide de la FSGT)  Jeunes jusqu'à cadets</t>
+  </si>
+  <si>
+    <t>Championnat d'Alsace Franche-Comté de CLM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLM ind. à Frotey-les-Lure  </t>
+  </si>
+  <si>
+    <t>Dim 17 Mai</t>
+  </si>
+  <si>
+    <t>Randonnée VTT Les Hauts du Pays de Montbéliard</t>
+  </si>
+  <si>
+    <t>etupes</t>
+  </si>
+  <si>
+    <t>Championnat du Doubs</t>
+  </si>
+  <si>
+    <t>Championnat de Bourgogne Franche-Comté</t>
+  </si>
+  <si>
+    <t>Reporté</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27ème Prix Super U Beaucourt  </t>
+  </si>
+  <si>
+    <t>Gentlemen de Nommay (épreuve FFC ouverte aux FSGT)*</t>
+  </si>
+  <si>
+    <t>Dim 7 Juin</t>
+  </si>
+  <si>
+    <t>Chrono de la Biscuiterie Gerthoffer à Retzwiller</t>
+  </si>
+  <si>
+    <t>Dim 14 Juin</t>
+  </si>
+  <si>
+    <t>Grand Prix de Seppois-le-Bas</t>
+  </si>
+  <si>
     <t>seppois</t>
-  </si>
-  <si>
-    <t>fontaine</t>
-  </si>
-  <si>
-    <t>eteimbes</t>
-  </si>
-  <si>
-    <t>vauthiermont</t>
-  </si>
-  <si>
-    <t>lure</t>
-  </si>
-  <si>
-    <t>frotey</t>
-  </si>
-  <si>
-    <t>rougemont</t>
-  </si>
-  <si>
-    <t>nommay</t>
-  </si>
-  <si>
-    <t>UC Lutterbach VTT</t>
-  </si>
-  <si>
-    <t>champduf</t>
-  </si>
-  <si>
-    <t>FileNameResults</t>
-  </si>
-  <si>
-    <t>Championnat Fédéral 2020 à Nogent sur Seine, Aube Grand Est</t>
-  </si>
-  <si>
-    <t>UC Nogentaise</t>
-  </si>
-  <si>
-    <t>Sam 21 Mars</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VTT des Transports Portmann  </t>
-  </si>
-  <si>
-    <t>Dim 22 Mars</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28ème Prix Agri-Center à Jettingen  </t>
-  </si>
-  <si>
-    <t>jettingen</t>
-  </si>
-  <si>
-    <t>Sam 28 Mars</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grand Prix du Grand Hamster  </t>
-  </si>
-  <si>
-    <t>Dim 5 Avril</t>
-  </si>
-  <si>
-    <t>Dim 12 Avril</t>
-  </si>
-  <si>
-    <t>Circuit du Vallon en 2 étapes, à Eteimbes</t>
-  </si>
-  <si>
-    <t>Dim 26 Avril</t>
-  </si>
-  <si>
-    <t>Dim 3 Mai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prix du Garage Wadel à Retzwiller  </t>
-  </si>
-  <si>
-    <t>Ven 8 Mai</t>
-  </si>
-  <si>
-    <t>Dim 10 Mai</t>
-  </si>
-  <si>
-    <t>La Juralsace à Waldighoffen</t>
-  </si>
-  <si>
-    <t>waldighoffen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grand Prix Dépannage 70 à Frotey les Lure  </t>
-  </si>
-  <si>
-    <t>Ven 15 Mai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nocturne de Lure (ouvert aux cadets)  </t>
-  </si>
-  <si>
-    <t>Sam 23 Mai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29ème Grand Prix Gestimmo à Magstatt le bas  </t>
-  </si>
-  <si>
-    <t>Dim 24 Mai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cyclosportive les Marcaires  </t>
-  </si>
-  <si>
-    <t>Sam 6 Juin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les 3h VTT du VCSA  </t>
-  </si>
-  <si>
-    <t>Dim 21 Juin</t>
-  </si>
-  <si>
-    <t>La Rando Tour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Munster Bike Tour à Muhlbach sur Munster  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VTT à Retzwiller  </t>
-  </si>
-  <si>
-    <t>retzwillerbis</t>
-  </si>
-  <si>
-    <t>Sam 27 Juin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Randonnée du Champ du Feu  </t>
-  </si>
-  <si>
-    <t>Dim 28 Juin</t>
-  </si>
-  <si>
-    <t>Journée Sport et Détente à Beaucourt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VTT du Champ du Feu       VeSPA = Vélo et Sport de Plein Air  </t>
-  </si>
-  <si>
-    <t>4 et 5 Juillet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Championnat Fédéral  à Saint Chinian et Prades sur Vernazobre (Hérault)  </t>
-  </si>
-  <si>
-    <t>Sam 4 Juillet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12ème Nuit des Gros Mollets à Flaxlanden  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">10ème Nuit des Gros Mollets jeunes à Flaxlanden (poussins à minimes)  </t>
-  </si>
-  <si>
-    <t>goros_mollets_jeunes</t>
-  </si>
-  <si>
-    <t>Dim 5 Juillet</t>
-  </si>
-  <si>
-    <t>Petit Ballon Rando Tour</t>
-  </si>
-  <si>
-    <t>rando_tour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1er Grand Prix du Petit Meublard à Bréchaumont  </t>
-  </si>
-  <si>
-    <t>brechaumont</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fédéraux de VTT à La Chapelle St Aubin (Sarthe)  </t>
-  </si>
-  <si>
-    <t>federaux</t>
-  </si>
-  <si>
-    <t>Sam 11 Juillet</t>
-  </si>
-  <si>
-    <t>Grimpée des Bagenelles</t>
-  </si>
-  <si>
-    <t>Dim 12 Juillet</t>
-  </si>
-  <si>
-    <t>Dim 2 Août</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grimpée Le Waldbach, d'Ammerschwihr à Labaroche   </t>
-  </si>
-  <si>
-    <t>Dim 23 Août</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grand Prix d'Ampfersbach  </t>
-  </si>
-  <si>
-    <t>ampfersbach</t>
-  </si>
-  <si>
-    <t>Sam 29 Août</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3ème VTT Peugeot  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">24ème Montée du Floridor, col du Hundsruck à Thann  </t>
-  </si>
-  <si>
-    <t>Dim 30 Août</t>
-  </si>
-  <si>
-    <t>Sam 5 Septembre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L'Urbaine VTT - Cernay  </t>
-  </si>
-  <si>
-    <t>Dim 6 Septembre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VTT des Bords de l'Ill (mixte sous l'égide de la FFC)  </t>
-  </si>
-  <si>
-    <t>ste_croix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11ème Prix de Boron  </t>
-  </si>
-  <si>
-    <t>AS de l'Allan</t>
-  </si>
-  <si>
-    <t>Sam 12 Septembre</t>
-  </si>
-  <si>
-    <t>15ème Grimpée du Col Amic à Soultz</t>
-  </si>
-  <si>
-    <t>Dim 13 Septembre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grand Prix VTT de Mollau  </t>
-  </si>
-  <si>
-    <t>Cyclo-cross de la Ville de Wittenheim</t>
-  </si>
-  <si>
-    <t>Sam 26 Septembre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5ème VTT MS Automobile Rixheim  </t>
-  </si>
-  <si>
-    <t>Dim 27 Septembre</t>
-  </si>
-  <si>
-    <t>La Geko-Bikes à Didenheim</t>
-  </si>
-  <si>
-    <t>didenheim</t>
-  </si>
-  <si>
-    <t>Sam 3 Octobre</t>
-  </si>
-  <si>
-    <t>Sam 10 Octobre</t>
-  </si>
-  <si>
-    <t>Cyclo-cross de Morschwiller le bas</t>
-  </si>
-  <si>
-    <t>Dim 11 Octobre</t>
-  </si>
-  <si>
-    <t>2ème Cyclo-cross de Giromagny. Epreuve FFC ouverte aux FSGT</t>
-  </si>
-  <si>
-    <t>Sam 17 Octobre</t>
-  </si>
-  <si>
-    <t>Cyclo-cross de Heimsbrunn</t>
-  </si>
-  <si>
-    <t>Sam 24 Octobre</t>
-  </si>
-  <si>
-    <t>Sam 7 Novembre</t>
-  </si>
-  <si>
-    <t>Sam 14 Novembre</t>
-  </si>
-  <si>
-    <t>Sam 21 Novembre</t>
-  </si>
-  <si>
-    <t>Sam 28 Novembre</t>
-  </si>
-  <si>
-    <t>Dim 6 Décembre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cyclo-cross du Bief de Niffer, Prix Vélotop Kembs  </t>
-  </si>
-  <si>
-    <t>Sam 12 Décembre</t>
-  </si>
-  <si>
-    <t>Grand Prix Landwerlin</t>
-  </si>
-  <si>
-    <t>Dim 20 Décembre</t>
-  </si>
-  <si>
-    <t>2ème cyclo-cross du Gloeckelsberg</t>
-  </si>
-  <si>
-    <t>19 et 20 Septembre</t>
-  </si>
-  <si>
-    <t>Championnat d'Alsace FSGT</t>
-  </si>
-  <si>
-    <t>VTT de Retzwiller</t>
-  </si>
-  <si>
-    <t>Grand Prix de Seppois-le-Bas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20ème Grand Prix Gestimmo à Magstatt-le-Bas  </t>
-  </si>
-  <si>
-    <t>25 et 26 Janvier</t>
-  </si>
-  <si>
-    <t>Sam 9 Mai</t>
-  </si>
-  <si>
-    <t>11 et 12 Juillet</t>
-  </si>
-  <si>
-    <t>La Super cUp VTT (mixte sous l'égide de la FSGT)  Jeunes jusqu'à cadets</t>
-  </si>
-  <si>
-    <t>Championnat d'Alsace Franche-Comté de CLM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLM ind. à Frotey-les-Lure  </t>
-  </si>
-  <si>
-    <t>Dim 14 Juin</t>
-  </si>
-  <si>
-    <t>Dim 17 Mai</t>
-  </si>
-  <si>
-    <t>Randonnée VTT Les Hauts du Pays de Montbéliard</t>
-  </si>
-  <si>
-    <t>etupes</t>
-  </si>
-  <si>
-    <t>Championnat du Doubs</t>
-  </si>
-  <si>
-    <t>Championnat de Bourgogne Franche-Comté</t>
-  </si>
-  <si>
-    <t>Reporté</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27ème Prix Super U Beaucourt  </t>
-  </si>
-  <si>
-    <t>Gentlemen de Nommay (épreuve FFC ouverte aux FSGT)*</t>
   </si>
 </sst>
 </file>
@@ -1494,7 +1488,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1502,20 +1496,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="66.88671875" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" customWidth="1"/>
-    <col min="5" max="5" width="28.5546875" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" customWidth="1"/>
-    <col min="7" max="7" width="65.88671875" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="66.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="65.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1523,47 +1517,47 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
         <v>43</v>
-      </c>
-      <c r="C1" t="s">
-        <v>44</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -1572,15 +1566,15 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1589,29 +1583,29 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1623,15 +1617,15 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -1640,18 +1634,18 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G7" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B8" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -1660,24 +1654,24 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" t="s">
         <v>110</v>
       </c>
-      <c r="B9" t="s">
-        <v>200</v>
-      </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1685,50 +1679,50 @@
         <v>111</v>
       </c>
       <c r="B10" t="s">
-        <v>112</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>196</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>198</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>202</v>
+        <v>112</v>
       </c>
       <c r="B12" t="s">
-        <v>204</v>
+        <v>113</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1739,38 +1733,38 @@
         <v>115</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>114</v>
+        <v>201</v>
       </c>
       <c r="B14" t="s">
-        <v>117</v>
+        <v>202</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>92</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -1779,32 +1773,32 @@
         <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>91</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>208</v>
+        <v>118</v>
       </c>
       <c r="B16" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>210</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B17" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
@@ -1813,231 +1807,231 @@
         <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B18" t="s">
-        <v>198</v>
+        <v>121</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>70</v>
-      </c>
-      <c r="G18" t="s">
-        <v>197</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>209</v>
       </c>
       <c r="B19" t="s">
-        <v>123</v>
+        <v>194</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>124</v>
+        <v>211</v>
       </c>
       <c r="B20" t="s">
-        <v>125</v>
+        <v>212</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>213</v>
+      </c>
+      <c r="G20" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>207</v>
+        <v>122</v>
       </c>
       <c r="B21" t="s">
-        <v>199</v>
+        <v>123</v>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>87</v>
-      </c>
-      <c r="G21" t="s">
-        <v>197</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B22" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E22" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B23" t="s">
-        <v>128</v>
+        <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
         <v>126</v>
       </c>
-      <c r="B24" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" t="s">
-        <v>86</v>
+      <c r="G24" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C25" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D25" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>130</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B26" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B27" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D27" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E27" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28" t="s">
         <v>133</v>
       </c>
-      <c r="B28" t="s">
-        <v>135</v>
-      </c>
-      <c r="C28" t="s">
-        <v>22</v>
-      </c>
       <c r="D28" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B29" t="s">
-        <v>137</v>
+        <v>135</v>
+      </c>
+      <c r="C29" t="s">
+        <v>20</v>
       </c>
       <c r="D29" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B30" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D30" t="s">
         <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>50</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -2045,500 +2039,500 @@
         <v>138</v>
       </c>
       <c r="B31" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
       <c r="C31" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D31" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E31" t="s">
-        <v>141</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B32" t="s">
-        <v>83</v>
+        <v>139</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E32" t="s">
-        <v>66</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
+        <v>138</v>
+      </c>
+      <c r="B33" t="s">
+        <v>141</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" t="s">
         <v>142</v>
-      </c>
-      <c r="B33" t="s">
-        <v>143</v>
-      </c>
-      <c r="C33" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>142</v>
+        <v>197</v>
       </c>
       <c r="B34" t="s">
-        <v>145</v>
-      </c>
-      <c r="C34" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="D34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>203</v>
+        <v>145</v>
       </c>
       <c r="B35" t="s">
-        <v>147</v>
+        <v>146</v>
+      </c>
+      <c r="C35" t="s">
+        <v>22</v>
       </c>
       <c r="D35" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E35" t="s">
-        <v>148</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B36" t="s">
-        <v>150</v>
+        <v>83</v>
       </c>
       <c r="C36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" t="s">
         <v>23</v>
       </c>
-      <c r="D36" t="s">
-        <v>24</v>
-      </c>
       <c r="E36" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B37" t="s">
-        <v>84</v>
+        <v>149</v>
       </c>
       <c r="C37" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E37" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
+        <v>150</v>
+      </c>
+      <c r="B38" t="s">
+        <v>151</v>
+      </c>
+      <c r="C38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" t="s">
         <v>152</v>
-      </c>
-      <c r="B38" t="s">
-        <v>153</v>
-      </c>
-      <c r="C38" t="s">
-        <v>26</v>
-      </c>
-      <c r="D38" t="s">
-        <v>24</v>
-      </c>
-      <c r="E38" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
+        <v>153</v>
+      </c>
+      <c r="B39" t="s">
         <v>154</v>
       </c>
-      <c r="B39" t="s">
-        <v>155</v>
-      </c>
       <c r="C39" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D39" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E39" t="s">
-        <v>156</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B40" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="D40" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E40" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B41" t="s">
-        <v>159</v>
+        <v>28</v>
       </c>
       <c r="C41" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="E41" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B42" t="s">
-        <v>29</v>
+        <v>158</v>
       </c>
       <c r="C42" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D42" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E42" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B43" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C43" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D43" t="s">
         <v>3</v>
       </c>
       <c r="E43" t="s">
-        <v>48</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
+        <v>159</v>
+      </c>
+      <c r="B44" t="s">
+        <v>162</v>
+      </c>
+      <c r="C44" t="s">
         <v>163</v>
       </c>
-      <c r="B44" t="s">
-        <v>164</v>
-      </c>
-      <c r="C44" t="s">
-        <v>19</v>
-      </c>
       <c r="D44" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E44" t="s">
-        <v>165</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B45" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C45" t="s">
-        <v>167</v>
+        <v>29</v>
       </c>
       <c r="D45" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="E45" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B46" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C46" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="E46" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B47" t="s">
-        <v>171</v>
+        <v>200</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D47" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E47" t="s">
-        <v>60</v>
+        <v>79</v>
+      </c>
+      <c r="G47" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>170</v>
+        <v>192</v>
       </c>
       <c r="B48" t="s">
-        <v>206</v>
+        <v>168</v>
       </c>
       <c r="C48" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D48" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E48" t="s">
-        <v>80</v>
-      </c>
-      <c r="G48" t="s">
-        <v>205</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>196</v>
+        <v>169</v>
       </c>
       <c r="B49" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C49" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="E49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B50" t="s">
-        <v>174</v>
+        <v>208</v>
       </c>
       <c r="C50" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D50" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E50" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B51" t="s">
-        <v>215</v>
+        <v>172</v>
       </c>
       <c r="C51" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="D51" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E51" t="s">
-        <v>94</v>
+        <v>173</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B52" t="s">
-        <v>176</v>
+        <v>33</v>
       </c>
       <c r="C52" t="s">
-        <v>95</v>
+        <v>7</v>
       </c>
       <c r="D52" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E52" t="s">
-        <v>177</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B53" t="s">
+        <v>176</v>
+      </c>
+      <c r="C53" t="s">
         <v>34</v>
       </c>
-      <c r="C53" t="s">
-        <v>7</v>
-      </c>
       <c r="D53" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E53" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B54" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C54" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="D54" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E54" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B55" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C55" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="D55" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E55" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B56" t="s">
-        <v>184</v>
+        <v>35</v>
       </c>
       <c r="C56" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D56" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E56" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B57" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C57" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D57" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E57" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B58" t="s">
         <v>39</v>
       </c>
       <c r="C58" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="D58" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E58" t="s">
         <v>55</v>
       </c>
+      <c r="G58" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B59" t="s">
         <v>40</v>
       </c>
       <c r="C59" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D59" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E59" t="s">
-        <v>56</v>
-      </c>
-      <c r="G59" t="s">
-        <v>211</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B60" t="s">
         <v>41</v>
@@ -2547,81 +2541,64 @@
         <v>37</v>
       </c>
       <c r="D60" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E60" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="G60" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B61" t="s">
-        <v>42</v>
+        <v>187</v>
       </c>
       <c r="C61" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="D61" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E61" t="s">
-        <v>57</v>
-      </c>
-      <c r="G61" t="s">
-        <v>212</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B62" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C62" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="D62" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E62" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B63" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C63" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="D63" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E63" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" t="s">
-        <v>194</v>
-      </c>
-      <c r="B64" t="s">
-        <v>195</v>
-      </c>
-      <c r="C64" t="s">
-        <v>77</v>
-      </c>
-      <c r="D64" t="s">
-        <v>32</v>
-      </c>
-      <c r="E64" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dates correctes et 29eme a jettingen
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7548"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
   </bookViews>
   <sheets>
     <sheet name="Calendrier" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -319,9 +319,6 @@
     <t>Dim 22 Mars</t>
   </si>
   <si>
-    <t xml:space="preserve">28ème Prix Agri-Center à Jettingen  </t>
-  </si>
-  <si>
     <t>jettingen</t>
   </si>
   <si>
@@ -364,9 +361,6 @@
     <t>Sam 23 Mai</t>
   </si>
   <si>
-    <t xml:space="preserve">29ème Grand Prix Gestimmo à Magstatt le bas  </t>
-  </si>
-  <si>
     <t>Dim 24 Mai</t>
   </si>
   <si>
@@ -418,12 +412,6 @@
     <t>Sam 4 Juillet</t>
   </si>
   <si>
-    <t xml:space="preserve">12ème Nuit des Gros Mollets à Flaxlanden  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">10ème Nuit des Gros Mollets jeunes à Flaxlanden (poussins à minimes)  </t>
-  </si>
-  <si>
     <t>goros_mollets_jeunes</t>
   </si>
   <si>
@@ -475,12 +463,6 @@
     <t>Sam 29 Août</t>
   </si>
   <si>
-    <t xml:space="preserve">3ème VTT Peugeot  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">24ème Montée du Floridor, col du Hundsruck à Thann  </t>
-  </si>
-  <si>
     <t>Dim 30 Août</t>
   </si>
   <si>
@@ -499,18 +481,12 @@
     <t>ste_croix</t>
   </si>
   <si>
-    <t xml:space="preserve">11ème Prix de Boron  </t>
-  </si>
-  <si>
     <t>AS de l'Allan</t>
   </si>
   <si>
     <t>Sam 12 Septembre</t>
   </si>
   <si>
-    <t>15ème Grimpée du Col Amic à Soultz</t>
-  </si>
-  <si>
     <t>Dim 13 Septembre</t>
   </si>
   <si>
@@ -523,9 +499,6 @@
     <t>Sam 26 Septembre</t>
   </si>
   <si>
-    <t xml:space="preserve">5ème VTT MS Automobile Rixheim  </t>
-  </si>
-  <si>
     <t>Dim 27 Septembre</t>
   </si>
   <si>
@@ -547,9 +520,6 @@
     <t>Dim 11 Octobre</t>
   </si>
   <si>
-    <t>2ème Cyclo-cross de Giromagny. Epreuve FFC ouverte aux FSGT</t>
-  </si>
-  <si>
     <t>Sam 17 Octobre</t>
   </si>
   <si>
@@ -586,18 +556,12 @@
     <t>Dim 20 Décembre</t>
   </si>
   <si>
-    <t>2ème cyclo-cross du Gloeckelsberg</t>
-  </si>
-  <si>
     <t>19 et 20 Septembre</t>
   </si>
   <si>
     <t>Championnat d'Alsace FSGT</t>
   </si>
   <si>
-    <t xml:space="preserve">20ème Grand Prix Gestimmo à Magstatt-le-Bas  </t>
-  </si>
-  <si>
     <t>25 et 26 Janvier</t>
   </si>
   <si>
@@ -631,9 +595,6 @@
     <t>Championnat de Bourgogne Franche-Comté</t>
   </si>
   <si>
-    <t xml:space="preserve">27ème Prix Super U Beaucourt  </t>
-  </si>
-  <si>
     <t>Gentlemen de Nommay (épreuve FFC ouverte aux FSGT)*</t>
   </si>
   <si>
@@ -674,6 +635,45 @@
   </si>
   <si>
     <t>Annulée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29e Prix Agri-Center à Jettingen  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">29e Grand Prix Gestimmo à Magstatt le bas  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">27e Prix Super U Beaucourt  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">20e Grand Prix Gestimmo à Magstatt-le-Bas  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12e Nuit des Gros Mollets à Flaxlanden  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10e Nuit des Gros Mollets jeunes à Flaxlanden (poussins à minimes)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3e VTT Peugeot  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">24e Montée du Floridor, col du Hundsruck à Thann  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11e Prix de Boron  </t>
+  </si>
+  <si>
+    <t>15e Grimpée du Col Amic à Soultz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5e VTT MS Automobile Rixheim  </t>
+  </si>
+  <si>
+    <t>2e Cyclo-cross de Giromagny. Epreuve FFC ouverte aux FSGT</t>
+  </si>
+  <si>
+    <t>2e cyclo-cross du Gloeckelsberg</t>
   </si>
 </sst>
 </file>
@@ -1514,7 +1514,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1524,18 +1524,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C11" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="66.88671875" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" customWidth="1"/>
-    <col min="5" max="5" width="28.5546875" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" customWidth="1"/>
-    <col min="7" max="7" width="65.88671875" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="66.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="65.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1563,7 +1563,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="B2" t="s">
         <v>96</v>
@@ -1600,7 +1600,7 @@
         <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>207</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1609,15 +1609,15 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" t="s">
         <v>103</v>
-      </c>
-      <c r="B5" t="s">
-        <v>104</v>
       </c>
       <c r="C5" t="s">
         <v>76</v>
@@ -1631,7 +1631,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1648,10 +1648,10 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -1665,10 +1665,10 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B8" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -1682,10 +1682,10 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" t="s">
         <v>108</v>
-      </c>
-      <c r="B9" t="s">
-        <v>109</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
@@ -1699,7 +1699,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
@@ -1716,10 +1716,10 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="B11" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -1733,10 +1733,10 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" t="s">
         <v>111</v>
-      </c>
-      <c r="B12" t="s">
-        <v>112</v>
       </c>
       <c r="C12" t="s">
         <v>15</v>
@@ -1750,10 +1750,10 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" t="s">
         <v>113</v>
-      </c>
-      <c r="B13" t="s">
-        <v>114</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
@@ -1767,10 +1767,10 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="B14" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="C14" t="s">
         <v>37</v>
@@ -1779,15 +1779,15 @@
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>208</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -1801,10 +1801,10 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B16" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
@@ -1818,10 +1818,10 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
@@ -1835,10 +1835,10 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -1852,10 +1852,10 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="B19" t="s">
-        <v>193</v>
+        <v>210</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -1869,10 +1869,10 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="B20" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -1881,18 +1881,18 @@
         <v>5</v>
       </c>
       <c r="E20" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="G20" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C21" t="s">
         <v>18</v>
@@ -1906,10 +1906,10 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
+        <v>119</v>
+      </c>
+      <c r="B22" t="s">
         <v>121</v>
-      </c>
-      <c r="B22" t="s">
-        <v>123</v>
       </c>
       <c r="C22" t="s">
         <v>10</v>
@@ -1921,12 +1921,12 @@
         <v>54</v>
       </c>
       <c r="G22" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
@@ -1943,10 +1943,10 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C24" t="s">
         <v>13</v>
@@ -1955,18 +1955,18 @@
         <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G24" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C25" t="s">
         <v>21</v>
@@ -1980,10 +1980,10 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B26" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
@@ -1997,10 +1997,10 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" t="s">
         <v>128</v>
-      </c>
-      <c r="B27" t="s">
-        <v>130</v>
       </c>
       <c r="C27" t="s">
         <v>21</v>
@@ -2014,10 +2014,10 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="C28" t="s">
         <v>37</v>
@@ -2026,18 +2026,18 @@
         <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="G28" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B29" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D29" t="s">
         <v>5</v>
@@ -2048,10 +2048,10 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B30" t="s">
-        <v>134</v>
+        <v>211</v>
       </c>
       <c r="C30" t="s">
         <v>20</v>
@@ -2065,10 +2065,10 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B31" t="s">
-        <v>135</v>
+        <v>212</v>
       </c>
       <c r="C31" t="s">
         <v>20</v>
@@ -2077,12 +2077,12 @@
         <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B32" t="s">
         <v>82</v>
@@ -2099,10 +2099,10 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B33" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C33" t="s">
         <v>10</v>
@@ -2111,15 +2111,15 @@
         <v>12</v>
       </c>
       <c r="E33" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B34" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C34" t="s">
         <v>13</v>
@@ -2128,29 +2128,29 @@
         <v>5</v>
       </c>
       <c r="E34" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="B35" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D35" t="s">
         <v>3</v>
       </c>
       <c r="E35" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B36" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C36" t="s">
         <v>22</v>
@@ -2164,7 +2164,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B37" t="s">
         <v>83</v>
@@ -2181,10 +2181,10 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B38" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C38" t="s">
         <v>25</v>
@@ -2198,10 +2198,10 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B39" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C39" t="s">
         <v>17</v>
@@ -2210,15 +2210,15 @@
         <v>5</v>
       </c>
       <c r="E39" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B40" t="s">
-        <v>153</v>
+        <v>213</v>
       </c>
       <c r="C40" t="s">
         <v>9</v>
@@ -2232,10 +2232,10 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B41" t="s">
-        <v>154</v>
+        <v>214</v>
       </c>
       <c r="C41" t="s">
         <v>27</v>
@@ -2249,7 +2249,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B42" t="s">
         <v>28</v>
@@ -2266,10 +2266,10 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B43" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C43" t="s">
         <v>27</v>
@@ -2283,10 +2283,10 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B44" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C44" t="s">
         <v>18</v>
@@ -2295,18 +2295,18 @@
         <v>3</v>
       </c>
       <c r="E44" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B45" t="s">
-        <v>161</v>
+        <v>215</v>
       </c>
       <c r="C45" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D45" t="s">
         <v>5</v>
@@ -2317,10 +2317,10 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B46" t="s">
-        <v>164</v>
+        <v>216</v>
       </c>
       <c r="C46" t="s">
         <v>29</v>
@@ -2334,10 +2334,10 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B47" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C47" t="s">
         <v>8</v>
@@ -2351,10 +2351,10 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B48" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="C48" t="s">
         <v>15</v>
@@ -2366,15 +2366,15 @@
         <v>79</v>
       </c>
       <c r="G48" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="B49" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C49" t="s">
         <v>30</v>
@@ -2388,10 +2388,10 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B50" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
       <c r="C50" t="s">
         <v>2</v>
@@ -2405,10 +2405,10 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B51" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="C51" t="s">
         <v>32</v>
@@ -2422,10 +2422,10 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B52" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C52" t="s">
         <v>93</v>
@@ -2434,12 +2434,12 @@
         <v>3</v>
       </c>
       <c r="E52" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B53" t="s">
         <v>33</v>
@@ -2456,10 +2456,10 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B54" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C54" t="s">
         <v>34</v>
@@ -2473,10 +2473,10 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B55" t="s">
-        <v>177</v>
+        <v>218</v>
       </c>
       <c r="C55" t="s">
         <v>80</v>
@@ -2490,10 +2490,10 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B56" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C56" t="s">
         <v>20</v>
@@ -2507,7 +2507,7 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="B57" t="s">
         <v>35</v>
@@ -2524,7 +2524,7 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="B58" t="s">
         <v>38</v>
@@ -2541,7 +2541,7 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="B59" t="s">
         <v>39</v>
@@ -2556,12 +2556,12 @@
         <v>55</v>
       </c>
       <c r="G59" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="B60" t="s">
         <v>40</v>
@@ -2578,7 +2578,7 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="B61" t="s">
         <v>41</v>
@@ -2593,15 +2593,15 @@
         <v>56</v>
       </c>
       <c r="G61" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="B62" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="C62" t="s">
         <v>2</v>
@@ -2615,10 +2615,10 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="B63" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C63" t="s">
         <v>24</v>
@@ -2632,10 +2632,10 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="C64" t="s">
         <v>37</v>
@@ -2644,15 +2644,15 @@
         <v>31</v>
       </c>
       <c r="E64" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="B65" t="s">
-        <v>190</v>
+        <v>219</v>
       </c>
       <c r="C65" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
changement date de nommay gentleman
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="221">
   <si>
     <t>Date</t>
   </si>
@@ -674,6 +674,9 @@
   </si>
   <si>
     <t>2e cyclo-cross du Gloeckelsberg</t>
+  </si>
+  <si>
+    <t>Dim 20 Septembre</t>
   </si>
 </sst>
 </file>
@@ -1514,7 +1517,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1524,8 +1527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2369,7 +2372,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" ht="15.75" customHeight="1">
       <c r="A49" t="s">
         <v>180</v>
       </c>
@@ -2388,36 +2391,36 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>160</v>
+        <v>220</v>
       </c>
       <c r="B50" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="C50" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D50" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E50" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B51" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="C51" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E51" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:7">

</xml_diff>

<commit_message>
nouveaux documents et bon numero a la grimpee du col amic
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="222">
   <si>
     <t>Date</t>
   </si>
@@ -664,9 +664,6 @@
     <t xml:space="preserve">11e Prix de Boron  </t>
   </si>
   <si>
-    <t>15e Grimpée du Col Amic à Soultz</t>
-  </si>
-  <si>
     <t xml:space="preserve">5e VTT MS Automobile Rixheim  </t>
   </si>
   <si>
@@ -677,6 +674,12 @@
   </si>
   <si>
     <t>Dim 20 Septembre</t>
+  </si>
+  <si>
+    <t>Annulé</t>
+  </si>
+  <si>
+    <t>20e Grimpée du Col Amic à Soultz</t>
   </si>
 </sst>
 </file>
@@ -1517,7 +1520,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1527,8 +1530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1665,6 +1668,9 @@
       <c r="E7" t="s">
         <v>87</v>
       </c>
+      <c r="G7" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
@@ -2323,7 +2329,7 @@
         <v>156</v>
       </c>
       <c r="B46" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="C46" t="s">
         <v>29</v>
@@ -2391,7 +2397,7 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B50" t="s">
         <v>193</v>
@@ -2411,7 +2417,7 @@
         <v>160</v>
       </c>
       <c r="B51" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C51" t="s">
         <v>2</v>
@@ -2479,7 +2485,7 @@
         <v>167</v>
       </c>
       <c r="B55" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C55" t="s">
         <v>80</v>
@@ -2655,7 +2661,7 @@
         <v>179</v>
       </c>
       <c r="B65" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C65" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
Macron a parlé. RIP LE VELO
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="225">
   <si>
     <t>Date</t>
   </si>
@@ -559,9 +559,6 @@
     <t>19 et 20 Septembre</t>
   </si>
   <si>
-    <t>Championnat d'Alsace FSGT</t>
-  </si>
-  <si>
     <t>25 et 26 Janvier</t>
   </si>
   <si>
@@ -616,9 +613,6 @@
     <t>Prix des Terres de Chaux</t>
   </si>
   <si>
-    <t>Championnat de Bourgogne Franche Comté</t>
-  </si>
-  <si>
     <t>terres_de_chaux</t>
   </si>
   <si>
@@ -689,6 +683,12 @@
   </si>
   <si>
     <t>Annulée</t>
+  </si>
+  <si>
+    <t>Reportées au 12 septembre</t>
+  </si>
+  <si>
+    <t>altkirch_old_nothing</t>
   </si>
 </sst>
 </file>
@@ -1529,7 +1529,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1537,10 +1537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1578,7 +1578,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B2" t="s">
         <v>96</v>
@@ -1610,7 +1610,7 @@
         <v>68</v>
       </c>
       <c r="G3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1618,7 +1618,7 @@
         <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1630,7 +1630,7 @@
         <v>101</v>
       </c>
       <c r="G4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1650,7 +1650,7 @@
         <v>71</v>
       </c>
       <c r="G5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1670,12 +1670,12 @@
         <v>86</v>
       </c>
       <c r="G6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B7" t="s">
         <v>105</v>
@@ -1690,7 +1690,7 @@
         <v>87</v>
       </c>
       <c r="G7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1698,7 +1698,7 @@
         <v>106</v>
       </c>
       <c r="B8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -1710,7 +1710,7 @@
         <v>70</v>
       </c>
       <c r="G8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1730,7 +1730,7 @@
         <v>69</v>
       </c>
       <c r="G9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1750,15 +1750,15 @@
         <v>88</v>
       </c>
       <c r="G10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -1768,6 +1768,9 @@
       </c>
       <c r="E11" t="s">
         <v>54</v>
+      </c>
+      <c r="G11" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1787,7 +1790,7 @@
         <v>90</v>
       </c>
       <c r="G12" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1807,15 +1810,15 @@
         <v>89</v>
       </c>
       <c r="G13" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
+        <v>187</v>
+      </c>
+      <c r="B14" t="s">
         <v>188</v>
-      </c>
-      <c r="B14" t="s">
-        <v>189</v>
       </c>
       <c r="C14" t="s">
         <v>37</v>
@@ -1824,7 +1827,10 @@
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>190</v>
+        <v>189</v>
+      </c>
+      <c r="G14" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1832,7 +1838,7 @@
         <v>114</v>
       </c>
       <c r="B15" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -1844,7 +1850,7 @@
         <v>45</v>
       </c>
       <c r="G15" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1852,7 +1858,7 @@
         <v>115</v>
       </c>
       <c r="B16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
@@ -1862,6 +1868,9 @@
       </c>
       <c r="E16" t="s">
         <v>69</v>
+      </c>
+      <c r="G16" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1881,7 +1890,7 @@
         <v>74</v>
       </c>
       <c r="G17" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1898,15 +1907,18 @@
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>77</v>
+        <v>224</v>
+      </c>
+      <c r="G18" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
@@ -1918,15 +1930,15 @@
         <v>45</v>
       </c>
       <c r="G19" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
+        <v>195</v>
+      </c>
+      <c r="B20" t="s">
         <v>196</v>
-      </c>
-      <c r="B20" t="s">
-        <v>197</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -1935,10 +1947,10 @@
         <v>5</v>
       </c>
       <c r="E20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G20" t="s">
-        <v>181</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1957,6 +1969,9 @@
       <c r="E21" t="s">
         <v>66</v>
       </c>
+      <c r="G21" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
@@ -1975,7 +1990,7 @@
         <v>54</v>
       </c>
       <c r="G22" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1994,6 +2009,9 @@
       <c r="E23" t="s">
         <v>85</v>
       </c>
+      <c r="G23" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
@@ -2012,7 +2030,7 @@
         <v>123</v>
       </c>
       <c r="G24" t="s">
-        <v>181</v>
+        <v>219</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -2031,6 +2049,9 @@
       <c r="E25" t="s">
         <v>94</v>
       </c>
+      <c r="G25" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
@@ -2048,6 +2069,9 @@
       <c r="E26" t="s">
         <v>67</v>
       </c>
+      <c r="G26" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
@@ -2065,13 +2089,16 @@
       <c r="E27" t="s">
         <v>50</v>
       </c>
+      <c r="G27" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>126</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C28" t="s">
         <v>37</v>
@@ -2080,10 +2107,10 @@
         <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G28" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -2100,7 +2127,7 @@
         <v>72</v>
       </c>
       <c r="G29" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -2108,7 +2135,7 @@
         <v>131</v>
       </c>
       <c r="B30" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C30" t="s">
         <v>20</v>
@@ -2118,6 +2145,9 @@
       </c>
       <c r="E30" t="s">
         <v>49</v>
+      </c>
+      <c r="G30" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -2125,7 +2155,7 @@
         <v>131</v>
       </c>
       <c r="B31" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C31" t="s">
         <v>20</v>
@@ -2135,6 +2165,9 @@
       </c>
       <c r="E31" t="s">
         <v>132</v>
+      </c>
+      <c r="G31" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -2153,6 +2186,9 @@
       <c r="E32" t="s">
         <v>65</v>
       </c>
+      <c r="G32" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
@@ -2170,6 +2206,9 @@
       <c r="E33" t="s">
         <v>135</v>
       </c>
+      <c r="G33" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
@@ -2187,10 +2226,13 @@
       <c r="E34" t="s">
         <v>137</v>
       </c>
+      <c r="G34" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B35" t="s">
         <v>138</v>
@@ -2202,7 +2244,7 @@
         <v>139</v>
       </c>
       <c r="G35" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -2221,6 +2263,9 @@
       <c r="E36" t="s">
         <v>61</v>
       </c>
+      <c r="G36" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
@@ -2238,6 +2283,9 @@
       <c r="E37" t="s">
         <v>84</v>
       </c>
+      <c r="G37" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
@@ -2278,7 +2326,7 @@
         <v>148</v>
       </c>
       <c r="B40" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C40" t="s">
         <v>9</v>
@@ -2295,7 +2343,7 @@
         <v>148</v>
       </c>
       <c r="B41" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C41" t="s">
         <v>27</v>
@@ -2363,7 +2411,7 @@
         <v>152</v>
       </c>
       <c r="B45" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C45" t="s">
         <v>155</v>
@@ -2380,33 +2428,33 @@
         <v>156</v>
       </c>
       <c r="B46" t="s">
-        <v>220</v>
+        <v>118</v>
       </c>
       <c r="C46" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E46" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B47" t="s">
-        <v>158</v>
+        <v>218</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="D47" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E47" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -2414,313 +2462,330 @@
         <v>157</v>
       </c>
       <c r="B48" t="s">
-        <v>187</v>
+        <v>158</v>
       </c>
       <c r="C48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
+        <v>157</v>
+      </c>
+      <c r="B49" t="s">
+        <v>186</v>
+      </c>
+      <c r="C49" t="s">
         <v>15</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>5</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E49" t="s">
         <v>79</v>
       </c>
-      <c r="G48" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A49" t="s">
+      <c r="G49" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A50" t="s">
         <v>180</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>159</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>30</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>31</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E50" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" t="s">
-        <v>218</v>
-      </c>
-      <c r="B50" t="s">
-        <v>193</v>
-      </c>
-      <c r="C50" t="s">
-        <v>32</v>
-      </c>
-      <c r="D50" t="s">
-        <v>5</v>
-      </c>
-      <c r="E50" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>160</v>
+        <v>216</v>
       </c>
       <c r="B51" t="s">
-        <v>215</v>
+        <v>192</v>
       </c>
       <c r="C51" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D51" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E51" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B52" t="s">
-        <v>162</v>
+        <v>213</v>
       </c>
       <c r="C52" t="s">
-        <v>93</v>
+        <v>2</v>
       </c>
       <c r="D52" t="s">
         <v>3</v>
       </c>
       <c r="E52" t="s">
-        <v>163</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B53" t="s">
-        <v>33</v>
+        <v>162</v>
       </c>
       <c r="C53" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="D53" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E53" t="s">
-        <v>64</v>
+        <v>163</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B54" t="s">
-        <v>166</v>
+        <v>33</v>
       </c>
       <c r="C54" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D54" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E54" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B55" t="s">
-        <v>216</v>
+        <v>166</v>
       </c>
       <c r="C55" t="s">
-        <v>80</v>
+        <v>34</v>
       </c>
       <c r="D55" t="s">
         <v>31</v>
       </c>
       <c r="E55" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B56" t="s">
-        <v>169</v>
+        <v>214</v>
       </c>
       <c r="C56" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="D56" t="s">
         <v>31</v>
       </c>
       <c r="E56" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B57" t="s">
-        <v>35</v>
+        <v>169</v>
       </c>
       <c r="C57" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D57" t="s">
         <v>31</v>
       </c>
       <c r="E57" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B58" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C58" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="D58" t="s">
         <v>31</v>
       </c>
       <c r="E58" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B59" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C59" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D59" t="s">
         <v>31</v>
       </c>
       <c r="E59" t="s">
-        <v>55</v>
-      </c>
-      <c r="G59" t="s">
-        <v>191</v>
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B60" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C60" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D60" t="s">
         <v>31</v>
       </c>
       <c r="E60" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="G60" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B61" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C61" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D61" t="s">
         <v>31</v>
       </c>
       <c r="E61" t="s">
-        <v>56</v>
-      </c>
-      <c r="G61" t="s">
-        <v>192</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B62" t="s">
-        <v>176</v>
+        <v>41</v>
       </c>
       <c r="C62" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="D62" t="s">
         <v>31</v>
       </c>
       <c r="E62" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="G62" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B63" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C63" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D63" t="s">
         <v>31</v>
       </c>
       <c r="E63" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>202</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>203</v>
+        <v>177</v>
+      </c>
+      <c r="B64" t="s">
+        <v>178</v>
       </c>
       <c r="C64" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="D64" t="s">
         <v>31</v>
       </c>
       <c r="E64" t="s">
-        <v>204</v>
+        <v>48</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>179</v>
-      </c>
-      <c r="B65" t="s">
-        <v>217</v>
+        <v>200</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="C65" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
       <c r="D65" t="s">
         <v>31</v>
       </c>
       <c r="E65" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>179</v>
+      </c>
+      <c r="B66" t="s">
+        <v>215</v>
+      </c>
+      <c r="C66" t="s">
+        <v>76</v>
+      </c>
+      <c r="D66" t="s">
+        <v>31</v>
+      </c>
+      <c r="E66" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nouvelle date nocturne Lure
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="231">
   <si>
     <t>Date</t>
   </si>
@@ -695,6 +695,18 @@
   </si>
   <si>
     <t>Annulés</t>
+  </si>
+  <si>
+    <t>Reportée au 11 septembre</t>
+  </si>
+  <si>
+    <t>Ven 11 Septembre</t>
+  </si>
+  <si>
+    <t>Nouvelle date</t>
+  </si>
+  <si>
+    <t>lure_old</t>
   </si>
 </sst>
 </file>
@@ -1543,10 +1555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" topLeftCell="B31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1816,7 +1828,7 @@
         <v>89</v>
       </c>
       <c r="G13" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2431,19 +2443,22 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>156</v>
+        <v>228</v>
       </c>
       <c r="B46" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C46" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D46" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E46" t="s">
-        <v>77</v>
+        <v>230</v>
+      </c>
+      <c r="G46" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -2451,33 +2466,36 @@
         <v>156</v>
       </c>
       <c r="B47" t="s">
-        <v>218</v>
+        <v>118</v>
       </c>
       <c r="C47" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E47" t="s">
-        <v>63</v>
+        <v>77</v>
+      </c>
+      <c r="G47" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B48" t="s">
-        <v>158</v>
+        <v>218</v>
       </c>
       <c r="C48" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="D48" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E48" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -2485,313 +2503,330 @@
         <v>157</v>
       </c>
       <c r="B49" t="s">
+        <v>158</v>
+      </c>
+      <c r="C49" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" t="s">
+        <v>157</v>
+      </c>
+      <c r="B50" t="s">
         <v>186</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>15</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>5</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E50" t="s">
         <v>79</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G50" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A50" t="s">
+    <row r="51" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A51" t="s">
         <v>180</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>159</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>30</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" t="s">
         <v>31</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E51" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51" t="s">
-        <v>216</v>
-      </c>
-      <c r="B51" t="s">
-        <v>192</v>
-      </c>
-      <c r="C51" t="s">
-        <v>32</v>
-      </c>
-      <c r="D51" t="s">
-        <v>5</v>
-      </c>
-      <c r="E51" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>160</v>
+        <v>216</v>
       </c>
       <c r="B52" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="C52" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D52" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E52" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B53" t="s">
-        <v>162</v>
+        <v>213</v>
       </c>
       <c r="C53" t="s">
-        <v>93</v>
+        <v>2</v>
       </c>
       <c r="D53" t="s">
         <v>3</v>
       </c>
       <c r="E53" t="s">
-        <v>163</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B54" t="s">
-        <v>33</v>
+        <v>162</v>
       </c>
       <c r="C54" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="D54" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E54" t="s">
-        <v>64</v>
+        <v>163</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B55" t="s">
-        <v>166</v>
+        <v>33</v>
       </c>
       <c r="C55" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D55" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E55" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B56" t="s">
-        <v>214</v>
+        <v>166</v>
       </c>
       <c r="C56" t="s">
-        <v>80</v>
+        <v>34</v>
       </c>
       <c r="D56" t="s">
         <v>31</v>
       </c>
       <c r="E56" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B57" t="s">
-        <v>169</v>
+        <v>214</v>
       </c>
       <c r="C57" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="D57" t="s">
         <v>31</v>
       </c>
       <c r="E57" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B58" t="s">
-        <v>35</v>
+        <v>169</v>
       </c>
       <c r="C58" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D58" t="s">
         <v>31</v>
       </c>
       <c r="E58" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B59" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C59" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="D59" t="s">
         <v>31</v>
       </c>
       <c r="E59" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B60" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C60" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D60" t="s">
         <v>31</v>
       </c>
       <c r="E60" t="s">
-        <v>55</v>
-      </c>
-      <c r="G60" t="s">
-        <v>190</v>
+        <v>54</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B61" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C61" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D61" t="s">
         <v>31</v>
       </c>
       <c r="E61" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="G61" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B62" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C62" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D62" t="s">
         <v>31</v>
       </c>
       <c r="E62" t="s">
-        <v>56</v>
-      </c>
-      <c r="G62" t="s">
-        <v>191</v>
+        <v>57</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B63" t="s">
-        <v>176</v>
+        <v>41</v>
       </c>
       <c r="C63" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="D63" t="s">
         <v>31</v>
       </c>
       <c r="E63" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="G63" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B64" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C64" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D64" t="s">
         <v>31</v>
       </c>
       <c r="E64" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>200</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>201</v>
+        <v>177</v>
+      </c>
+      <c r="B65" t="s">
+        <v>178</v>
       </c>
       <c r="C65" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="D65" t="s">
         <v>31</v>
       </c>
       <c r="E65" t="s">
-        <v>202</v>
+        <v>48</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>179</v>
-      </c>
-      <c r="B66" t="s">
-        <v>215</v>
+        <v>200</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="C66" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
       <c r="D66" t="s">
         <v>31</v>
       </c>
       <c r="E66" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>179</v>
+      </c>
+      <c r="B67" t="s">
+        <v>215</v>
+      </c>
+      <c r="C67" t="s">
+        <v>76</v>
+      </c>
+      <c r="D67" t="s">
+        <v>31</v>
+      </c>
+      <c r="E67" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Report au lieu de annulation
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -1547,7 +1547,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1557,8 +1557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1748,7 +1748,7 @@
         <v>69</v>
       </c>
       <c r="G9" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1768,7 +1768,7 @@
         <v>88</v>
       </c>
       <c r="G10" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:7">

</xml_diff>

<commit_message>
annulation grimpee col amic
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="235">
   <si>
     <t>Date</t>
   </si>
@@ -1559,7 +1559,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1569,8 +1569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1700,7 +1700,7 @@
         <v>86</v>
       </c>
       <c r="G6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2508,6 +2508,9 @@
       </c>
       <c r="E48" t="s">
         <v>63</v>
+      </c>
+      <c r="G48" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="49" spans="1:7">

</xml_diff>

<commit_message>
nouveau reglement et suppression 3h vtt
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7548"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
   </bookViews>
   <sheets>
     <sheet name="Calendrier" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="228">
   <si>
     <t>Date</t>
   </si>
@@ -367,9 +367,6 @@
     <t xml:space="preserve">Cyclosportive les Marcaires  </t>
   </si>
   <si>
-    <t>Sam 6 Juin</t>
-  </si>
-  <si>
     <t xml:space="preserve">Les 3h VTT du VCSA  </t>
   </si>
   <si>
@@ -676,16 +673,7 @@
     <t>Reporté</t>
   </si>
   <si>
-    <t>Reporté au 26 juillet</t>
-  </si>
-  <si>
     <t>Annulée</t>
-  </si>
-  <si>
-    <t>Reportées au 12 septembre</t>
-  </si>
-  <si>
-    <t>altkirch_old_nothing</t>
   </si>
   <si>
     <t>Annulée ou reportée</t>
@@ -1550,7 +1538,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1558,20 +1546,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="66.88671875" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" customWidth="1"/>
-    <col min="5" max="5" width="28.5546875" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" customWidth="1"/>
-    <col min="7" max="7" width="65.88671875" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="66.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="65.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1599,7 +1587,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" t="s">
         <v>96</v>
@@ -1631,7 +1619,7 @@
         <v>68</v>
       </c>
       <c r="G3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1639,7 +1627,7 @@
         <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1651,7 +1639,7 @@
         <v>101</v>
       </c>
       <c r="G4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1671,7 +1659,7 @@
         <v>71</v>
       </c>
       <c r="G5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1691,12 +1679,12 @@
         <v>86</v>
       </c>
       <c r="G6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B7" t="s">
         <v>105</v>
@@ -1711,7 +1699,7 @@
         <v>87</v>
       </c>
       <c r="G7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1719,7 +1707,7 @@
         <v>106</v>
       </c>
       <c r="B8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -1731,7 +1719,7 @@
         <v>70</v>
       </c>
       <c r="G8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1751,7 +1739,7 @@
         <v>69</v>
       </c>
       <c r="G9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1771,15 +1759,15 @@
         <v>88</v>
       </c>
       <c r="G10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -1791,7 +1779,7 @@
         <v>54</v>
       </c>
       <c r="G11" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1811,7 +1799,7 @@
         <v>90</v>
       </c>
       <c r="G12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1831,15 +1819,15 @@
         <v>89</v>
       </c>
       <c r="G13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
+        <v>186</v>
+      </c>
+      <c r="B14" t="s">
         <v>187</v>
-      </c>
-      <c r="B14" t="s">
-        <v>188</v>
       </c>
       <c r="C14" t="s">
         <v>37</v>
@@ -1848,10 +1836,10 @@
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G14" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1859,7 +1847,7 @@
         <v>114</v>
       </c>
       <c r="B15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -1871,7 +1859,7 @@
         <v>45</v>
       </c>
       <c r="G15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1879,7 +1867,7 @@
         <v>115</v>
       </c>
       <c r="B16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
@@ -1891,7 +1879,7 @@
         <v>69</v>
       </c>
       <c r="G16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1911,249 +1899,249 @@
         <v>74</v>
       </c>
       <c r="G17" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>117</v>
+        <v>192</v>
       </c>
       <c r="B18" t="s">
-        <v>118</v>
+        <v>205</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="D18" t="s">
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>223</v>
+        <v>45</v>
       </c>
       <c r="G18" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B19" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>45</v>
+        <v>223</v>
       </c>
       <c r="G19" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>195</v>
+        <v>118</v>
       </c>
       <c r="B20" t="s">
-        <v>196</v>
+        <v>119</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>227</v>
+        <v>66</v>
       </c>
       <c r="G20" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B21" t="s">
         <v>120</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
         <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G21" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B22" t="s">
-        <v>121</v>
+        <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E22" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="G22" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>121</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D23" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>85</v>
+        <v>225</v>
       </c>
       <c r="G23" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B24" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D24" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E24" t="s">
-        <v>229</v>
+        <v>94</v>
       </c>
       <c r="G24" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B25" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D25" t="s">
         <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="G25" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B26" t="s">
         <v>127</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E26" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="G26" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>126</v>
-      </c>
-      <c r="B27" t="s">
-        <v>128</v>
+        <v>125</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="C27" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D27" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>50</v>
+        <v>197</v>
       </c>
       <c r="G27" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>126</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C28" t="s">
-        <v>37</v>
+        <v>128</v>
+      </c>
+      <c r="B28" t="s">
+        <v>129</v>
       </c>
       <c r="D28" t="s">
         <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>198</v>
+        <v>72</v>
       </c>
       <c r="G28" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B29" t="s">
-        <v>130</v>
+        <v>206</v>
+      </c>
+      <c r="C29" t="s">
+        <v>20</v>
       </c>
       <c r="D29" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="G29" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B30" t="s">
         <v>207</v>
@@ -2165,127 +2153,127 @@
         <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>49</v>
+        <v>131</v>
       </c>
       <c r="G30" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B31" t="s">
-        <v>208</v>
+        <v>82</v>
       </c>
       <c r="C31" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D31" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E31" t="s">
-        <v>132</v>
+        <v>65</v>
       </c>
       <c r="G31" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
+        <v>132</v>
+      </c>
+      <c r="B32" t="s">
         <v>133</v>
       </c>
-      <c r="B32" t="s">
-        <v>82</v>
-      </c>
       <c r="C32" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
       </c>
       <c r="E32" t="s">
-        <v>65</v>
+        <v>134</v>
       </c>
       <c r="G32" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B33" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D33" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E33" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>133</v>
+        <v>182</v>
       </c>
       <c r="B34" t="s">
-        <v>136</v>
-      </c>
-      <c r="C34" t="s">
-        <v>13</v>
+        <v>137</v>
       </c>
       <c r="D34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G34" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>183</v>
+        <v>139</v>
       </c>
       <c r="B35" t="s">
-        <v>138</v>
+        <v>140</v>
+      </c>
+      <c r="C35" t="s">
+        <v>22</v>
       </c>
       <c r="D35" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E35" t="s">
-        <v>139</v>
+        <v>61</v>
       </c>
       <c r="G35" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B36" t="s">
-        <v>141</v>
+        <v>83</v>
       </c>
       <c r="C36" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D36" t="s">
         <v>23</v>
       </c>
       <c r="E36" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="G36" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2293,70 +2281,67 @@
         <v>142</v>
       </c>
       <c r="B37" t="s">
-        <v>83</v>
+        <v>143</v>
       </c>
       <c r="C37" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D37" t="s">
         <v>23</v>
       </c>
       <c r="E37" t="s">
-        <v>84</v>
-      </c>
-      <c r="G37" t="s">
-        <v>224</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B38" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C38" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D38" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="E38" t="s">
-        <v>62</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B39" t="s">
-        <v>146</v>
+        <v>208</v>
       </c>
       <c r="C39" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D39" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E39" t="s">
-        <v>147</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B40" t="s">
         <v>209</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="D40" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E40" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -2364,16 +2349,16 @@
         <v>148</v>
       </c>
       <c r="B41" t="s">
-        <v>210</v>
+        <v>28</v>
       </c>
       <c r="C41" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="E41" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -2381,87 +2366,90 @@
         <v>149</v>
       </c>
       <c r="B42" t="s">
-        <v>28</v>
+        <v>150</v>
       </c>
       <c r="C42" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D42" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E42" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B43" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C43" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D43" t="s">
         <v>3</v>
       </c>
       <c r="E43" t="s">
-        <v>47</v>
+        <v>153</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B44" t="s">
-        <v>153</v>
+        <v>210</v>
       </c>
       <c r="C44" t="s">
-        <v>18</v>
+        <v>154</v>
       </c>
       <c r="D44" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E44" t="s">
-        <v>154</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B45" t="s">
-        <v>211</v>
+        <v>117</v>
       </c>
       <c r="C45" t="s">
-        <v>155</v>
+        <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E45" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="G45" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B46" t="s">
-        <v>118</v>
+        <v>216</v>
       </c>
       <c r="C46" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="D46" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E46" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="G46" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -2469,90 +2457,87 @@
         <v>156</v>
       </c>
       <c r="B47" t="s">
-        <v>217</v>
+        <v>157</v>
       </c>
       <c r="C47" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E47" t="s">
-        <v>63</v>
-      </c>
-      <c r="G47" t="s">
-        <v>221</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B48" t="s">
+        <v>185</v>
+      </c>
+      <c r="C48" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" t="s">
+        <v>79</v>
+      </c>
+      <c r="G48" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A49" t="s">
+        <v>179</v>
+      </c>
+      <c r="B49" t="s">
         <v>158</v>
       </c>
-      <c r="C48" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" t="s">
-        <v>3</v>
-      </c>
-      <c r="E48" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" t="s">
-        <v>157</v>
-      </c>
-      <c r="B49" t="s">
-        <v>186</v>
-      </c>
       <c r="C49" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D49" t="s">
+        <v>31</v>
+      </c>
+      <c r="E49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" t="s">
+        <v>214</v>
+      </c>
+      <c r="B50" t="s">
+        <v>191</v>
+      </c>
+      <c r="C50" t="s">
+        <v>32</v>
+      </c>
+      <c r="D50" t="s">
         <v>5</v>
       </c>
-      <c r="E49" t="s">
-        <v>79</v>
-      </c>
-      <c r="G49" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A50" t="s">
-        <v>180</v>
-      </c>
-      <c r="B50" t="s">
-        <v>159</v>
-      </c>
-      <c r="C50" t="s">
-        <v>30</v>
-      </c>
-      <c r="D50" t="s">
-        <v>31</v>
-      </c>
       <c r="E50" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>215</v>
+        <v>159</v>
       </c>
       <c r="B51" t="s">
-        <v>192</v>
+        <v>211</v>
       </c>
       <c r="C51" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E51" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -2560,87 +2545,87 @@
         <v>160</v>
       </c>
       <c r="B52" t="s">
-        <v>212</v>
+        <v>161</v>
       </c>
       <c r="C52" t="s">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="D52" t="s">
         <v>3</v>
       </c>
       <c r="E52" t="s">
-        <v>60</v>
+        <v>162</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B53" t="s">
-        <v>162</v>
+        <v>33</v>
       </c>
       <c r="C53" t="s">
-        <v>93</v>
+        <v>7</v>
       </c>
       <c r="D53" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E53" t="s">
-        <v>163</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>164</v>
+        <v>226</v>
       </c>
       <c r="B54" t="s">
-        <v>33</v>
+        <v>121</v>
       </c>
       <c r="C54" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D54" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E54" t="s">
-        <v>64</v>
+        <v>122</v>
+      </c>
+      <c r="G54" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>230</v>
+        <v>164</v>
       </c>
       <c r="B55" t="s">
-        <v>122</v>
+        <v>165</v>
       </c>
       <c r="C55" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D55" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="E55" t="s">
-        <v>123</v>
-      </c>
-      <c r="G55" t="s">
-        <v>231</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B56" t="s">
-        <v>166</v>
+        <v>212</v>
       </c>
       <c r="C56" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="D56" t="s">
         <v>31</v>
       </c>
       <c r="E56" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2648,33 +2633,33 @@
         <v>167</v>
       </c>
       <c r="B57" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="C57" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="D57" t="s">
         <v>31</v>
       </c>
       <c r="E57" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B58" t="s">
-        <v>169</v>
+        <v>35</v>
       </c>
       <c r="C58" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D58" t="s">
         <v>31</v>
       </c>
       <c r="E58" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -2682,16 +2667,16 @@
         <v>170</v>
       </c>
       <c r="B59" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C59" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="D59" t="s">
         <v>31</v>
       </c>
       <c r="E59" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2699,16 +2684,19 @@
         <v>171</v>
       </c>
       <c r="B60" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C60" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="D60" t="s">
         <v>31</v>
       </c>
       <c r="E60" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="G60" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -2716,19 +2704,16 @@
         <v>172</v>
       </c>
       <c r="B61" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C61" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D61" t="s">
         <v>31</v>
       </c>
       <c r="E61" t="s">
-        <v>55</v>
-      </c>
-      <c r="G61" t="s">
-        <v>190</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -2736,16 +2721,19 @@
         <v>173</v>
       </c>
       <c r="B62" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C62" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D62" t="s">
         <v>31</v>
       </c>
       <c r="E62" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="G62" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2753,86 +2741,66 @@
         <v>174</v>
       </c>
       <c r="B63" t="s">
-        <v>41</v>
+        <v>175</v>
       </c>
       <c r="C63" t="s">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="D63" t="s">
         <v>31</v>
       </c>
       <c r="E63" t="s">
-        <v>56</v>
-      </c>
-      <c r="G63" t="s">
-        <v>191</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B64" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C64" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="D64" t="s">
         <v>31</v>
       </c>
       <c r="E64" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>177</v>
-      </c>
-      <c r="B65" t="s">
-        <v>178</v>
+        <v>198</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>199</v>
       </c>
       <c r="C65" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="D65" t="s">
         <v>31</v>
       </c>
       <c r="E65" t="s">
-        <v>48</v>
+        <v>200</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>199</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>200</v>
+        <v>178</v>
+      </c>
+      <c r="B66" t="s">
+        <v>213</v>
       </c>
       <c r="C66" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="D66" t="s">
         <v>31</v>
       </c>
       <c r="E66" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" t="s">
-        <v>179</v>
-      </c>
-      <c r="B67" t="s">
-        <v>214</v>
-      </c>
-      <c r="C67" t="s">
-        <v>76</v>
-      </c>
-      <c r="D67" t="s">
-        <v>31</v>
-      </c>
-      <c r="E67" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>

<commit_message>
danjoutin au lieu de rougemont
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="226">
   <si>
     <t>Date</t>
   </si>
@@ -100,9 +100,6 @@
     <t>AC Thann</t>
   </si>
   <si>
-    <t xml:space="preserve">Prix du Crédit Mutuel à Rougemont le Château  </t>
-  </si>
-  <si>
     <t>VC Soultzia</t>
   </si>
   <si>
@@ -287,9 +284,6 @@
   </si>
   <si>
     <t>frotey</t>
-  </si>
-  <si>
-    <t>rougemont</t>
   </si>
   <si>
     <t>nommay</t>
@@ -1538,7 +1532,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1546,10 +1540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="A18:XFD18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1567,47 +1561,47 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
         <v>42</v>
-      </c>
-      <c r="C1" t="s">
-        <v>43</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -1616,18 +1610,18 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1636,35 +1630,35 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1676,18 +1670,18 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -1696,18 +1690,18 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -1716,18 +1710,18 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
@@ -1736,15 +1730,15 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
@@ -1756,18 +1750,18 @@
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B11" t="s">
         <v>181</v>
-      </c>
-      <c r="B11" t="s">
-        <v>183</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -1776,18 +1770,18 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C12" t="s">
         <v>15</v>
@@ -1796,18 +1790,18 @@
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G12" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
@@ -1816,38 +1810,38 @@
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G13" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G14" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B15" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -1856,18 +1850,18 @@
         <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G15" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B16" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
@@ -1876,18 +1870,18 @@
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G16" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
@@ -1896,18 +1890,18 @@
         <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G17" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B18" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -1916,18 +1910,18 @@
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G18" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B19" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -1936,18 +1930,18 @@
         <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G19" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
@@ -1956,18 +1950,18 @@
         <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G20" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" t="s">
         <v>118</v>
-      </c>
-      <c r="B21" t="s">
-        <v>120</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
@@ -1976,50 +1970,50 @@
         <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G21" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>119</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D22" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>85</v>
+        <v>223</v>
       </c>
       <c r="G22" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B23" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>225</v>
+        <v>92</v>
       </c>
       <c r="G23" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -2030,53 +2024,53 @@
         <v>124</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
       </c>
       <c r="E24" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="G24" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" t="s">
         <v>125</v>
       </c>
-      <c r="B25" t="s">
-        <v>126</v>
-      </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="G25" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>125</v>
-      </c>
-      <c r="B26" t="s">
-        <v>127</v>
+        <v>123</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="C26" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>50</v>
+        <v>195</v>
       </c>
       <c r="G26" t="s">
         <v>215</v>
@@ -2084,22 +2078,19 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>125</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C27" t="s">
-        <v>37</v>
+        <v>126</v>
+      </c>
+      <c r="B27" t="s">
+        <v>127</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>197</v>
+        <v>71</v>
       </c>
       <c r="G27" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -2107,24 +2098,27 @@
         <v>128</v>
       </c>
       <c r="B28" t="s">
-        <v>129</v>
+        <v>204</v>
+      </c>
+      <c r="C28" t="s">
+        <v>20</v>
       </c>
       <c r="D28" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E28" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="G28" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C29" t="s">
         <v>20</v>
@@ -2133,10 +2127,10 @@
         <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="G29" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -2144,96 +2138,96 @@
         <v>130</v>
       </c>
       <c r="B30" t="s">
-        <v>207</v>
+        <v>81</v>
       </c>
       <c r="C30" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D30" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E30" t="s">
-        <v>131</v>
+        <v>64</v>
       </c>
       <c r="G30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B31" t="s">
-        <v>82</v>
+        <v>131</v>
       </c>
       <c r="C31" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
       </c>
       <c r="E31" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="G31" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B32" t="s">
         <v>133</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D32" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E32" t="s">
         <v>134</v>
       </c>
       <c r="G32" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>132</v>
+        <v>180</v>
       </c>
       <c r="B33" t="s">
         <v>135</v>
       </c>
-      <c r="C33" t="s">
-        <v>13</v>
-      </c>
       <c r="D33" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E33" t="s">
         <v>136</v>
       </c>
       <c r="G33" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>182</v>
+        <v>137</v>
       </c>
       <c r="B34" t="s">
-        <v>137</v>
+        <v>138</v>
+      </c>
+      <c r="C34" t="s">
+        <v>22</v>
       </c>
       <c r="D34" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E34" t="s">
-        <v>138</v>
+        <v>60</v>
       </c>
       <c r="G34" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -2241,39 +2235,36 @@
         <v>139</v>
       </c>
       <c r="B35" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
       <c r="C35" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D35" t="s">
         <v>23</v>
       </c>
       <c r="E35" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="G35" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" t="s">
         <v>141</v>
       </c>
-      <c r="B36" t="s">
-        <v>83</v>
-      </c>
       <c r="C36" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D36" t="s">
         <v>23</v>
       </c>
       <c r="E36" t="s">
-        <v>84</v>
-      </c>
-      <c r="G36" t="s">
-        <v>220</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2284,81 +2275,81 @@
         <v>143</v>
       </c>
       <c r="C37" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="E37" t="s">
-        <v>62</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B38" t="s">
-        <v>145</v>
+        <v>206</v>
       </c>
       <c r="C38" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E38" t="s">
-        <v>146</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B39" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C39" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="D39" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E39" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B40" t="s">
-        <v>209</v>
+        <v>19</v>
       </c>
       <c r="C40" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="E40" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
+        <v>147</v>
+      </c>
+      <c r="B41" t="s">
         <v>148</v>
       </c>
-      <c r="B41" t="s">
-        <v>28</v>
-      </c>
       <c r="C41" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D41" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E41" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -2369,229 +2360,229 @@
         <v>150</v>
       </c>
       <c r="C42" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D42" t="s">
         <v>3</v>
       </c>
       <c r="E42" t="s">
-        <v>47</v>
+        <v>151</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B43" t="s">
+        <v>208</v>
+      </c>
+      <c r="C43" t="s">
         <v>152</v>
       </c>
-      <c r="C43" t="s">
-        <v>18</v>
-      </c>
       <c r="D43" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E43" t="s">
-        <v>153</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B44" t="s">
-        <v>210</v>
+        <v>115</v>
       </c>
       <c r="C44" t="s">
-        <v>154</v>
+        <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E44" t="s">
-        <v>78</v>
+        <v>76</v>
+      </c>
+      <c r="G44" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B45" t="s">
-        <v>117</v>
+        <v>214</v>
       </c>
       <c r="C45" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="D45" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E45" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="G45" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
+        <v>154</v>
+      </c>
+      <c r="B46" t="s">
         <v>155</v>
       </c>
-      <c r="B46" t="s">
-        <v>216</v>
-      </c>
       <c r="C46" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E46" t="s">
-        <v>63</v>
-      </c>
-      <c r="G46" t="s">
-        <v>219</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" t="s">
+        <v>183</v>
+      </c>
+      <c r="C47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" t="s">
+        <v>78</v>
+      </c>
+      <c r="G47" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A48" t="s">
+        <v>177</v>
+      </c>
+      <c r="B48" t="s">
         <v>156</v>
       </c>
-      <c r="B47" t="s">
-        <v>157</v>
-      </c>
-      <c r="C47" t="s">
-        <v>8</v>
-      </c>
-      <c r="D47" t="s">
-        <v>3</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="C48" t="s">
+        <v>29</v>
+      </c>
+      <c r="D48" t="s">
+        <v>30</v>
+      </c>
+      <c r="E48" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
-      <c r="A48" t="s">
-        <v>156</v>
-      </c>
-      <c r="B48" t="s">
-        <v>185</v>
-      </c>
-      <c r="C48" t="s">
-        <v>15</v>
-      </c>
-      <c r="D48" t="s">
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
+        <v>212</v>
+      </c>
+      <c r="B49" t="s">
+        <v>189</v>
+      </c>
+      <c r="C49" t="s">
+        <v>31</v>
+      </c>
+      <c r="D49" t="s">
         <v>5</v>
       </c>
-      <c r="E48" t="s">
-        <v>79</v>
-      </c>
-      <c r="G48" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A49" t="s">
-        <v>179</v>
-      </c>
-      <c r="B49" t="s">
-        <v>158</v>
-      </c>
-      <c r="C49" t="s">
-        <v>30</v>
-      </c>
-      <c r="D49" t="s">
-        <v>31</v>
-      </c>
       <c r="E49" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>214</v>
+        <v>157</v>
       </c>
       <c r="B50" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="C50" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D50" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E50" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
+        <v>158</v>
+      </c>
+      <c r="B51" t="s">
         <v>159</v>
       </c>
-      <c r="B51" t="s">
-        <v>211</v>
-      </c>
       <c r="C51" t="s">
-        <v>2</v>
+        <v>91</v>
       </c>
       <c r="D51" t="s">
         <v>3</v>
       </c>
       <c r="E51" t="s">
-        <v>60</v>
+        <v>160</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B52" t="s">
-        <v>161</v>
+        <v>32</v>
       </c>
       <c r="C52" t="s">
-        <v>93</v>
+        <v>7</v>
       </c>
       <c r="D52" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E52" t="s">
-        <v>162</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>163</v>
+        <v>224</v>
       </c>
       <c r="B53" t="s">
-        <v>33</v>
+        <v>119</v>
       </c>
       <c r="C53" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D53" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E53" t="s">
-        <v>64</v>
+        <v>120</v>
+      </c>
+      <c r="G53" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>226</v>
+        <v>162</v>
       </c>
       <c r="B54" t="s">
-        <v>121</v>
+        <v>163</v>
       </c>
       <c r="C54" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="D54" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E54" t="s">
-        <v>122</v>
-      </c>
-      <c r="G54" t="s">
-        <v>227</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -2599,33 +2590,33 @@
         <v>164</v>
       </c>
       <c r="B55" t="s">
-        <v>165</v>
+        <v>210</v>
       </c>
       <c r="C55" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="D55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E55" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
+        <v>165</v>
+      </c>
+      <c r="B56" t="s">
         <v>166</v>
       </c>
-      <c r="B56" t="s">
-        <v>212</v>
-      </c>
       <c r="C56" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="D56" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E56" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2633,75 +2624,75 @@
         <v>167</v>
       </c>
       <c r="B57" t="s">
-        <v>168</v>
+        <v>34</v>
       </c>
       <c r="C57" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D57" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E57" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B58" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C58" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="D58" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E58" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B59" t="s">
         <v>38</v>
       </c>
       <c r="C59" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="D59" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E59" t="s">
         <v>54</v>
       </c>
+      <c r="G59" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B60" t="s">
         <v>39</v>
       </c>
       <c r="C60" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D60" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E60" t="s">
-        <v>55</v>
-      </c>
-      <c r="G60" t="s">
-        <v>189</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B61" t="s">
         <v>40</v>
@@ -2710,30 +2701,30 @@
         <v>36</v>
       </c>
       <c r="D61" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E61" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="G61" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
+        <v>172</v>
+      </c>
+      <c r="B62" t="s">
         <v>173</v>
       </c>
-      <c r="B62" t="s">
-        <v>41</v>
-      </c>
       <c r="C62" t="s">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E62" t="s">
-        <v>56</v>
-      </c>
-      <c r="G62" t="s">
-        <v>190</v>
+        <v>57</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2744,64 +2735,47 @@
         <v>175</v>
       </c>
       <c r="C63" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="D63" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E63" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>176</v>
-      </c>
-      <c r="B64" t="s">
-        <v>177</v>
+        <v>196</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="C64" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D64" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E64" t="s">
-        <v>48</v>
+        <v>198</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>198</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>199</v>
+        <v>176</v>
+      </c>
+      <c r="B65" t="s">
+        <v>211</v>
       </c>
       <c r="C65" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="D65" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E65" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" t="s">
-        <v>178</v>
-      </c>
-      <c r="B66" t="s">
-        <v>213</v>
-      </c>
-      <c r="C66" t="s">
-        <v>76</v>
-      </c>
-      <c r="D66" t="s">
-        <v>31</v>
-      </c>
-      <c r="E66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actu et nommay deplace
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7548"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
   </bookViews>
   <sheets>
     <sheet name="Calendrier" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -631,9 +631,6 @@
     <t xml:space="preserve">5e VTT MS Automobile Rixheim  </t>
   </si>
   <si>
-    <t>Dim 20 Septembre</t>
-  </si>
-  <si>
     <t>Annulé</t>
   </si>
   <si>
@@ -701,6 +698,9 @@
   </si>
   <si>
     <t>Annulé (refus de l'ONF)</t>
+  </si>
+  <si>
+    <t>Dim 18 Octobre</t>
   </si>
 </sst>
 </file>
@@ -1541,7 +1541,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1551,18 +1551,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="66.88671875" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" customWidth="1"/>
-    <col min="5" max="5" width="28.5546875" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" customWidth="1"/>
-    <col min="7" max="7" width="65.88671875" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="66.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="65.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1622,7 +1622,7 @@
         <v>67</v>
       </c>
       <c r="G3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1642,7 +1642,7 @@
         <v>99</v>
       </c>
       <c r="G4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1662,7 +1662,7 @@
         <v>70</v>
       </c>
       <c r="G5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1682,7 +1682,7 @@
         <v>85</v>
       </c>
       <c r="G6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1702,7 +1702,7 @@
         <v>86</v>
       </c>
       <c r="G7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1722,7 +1722,7 @@
         <v>69</v>
       </c>
       <c r="G8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1742,7 +1742,7 @@
         <v>68</v>
       </c>
       <c r="G9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1762,7 +1762,7 @@
         <v>87</v>
       </c>
       <c r="G10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1782,7 +1782,7 @@
         <v>53</v>
       </c>
       <c r="G11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1802,7 +1802,7 @@
         <v>89</v>
       </c>
       <c r="G12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1822,7 +1822,7 @@
         <v>88</v>
       </c>
       <c r="G13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1842,7 +1842,7 @@
         <v>181</v>
       </c>
       <c r="G14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1862,7 +1862,7 @@
         <v>44</v>
       </c>
       <c r="G15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1882,7 +1882,7 @@
         <v>68</v>
       </c>
       <c r="G16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1902,7 +1902,7 @@
         <v>73</v>
       </c>
       <c r="G17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1922,7 +1922,7 @@
         <v>44</v>
       </c>
       <c r="G18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1939,10 +1939,10 @@
         <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1962,7 +1962,7 @@
         <v>65</v>
       </c>
       <c r="G20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1982,7 +1982,7 @@
         <v>53</v>
       </c>
       <c r="G21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2002,7 +2002,7 @@
         <v>92</v>
       </c>
       <c r="G22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -2022,7 +2022,7 @@
         <v>66</v>
       </c>
       <c r="G23" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -2042,7 +2042,7 @@
         <v>49</v>
       </c>
       <c r="G24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -2062,7 +2062,7 @@
         <v>190</v>
       </c>
       <c r="G25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -2079,7 +2079,7 @@
         <v>71</v>
       </c>
       <c r="G26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -2099,7 +2099,7 @@
         <v>48</v>
       </c>
       <c r="G27" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -2119,7 +2119,7 @@
         <v>128</v>
       </c>
       <c r="G28" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -2139,7 +2139,7 @@
         <v>64</v>
       </c>
       <c r="G29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -2159,7 +2159,7 @@
         <v>131</v>
       </c>
       <c r="G30" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -2179,7 +2179,7 @@
         <v>133</v>
       </c>
       <c r="G31" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -2196,7 +2196,7 @@
         <v>135</v>
       </c>
       <c r="G32" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -2216,7 +2216,7 @@
         <v>60</v>
       </c>
       <c r="G33" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -2236,7 +2236,7 @@
         <v>83</v>
       </c>
       <c r="G34" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -2256,7 +2256,7 @@
         <v>61</v>
       </c>
       <c r="G35" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -2276,7 +2276,7 @@
         <v>143</v>
       </c>
       <c r="G36" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2296,7 +2296,7 @@
         <v>50</v>
       </c>
       <c r="G37" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -2316,7 +2316,7 @@
         <v>72</v>
       </c>
       <c r="G38" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -2353,7 +2353,7 @@
         <v>46</v>
       </c>
       <c r="G40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -2407,7 +2407,7 @@
         <v>76</v>
       </c>
       <c r="G43" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -2415,7 +2415,7 @@
         <v>152</v>
       </c>
       <c r="B44" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C44" t="s">
         <v>4</v>
@@ -2424,10 +2424,10 @@
         <v>3</v>
       </c>
       <c r="E44" t="s">
+        <v>216</v>
+      </c>
+      <c r="G44" t="s">
         <v>217</v>
-      </c>
-      <c r="G44" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -2435,7 +2435,7 @@
         <v>152</v>
       </c>
       <c r="B45" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C45" t="s">
         <v>28</v>
@@ -2447,7 +2447,7 @@
         <v>62</v>
       </c>
       <c r="G45" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -2506,132 +2506,132 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>205</v>
+        <v>156</v>
       </c>
       <c r="B49" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="C49" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E49" t="s">
-        <v>90</v>
+        <v>226</v>
+      </c>
+      <c r="G49" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B50" t="s">
-        <v>204</v>
+        <v>158</v>
       </c>
       <c r="C50" t="s">
-        <v>2</v>
+        <v>91</v>
       </c>
       <c r="D50" t="s">
         <v>3</v>
       </c>
       <c r="E50" t="s">
-        <v>227</v>
-      </c>
-      <c r="G50" t="s">
-        <v>228</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B51" t="s">
-        <v>158</v>
+        <v>32</v>
       </c>
       <c r="C51" t="s">
-        <v>91</v>
+        <v>7</v>
       </c>
       <c r="D51" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E51" t="s">
-        <v>159</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>160</v>
+        <v>213</v>
       </c>
       <c r="B52" t="s">
-        <v>32</v>
+        <v>218</v>
       </c>
       <c r="C52" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D52" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E52" t="s">
-        <v>63</v>
+        <v>119</v>
+      </c>
+      <c r="G52" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>214</v>
+        <v>161</v>
       </c>
       <c r="B53" t="s">
-        <v>219</v>
+        <v>162</v>
       </c>
       <c r="C53" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="D53" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E53" t="s">
-        <v>119</v>
-      </c>
-      <c r="G53" t="s">
-        <v>215</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B54" t="s">
-        <v>162</v>
+        <v>223</v>
       </c>
       <c r="C54" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="D54" t="s">
         <v>30</v>
       </c>
       <c r="E54" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>163</v>
+        <v>228</v>
       </c>
       <c r="B55" t="s">
-        <v>224</v>
+        <v>184</v>
       </c>
       <c r="C55" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="D55" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E55" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B56" t="s">
         <v>164</v>
@@ -2648,7 +2648,7 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B57" t="s">
         <v>34</v>
@@ -2702,10 +2702,10 @@
     </row>
     <row r="60" spans="1:7" ht="14.25" customHeight="1">
       <c r="A60" t="s">
+        <v>221</v>
+      </c>
+      <c r="B60" t="s">
         <v>222</v>
-      </c>
-      <c r="B60" t="s">
-        <v>223</v>
       </c>
       <c r="C60" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
3h vtt complet et consignes sanitaires
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -646,9 +646,6 @@
     <t>Annulés</t>
   </si>
   <si>
-    <t>Nouvelle date</t>
-  </si>
-  <si>
     <t>seppois_old</t>
   </si>
   <si>
@@ -698,6 +695,9 @@
   </si>
   <si>
     <t>Dim 18 Octobre</t>
+  </si>
+  <si>
+    <t>COMPLET !</t>
   </si>
 </sst>
 </file>
@@ -1538,7 +1538,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1549,7 +1549,7 @@
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1936,7 +1936,7 @@
         <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G19" t="s">
         <v>204</v>
@@ -2253,7 +2253,7 @@
         <v>61</v>
       </c>
       <c r="G35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -2293,7 +2293,7 @@
         <v>50</v>
       </c>
       <c r="G37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -2404,7 +2404,7 @@
         <v>76</v>
       </c>
       <c r="G43" t="s">
-        <v>210</v>
+        <v>227</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -2412,7 +2412,7 @@
         <v>152</v>
       </c>
       <c r="B44" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C44" t="s">
         <v>4</v>
@@ -2421,10 +2421,10 @@
         <v>3</v>
       </c>
       <c r="E44" t="s">
+        <v>214</v>
+      </c>
+      <c r="G44" t="s">
         <v>215</v>
-      </c>
-      <c r="G44" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -2521,10 +2521,10 @@
         <v>3</v>
       </c>
       <c r="E49" t="s">
+        <v>224</v>
+      </c>
+      <c r="G49" t="s">
         <v>225</v>
-      </c>
-      <c r="G49" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -2563,10 +2563,10 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B52" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C52" t="s">
         <v>13</v>
@@ -2578,7 +2578,7 @@
         <v>119</v>
       </c>
       <c r="G52" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -2603,7 +2603,7 @@
         <v>163</v>
       </c>
       <c r="B54" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C54" t="s">
         <v>79</v>
@@ -2617,7 +2617,7 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B55" t="s">
         <v>183</v>
@@ -2634,7 +2634,7 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B56" t="s">
         <v>164</v>
@@ -2651,7 +2651,7 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B57" t="s">
         <v>34</v>
@@ -2705,10 +2705,10 @@
     </row>
     <row r="60" spans="1:7" ht="14.25" customHeight="1">
       <c r="A60" t="s">
+        <v>219</v>
+      </c>
+      <c r="B60" t="s">
         <v>220</v>
-      </c>
-      <c r="B60" t="s">
-        <v>221</v>
       </c>
       <c r="C60" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
rmv publi Autechaux et changement date journee sport detente
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Calendrier" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -538,9 +538,6 @@
     <t>https://www.cyclosportive-lesmarcaires.fr/</t>
   </si>
   <si>
-    <t>Journée Sport et Détente à Beaucourt (à confirmer)</t>
-  </si>
-  <si>
     <t>3&lt;sup&gt;e&lt;/sup&gt; VTT Peugeot (à confirmer)</t>
   </si>
   <si>
@@ -743,6 +740,9 @@
   </si>
   <si>
     <t xml:space="preserve">La Super cUp VTT (toutes catégories FSGT uniquement) </t>
+  </si>
+  <si>
+    <t>Journée Sport et Détente à Beaucourt</t>
   </si>
 </sst>
 </file>
@@ -1579,8 +1579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1618,10 +1618,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1633,7 +1633,7 @@
         <v>157</v>
       </c>
       <c r="G2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1653,7 +1653,7 @@
         <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1673,7 +1673,7 @@
         <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1681,7 +1681,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
@@ -1693,7 +1693,7 @@
         <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1713,7 +1713,7 @@
         <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1733,7 +1733,7 @@
         <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1753,7 +1753,7 @@
         <v>27</v>
       </c>
       <c r="G8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1773,7 +1773,7 @@
         <v>31</v>
       </c>
       <c r="G9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1781,7 +1781,7 @@
         <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C10" t="s">
         <v>33</v>
@@ -1793,7 +1793,7 @@
         <v>34</v>
       </c>
       <c r="G10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1810,10 +1810,10 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1821,7 +1821,7 @@
         <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C12" t="s">
         <v>30</v>
@@ -1833,7 +1833,7 @@
         <v>37</v>
       </c>
       <c r="G12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1853,7 +1853,7 @@
         <v>15</v>
       </c>
       <c r="G13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1873,10 +1873,10 @@
         <v>173</v>
       </c>
       <c r="F14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1884,7 +1884,7 @@
         <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C15" t="s">
         <v>43</v>
@@ -1893,18 +1893,18 @@
         <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C16" t="s">
         <v>59</v>
@@ -1913,10 +1913,10 @@
         <v>5</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1924,7 +1924,7 @@
         <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
@@ -1941,7 +1941,7 @@
         <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C18" t="s">
         <v>47</v>
@@ -1984,7 +1984,7 @@
         <v>5</v>
       </c>
       <c r="E20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -2006,56 +2006,59 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>174</v>
+        <v>233</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>58</v>
+        <v>60</v>
+      </c>
+      <c r="G22" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>234</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>60</v>
-      </c>
-      <c r="G23" t="s">
-        <v>192</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>167</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D24" t="s">
         <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>62</v>
+        <v>65</v>
+      </c>
+      <c r="G24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -2063,7 +2066,7 @@
         <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C25" t="s">
         <v>64</v>
@@ -2072,10 +2075,7 @@
         <v>5</v>
       </c>
       <c r="E25" t="s">
-        <v>65</v>
-      </c>
-      <c r="G25" t="s">
-        <v>180</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -2083,7 +2083,7 @@
         <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>168</v>
+        <v>234</v>
       </c>
       <c r="C26" t="s">
         <v>64</v>
@@ -2092,7 +2092,7 @@
         <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>66</v>
+        <v>229</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -2114,36 +2114,36 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>224</v>
       </c>
       <c r="B28" t="s">
-        <v>236</v>
-      </c>
-      <c r="C28" t="s">
-        <v>64</v>
+        <v>223</v>
       </c>
       <c r="D28" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>231</v>
+        <v>67</v>
+      </c>
+      <c r="G28" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>225</v>
+        <v>68</v>
       </c>
       <c r="B29" t="s">
-        <v>224</v>
+        <v>242</v>
+      </c>
+      <c r="C29" t="s">
+        <v>23</v>
       </c>
       <c r="D29" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="E29" t="s">
-        <v>67</v>
-      </c>
-      <c r="G29" t="s">
-        <v>192</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -2185,7 +2185,7 @@
         <v>68</v>
       </c>
       <c r="B32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C32" t="s">
         <v>14</v>
@@ -2219,7 +2219,7 @@
         <v>75</v>
       </c>
       <c r="B34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C34" t="s">
         <v>16</v>
@@ -2228,7 +2228,7 @@
         <v>5</v>
       </c>
       <c r="E34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -2236,7 +2236,7 @@
         <v>75</v>
       </c>
       <c r="B35" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C35" t="s">
         <v>78</v>
@@ -2265,7 +2265,7 @@
         <v>6</v>
       </c>
       <c r="G36" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2273,7 +2273,7 @@
         <v>81</v>
       </c>
       <c r="B37" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C37" t="s">
         <v>82</v>
@@ -2285,7 +2285,7 @@
         <v>83</v>
       </c>
       <c r="G37" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -2305,7 +2305,7 @@
         <v>15</v>
       </c>
       <c r="G38" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -2327,10 +2327,10 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B40" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C40" t="s">
         <v>16</v>
@@ -2342,24 +2342,24 @@
         <v>17</v>
       </c>
       <c r="G40" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
+        <v>193</v>
+      </c>
+      <c r="B41" t="s">
         <v>194</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>195</v>
-      </c>
-      <c r="C41" t="s">
-        <v>196</v>
       </c>
       <c r="D41" t="s">
         <v>10</v>
       </c>
       <c r="E41" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -2398,22 +2398,22 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
+        <v>203</v>
+      </c>
+      <c r="B44" t="s">
+        <v>240</v>
+      </c>
+      <c r="C44" t="s">
         <v>204</v>
-      </c>
-      <c r="B44" t="s">
-        <v>241</v>
-      </c>
-      <c r="C44" t="s">
-        <v>205</v>
       </c>
       <c r="D44" t="s">
         <v>10</v>
       </c>
       <c r="E44" t="s">
+        <v>205</v>
+      </c>
+      <c r="G44" t="s">
         <v>206</v>
-      </c>
-      <c r="G44" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -2447,7 +2447,7 @@
         <v>5</v>
       </c>
       <c r="E46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -2455,7 +2455,7 @@
         <v>97</v>
       </c>
       <c r="B47" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C47" t="s">
         <v>20</v>
@@ -2523,7 +2523,7 @@
         <v>102</v>
       </c>
       <c r="B51" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C51" t="s">
         <v>108</v>
@@ -2540,7 +2540,7 @@
         <v>105</v>
       </c>
       <c r="B52" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C52" t="s">
         <v>59</v>
@@ -2549,7 +2549,7 @@
         <v>48</v>
       </c>
       <c r="E52" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -2574,7 +2574,7 @@
         <v>113</v>
       </c>
       <c r="B54" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C54" t="s">
         <v>114</v>
@@ -2591,7 +2591,7 @@
         <v>113</v>
       </c>
       <c r="B55" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C55" t="s">
         <v>30</v>
@@ -2608,7 +2608,7 @@
         <v>117</v>
       </c>
       <c r="B56" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C56" t="s">
         <v>33</v>
@@ -2620,7 +2620,7 @@
         <v>34</v>
       </c>
       <c r="G56" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2628,7 +2628,7 @@
         <v>117</v>
       </c>
       <c r="B57" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C57" t="s">
         <v>118</v>
@@ -2645,7 +2645,7 @@
         <v>121</v>
       </c>
       <c r="B58" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C58" t="s">
         <v>118</v>
@@ -2662,7 +2662,7 @@
         <v>122</v>
       </c>
       <c r="B59" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C59" t="s">
         <v>16</v>
@@ -2674,7 +2674,7 @@
         <v>17</v>
       </c>
       <c r="G59" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2713,7 +2713,7 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B62" t="s">
         <v>26</v>
@@ -2728,7 +2728,7 @@
         <v>27</v>
       </c>
       <c r="G62" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2770,7 +2770,7 @@
         <v>133</v>
       </c>
       <c r="B65" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C65" t="s">
         <v>134</v>
@@ -2801,7 +2801,7 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B67" t="s">
         <v>139</v>
@@ -2838,7 +2838,7 @@
         <v>146</v>
       </c>
       <c r="B69" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C69" t="s">
         <v>59</v>
@@ -2889,7 +2889,7 @@
         <v>151</v>
       </c>
       <c r="B72" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C72" t="s">
         <v>59</v>
@@ -2923,7 +2923,7 @@
         <v>158</v>
       </c>
       <c r="B74" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C74" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
ajout cyclo tour alsace
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="245">
   <si>
     <t>Date</t>
   </si>
@@ -637,9 +637,6 @@
     <t>Reporté au 18 Juillet</t>
   </si>
   <si>
-    <t>Dim 18 Juillet</t>
-  </si>
-  <si>
     <t>12&lt;sup&gt;e&lt;/sup&gt; Prix de Boron</t>
   </si>
   <si>
@@ -688,9 +685,6 @@
     <t>3 et 4 Juillet</t>
   </si>
   <si>
-    <t>Reporté au 26 Septembre (en raison du TTB)</t>
-  </si>
-  <si>
     <t>magstatt_vtt</t>
   </si>
   <si>
@@ -743,6 +737,18 @@
   </si>
   <si>
     <t>Grimpée des Bagenelles</t>
+  </si>
+  <si>
+    <t>Sam 24 Juillet</t>
+  </si>
+  <si>
+    <t>Etape Cyclo du Tour Alsace</t>
+  </si>
+  <si>
+    <t>FSGT</t>
+  </si>
+  <si>
+    <t>https://www.touralsace.fr/boutique/etape-cyclo/</t>
   </si>
 </sst>
 </file>
@@ -1579,8 +1585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1753,7 +1759,7 @@
         <v>27</v>
       </c>
       <c r="G8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1773,7 +1779,7 @@
         <v>31</v>
       </c>
       <c r="G9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1781,7 +1787,7 @@
         <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C10" t="s">
         <v>33</v>
@@ -1793,7 +1799,7 @@
         <v>34</v>
       </c>
       <c r="G10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1833,7 +1839,7 @@
         <v>37</v>
       </c>
       <c r="G12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1853,7 +1859,7 @@
         <v>15</v>
       </c>
       <c r="G13" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1896,15 +1902,15 @@
         <v>199</v>
       </c>
       <c r="G15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B16" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C16" t="s">
         <v>59</v>
@@ -1913,10 +1919,10 @@
         <v>5</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1924,7 +1930,7 @@
         <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
@@ -1941,7 +1947,7 @@
         <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C18" t="s">
         <v>47</v>
@@ -1984,7 +1990,7 @@
         <v>5</v>
       </c>
       <c r="E20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -2009,7 +2015,7 @@
         <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C22" t="s">
         <v>59</v>
@@ -2083,7 +2089,7 @@
         <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C26" t="s">
         <v>64</v>
@@ -2092,7 +2098,7 @@
         <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -2100,7 +2106,7 @@
         <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C27" t="s">
         <v>64</v>
@@ -2109,15 +2115,15 @@
         <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B28" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D28" t="s">
         <v>10</v>
@@ -2134,7 +2140,7 @@
         <v>68</v>
       </c>
       <c r="B29" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C29" t="s">
         <v>23</v>
@@ -2236,7 +2242,7 @@
         <v>75</v>
       </c>
       <c r="B35" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C35" t="s">
         <v>78</v>
@@ -2248,7 +2254,7 @@
         <v>80</v>
       </c>
       <c r="G35" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -2268,7 +2274,7 @@
         <v>6</v>
       </c>
       <c r="G36" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2308,7 +2314,7 @@
         <v>15</v>
       </c>
       <c r="G38" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -2330,22 +2336,19 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>207</v>
+        <v>241</v>
       </c>
       <c r="B40" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
       <c r="C40" t="s">
-        <v>16</v>
+        <v>243</v>
       </c>
       <c r="D40" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="E40" t="s">
-        <v>17</v>
-      </c>
-      <c r="G40" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -2404,7 +2407,7 @@
         <v>202</v>
       </c>
       <c r="B44" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C44" t="s">
         <v>203</v>
@@ -2450,7 +2453,7 @@
         <v>5</v>
       </c>
       <c r="E46" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -2526,7 +2529,7 @@
         <v>102</v>
       </c>
       <c r="B51" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C51" t="s">
         <v>108</v>
@@ -2543,7 +2546,7 @@
         <v>105</v>
       </c>
       <c r="B52" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C52" t="s">
         <v>59</v>
@@ -2552,7 +2555,7 @@
         <v>48</v>
       </c>
       <c r="E52" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -2611,7 +2614,7 @@
         <v>117</v>
       </c>
       <c r="B56" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C56" t="s">
         <v>33</v>
@@ -2623,7 +2626,7 @@
         <v>34</v>
       </c>
       <c r="G56" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2665,7 +2668,7 @@
         <v>122</v>
       </c>
       <c r="B59" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C59" t="s">
         <v>16</v>
@@ -2677,7 +2680,7 @@
         <v>17</v>
       </c>
       <c r="G59" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2716,7 +2719,7 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B62" t="s">
         <v>26</v>
@@ -2731,7 +2734,7 @@
         <v>27</v>
       </c>
       <c r="G62" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="63" spans="1:7">

</xml_diff>

<commit_message>
maj calendrier et suppression de ../
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Calendrier" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="244">
   <si>
     <t>Date</t>
   </si>
@@ -520,9 +520,6 @@
     <t xml:space="preserve">12&lt;sup&gt;e&lt;/sup&gt; Nuit des Gros Mollets jeunes à Flaxlanden (poussins à minimes)  </t>
   </si>
   <si>
-    <t xml:space="preserve">24&lt;sup&gt;e&lt;/sup&gt; Montée du Floridor, col du Hundsruck à Thann  </t>
-  </si>
-  <si>
     <t xml:space="preserve">20&lt;sup&gt;e&lt;/sup&gt; Grimpée du Col Amic à Soultz  </t>
   </si>
   <si>
@@ -535,9 +532,6 @@
     <t>https://www.cyclosportive-lesmarcaires.fr/</t>
   </si>
   <si>
-    <t>3&lt;sup&gt;e&lt;/sup&gt; VTT Peugeot (à confirmer)</t>
-  </si>
-  <si>
     <t>Dim 24 Janvier</t>
   </si>
   <si>
@@ -746,6 +740,12 @@
   </si>
   <si>
     <t>Sous l'égide de la FFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24&lt;sup&gt;e&lt;/sup&gt; Montée du Floridor, col du Hundsrück à Thann  </t>
+  </si>
+  <si>
+    <t>3&lt;sup&gt;e&lt;/sup&gt; VTT Peugeot</t>
   </si>
 </sst>
 </file>
@@ -1582,8 +1582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1621,10 +1621,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1636,7 +1636,7 @@
         <v>156</v>
       </c>
       <c r="G2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1656,7 +1656,7 @@
         <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1676,7 +1676,7 @@
         <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1696,7 +1696,7 @@
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1716,7 +1716,7 @@
         <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1736,7 +1736,7 @@
         <v>26</v>
       </c>
       <c r="G7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1756,7 +1756,7 @@
         <v>30</v>
       </c>
       <c r="G8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1764,7 +1764,7 @@
         <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C9" t="s">
         <v>32</v>
@@ -1776,7 +1776,7 @@
         <v>33</v>
       </c>
       <c r="G9" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1793,10 +1793,10 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G10" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1804,7 +1804,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C11" t="s">
         <v>29</v>
@@ -1816,7 +1816,7 @@
         <v>36</v>
       </c>
       <c r="G11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1836,7 +1836,7 @@
         <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1853,13 +1853,13 @@
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1867,7 +1867,7 @@
         <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C14" t="s">
         <v>42</v>
@@ -1876,18 +1876,18 @@
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C15" t="s">
         <v>58</v>
@@ -1896,10 +1896,10 @@
         <v>5</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1907,7 +1907,7 @@
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
@@ -1924,7 +1924,7 @@
         <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C17" t="s">
         <v>46</v>
@@ -1967,7 +1967,7 @@
         <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1992,7 +1992,7 @@
         <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C21" t="s">
         <v>58</v>
@@ -2004,7 +2004,7 @@
         <v>59</v>
       </c>
       <c r="G21" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2041,7 +2041,7 @@
         <v>64</v>
       </c>
       <c r="G23" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -2061,7 +2061,7 @@
         <v>65</v>
       </c>
       <c r="G24" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -2069,7 +2069,7 @@
         <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C25" t="s">
         <v>63</v>
@@ -2078,10 +2078,10 @@
         <v>5</v>
       </c>
       <c r="E25" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G25" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -2089,7 +2089,7 @@
         <v>62</v>
       </c>
       <c r="B26" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C26" t="s">
         <v>63</v>
@@ -2098,18 +2098,18 @@
         <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G26" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B27" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
@@ -2118,7 +2118,7 @@
         <v>66</v>
       </c>
       <c r="G27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -2126,7 +2126,7 @@
         <v>67</v>
       </c>
       <c r="B28" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C28" t="s">
         <v>22</v>
@@ -2177,7 +2177,7 @@
         <v>67</v>
       </c>
       <c r="B31" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C31" t="s">
         <v>13</v>
@@ -2211,7 +2211,7 @@
         <v>74</v>
       </c>
       <c r="B33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C33" t="s">
         <v>15</v>
@@ -2220,7 +2220,7 @@
         <v>5</v>
       </c>
       <c r="E33" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -2228,7 +2228,7 @@
         <v>74</v>
       </c>
       <c r="B34" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C34" t="s">
         <v>77</v>
@@ -2240,7 +2240,7 @@
         <v>79</v>
       </c>
       <c r="G34" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -2265,7 +2265,7 @@
         <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C36" t="s">
         <v>81</v>
@@ -2277,7 +2277,7 @@
         <v>82</v>
       </c>
       <c r="G36" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2314,41 +2314,41 @@
         <v>85</v>
       </c>
       <c r="G38" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
+        <v>227</v>
+      </c>
+      <c r="B39" t="s">
+        <v>228</v>
+      </c>
+      <c r="C39" t="s">
         <v>229</v>
-      </c>
-      <c r="B39" t="s">
-        <v>230</v>
-      </c>
-      <c r="C39" t="s">
-        <v>231</v>
       </c>
       <c r="D39" t="s">
         <v>47</v>
       </c>
       <c r="E39" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
+        <v>187</v>
+      </c>
+      <c r="B40" t="s">
+        <v>188</v>
+      </c>
+      <c r="C40" t="s">
         <v>189</v>
-      </c>
-      <c r="B40" t="s">
-        <v>190</v>
-      </c>
-      <c r="C40" t="s">
-        <v>191</v>
       </c>
       <c r="D40" t="s">
         <v>10</v>
       </c>
       <c r="E40" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -2370,22 +2370,22 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B42" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C42" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D42" t="s">
         <v>10</v>
       </c>
       <c r="E42" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G42" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -2393,7 +2393,7 @@
         <v>90</v>
       </c>
       <c r="B43" t="s">
-        <v>168</v>
+        <v>242</v>
       </c>
       <c r="C43" t="s">
         <v>91</v>
@@ -2403,6 +2403,9 @@
       </c>
       <c r="E43" t="s">
         <v>92</v>
+      </c>
+      <c r="G43" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -2422,7 +2425,7 @@
         <v>95</v>
       </c>
       <c r="G44" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -2439,7 +2442,7 @@
         <v>5</v>
       </c>
       <c r="E45" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -2447,7 +2450,7 @@
         <v>96</v>
       </c>
       <c r="B46" t="s">
-        <v>173</v>
+        <v>243</v>
       </c>
       <c r="C46" t="s">
         <v>19</v>
@@ -2459,7 +2462,7 @@
         <v>97</v>
       </c>
       <c r="G46" t="s">
-        <v>239</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -2496,7 +2499,7 @@
         <v>103</v>
       </c>
       <c r="G48" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -2504,7 +2507,7 @@
         <v>101</v>
       </c>
       <c r="B49" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C49" t="s">
         <v>107</v>
@@ -2533,7 +2536,7 @@
         <v>106</v>
       </c>
       <c r="G50" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -2541,7 +2544,7 @@
         <v>104</v>
       </c>
       <c r="B51" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C51" t="s">
         <v>58</v>
@@ -2550,7 +2553,7 @@
         <v>47</v>
       </c>
       <c r="E51" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -2558,7 +2561,7 @@
         <v>109</v>
       </c>
       <c r="B52" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C52" t="s">
         <v>110</v>
@@ -2575,7 +2578,7 @@
         <v>112</v>
       </c>
       <c r="B53" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C53" t="s">
         <v>113</v>
@@ -2587,7 +2590,7 @@
         <v>114</v>
       </c>
       <c r="G53" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -2595,7 +2598,7 @@
         <v>112</v>
       </c>
       <c r="B54" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C54" t="s">
         <v>29</v>
@@ -2612,7 +2615,7 @@
         <v>116</v>
       </c>
       <c r="B55" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C55" t="s">
         <v>32</v>
@@ -2624,7 +2627,7 @@
         <v>33</v>
       </c>
       <c r="G55" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -2632,7 +2635,7 @@
         <v>116</v>
       </c>
       <c r="B56" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C56" t="s">
         <v>117</v>
@@ -2649,7 +2652,7 @@
         <v>120</v>
       </c>
       <c r="B57" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C57" t="s">
         <v>117</v>
@@ -2666,7 +2669,7 @@
         <v>121</v>
       </c>
       <c r="B58" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C58" t="s">
         <v>15</v>
@@ -2678,7 +2681,7 @@
         <v>16</v>
       </c>
       <c r="G58" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -2698,7 +2701,7 @@
         <v>123</v>
       </c>
       <c r="G59" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2720,7 +2723,7 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B61" t="s">
         <v>25</v>
@@ -2757,7 +2760,7 @@
         <v>130</v>
       </c>
       <c r="B63" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C63" t="s">
         <v>81</v>
@@ -2774,7 +2777,7 @@
         <v>132</v>
       </c>
       <c r="B64" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C64" t="s">
         <v>133</v>
@@ -2805,7 +2808,7 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B66" t="s">
         <v>138</v>
@@ -2839,10 +2842,10 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B68" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C68" t="s">
         <v>143</v>
@@ -2851,7 +2854,7 @@
         <v>118</v>
       </c>
       <c r="E68" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -2859,7 +2862,7 @@
         <v>145</v>
       </c>
       <c r="B69" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C69" t="s">
         <v>58</v>
@@ -2876,7 +2879,7 @@
         <v>147</v>
       </c>
       <c r="B70" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C70" t="s">
         <v>148</v>
@@ -2910,7 +2913,7 @@
         <v>150</v>
       </c>
       <c r="B72" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C72" t="s">
         <v>58</v>
@@ -2944,7 +2947,7 @@
         <v>157</v>
       </c>
       <c r="B74" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C74" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
changement date gentleman nommay
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Calendrier" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="238">
   <si>
     <t>Date</t>
   </si>
@@ -394,9 +394,6 @@
     <t>morschwiller</t>
   </si>
   <si>
-    <t>Dim 17 Octobre</t>
-  </si>
-  <si>
     <t>CCI Nommay</t>
   </si>
   <si>
@@ -724,16 +721,13 @@
     <t>Wittenheim Cross Tour</t>
   </si>
   <si>
-    <t>Anciennement Rougemont-le-Château</t>
-  </si>
-  <si>
-    <t>Annulé (nouvelles restrictions sanitaires depuis le 9 Août)</t>
-  </si>
-  <si>
     <t>Prix Gekobike à Heimsbrunn</t>
   </si>
   <si>
     <t>heimsbrunn_vtt</t>
+  </si>
+  <si>
+    <t>Dim 10 Octobre</t>
   </si>
 </sst>
 </file>
@@ -1570,8 +1564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1589,30 +1583,30 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" t="s">
         <v>156</v>
-      </c>
-      <c r="C1" t="s">
-        <v>157</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F1" t="s">
         <v>153</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>154</v>
-      </c>
-      <c r="G1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1621,10 +1615,10 @@
         <v>114</v>
       </c>
       <c r="E2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1644,7 +1638,7 @@
         <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1652,7 +1646,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -1664,7 +1658,7 @@
         <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1684,7 +1678,7 @@
         <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1704,7 +1698,7 @@
         <v>28</v>
       </c>
       <c r="G6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1712,7 +1706,7 @@
         <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C7" t="s">
         <v>30</v>
@@ -1724,7 +1718,7 @@
         <v>31</v>
       </c>
       <c r="G7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1741,10 +1735,10 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1752,7 +1746,7 @@
         <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
@@ -1764,7 +1758,7 @@
         <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1781,13 +1775,13 @@
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1795,7 +1789,7 @@
         <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C11" t="s">
         <v>40</v>
@@ -1804,18 +1798,18 @@
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C12" t="s">
         <v>56</v>
@@ -1824,10 +1818,10 @@
         <v>4</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1835,7 +1829,7 @@
         <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
@@ -1852,7 +1846,7 @@
         <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C14" t="s">
         <v>44</v>
@@ -1895,7 +1889,7 @@
         <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1920,7 +1914,7 @@
         <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C18" t="s">
         <v>56</v>
@@ -1932,7 +1926,7 @@
         <v>57</v>
       </c>
       <c r="G18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1957,7 +1951,7 @@
         <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C20" t="s">
         <v>61</v>
@@ -1969,7 +1963,7 @@
         <v>62</v>
       </c>
       <c r="G20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1977,7 +1971,7 @@
         <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C21" t="s">
         <v>61</v>
@@ -1989,7 +1983,7 @@
         <v>63</v>
       </c>
       <c r="G21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1997,7 +1991,7 @@
         <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C22" t="s">
         <v>61</v>
@@ -2006,10 +2000,10 @@
         <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -2017,7 +2011,7 @@
         <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C23" t="s">
         <v>61</v>
@@ -2026,18 +2020,18 @@
         <v>4</v>
       </c>
       <c r="E23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
@@ -2046,7 +2040,7 @@
         <v>64</v>
       </c>
       <c r="G24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -2054,7 +2048,7 @@
         <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C25" t="s">
         <v>20</v>
@@ -2105,7 +2099,7 @@
         <v>65</v>
       </c>
       <c r="B28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C28" t="s">
         <v>11</v>
@@ -2139,7 +2133,7 @@
         <v>72</v>
       </c>
       <c r="B30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C30" t="s">
         <v>13</v>
@@ -2148,7 +2142,7 @@
         <v>4</v>
       </c>
       <c r="E30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -2156,7 +2150,7 @@
         <v>72</v>
       </c>
       <c r="B31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C31" t="s">
         <v>75</v>
@@ -2168,7 +2162,7 @@
         <v>77</v>
       </c>
       <c r="G31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -2193,7 +2187,7 @@
         <v>78</v>
       </c>
       <c r="B33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C33" t="s">
         <v>79</v>
@@ -2205,7 +2199,7 @@
         <v>80</v>
       </c>
       <c r="G33" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -2242,41 +2236,41 @@
         <v>83</v>
       </c>
       <c r="G35" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
+        <v>217</v>
+      </c>
+      <c r="B36" t="s">
         <v>218</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>219</v>
-      </c>
-      <c r="C36" t="s">
-        <v>220</v>
       </c>
       <c r="D36" t="s">
         <v>45</v>
       </c>
       <c r="E36" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
+        <v>179</v>
+      </c>
+      <c r="B37" t="s">
         <v>180</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>181</v>
-      </c>
-      <c r="C37" t="s">
-        <v>182</v>
       </c>
       <c r="D37" t="s">
         <v>8</v>
       </c>
       <c r="E37" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -2298,22 +2292,22 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
+        <v>188</v>
+      </c>
+      <c r="B39" t="s">
+        <v>214</v>
+      </c>
+      <c r="C39" t="s">
         <v>189</v>
-      </c>
-      <c r="B39" t="s">
-        <v>215</v>
-      </c>
-      <c r="C39" t="s">
-        <v>190</v>
       </c>
       <c r="D39" t="s">
         <v>8</v>
       </c>
       <c r="E39" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G39" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -2321,7 +2315,7 @@
         <v>88</v>
       </c>
       <c r="B40" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C40" t="s">
         <v>89</v>
@@ -2333,7 +2327,7 @@
         <v>90</v>
       </c>
       <c r="G40" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -2353,7 +2347,7 @@
         <v>93</v>
       </c>
       <c r="G41" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -2361,7 +2355,7 @@
         <v>91</v>
       </c>
       <c r="B42" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C42" t="s">
         <v>35</v>
@@ -2370,10 +2364,10 @@
         <v>4</v>
       </c>
       <c r="E42" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G42" t="s">
-        <v>237</v>
+        <v>177</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -2381,7 +2375,7 @@
         <v>94</v>
       </c>
       <c r="B43" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C43" t="s">
         <v>17</v>
@@ -2393,7 +2387,7 @@
         <v>95</v>
       </c>
       <c r="G43" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -2412,9 +2406,6 @@
       <c r="E44" t="s">
         <v>9</v>
       </c>
-      <c r="G44" t="s">
-        <v>236</v>
-      </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
@@ -2433,7 +2424,7 @@
         <v>99</v>
       </c>
       <c r="G45" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -2441,7 +2432,7 @@
         <v>97</v>
       </c>
       <c r="B46" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C46" t="s">
         <v>103</v>
@@ -2470,7 +2461,7 @@
         <v>102</v>
       </c>
       <c r="G47" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -2478,7 +2469,7 @@
         <v>100</v>
       </c>
       <c r="B48" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C48" t="s">
         <v>56</v>
@@ -2487,7 +2478,7 @@
         <v>45</v>
       </c>
       <c r="E48" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -2495,7 +2486,7 @@
         <v>105</v>
       </c>
       <c r="B49" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C49" t="s">
         <v>106</v>
@@ -2512,7 +2503,7 @@
         <v>108</v>
       </c>
       <c r="B50" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C50" t="s">
         <v>109</v>
@@ -2524,7 +2515,7 @@
         <v>110</v>
       </c>
       <c r="G50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -2532,7 +2523,7 @@
         <v>108</v>
       </c>
       <c r="B51" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C51" t="s">
         <v>27</v>
@@ -2549,7 +2540,7 @@
         <v>112</v>
       </c>
       <c r="B52" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C52" t="s">
         <v>30</v>
@@ -2561,7 +2552,7 @@
         <v>31</v>
       </c>
       <c r="G52" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -2569,7 +2560,7 @@
         <v>116</v>
       </c>
       <c r="B53" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C53" t="s">
         <v>113</v>
@@ -2586,7 +2577,7 @@
         <v>117</v>
       </c>
       <c r="B54" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C54" t="s">
         <v>13</v>
@@ -2598,7 +2589,7 @@
         <v>14</v>
       </c>
       <c r="G54" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -2606,7 +2597,7 @@
         <v>117</v>
       </c>
       <c r="B55" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C55" t="s">
         <v>61</v>
@@ -2615,10 +2606,10 @@
         <v>4</v>
       </c>
       <c r="E55" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="G55" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -2640,7 +2631,7 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B57" t="s">
         <v>23</v>
@@ -2674,44 +2665,44 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>124</v>
+        <v>237</v>
       </c>
       <c r="B59" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C59" t="s">
-        <v>79</v>
+        <v>126</v>
       </c>
       <c r="D59" t="s">
-        <v>114</v>
+        <v>8</v>
       </c>
       <c r="E59" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B60" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C60" t="s">
-        <v>127</v>
+        <v>79</v>
       </c>
       <c r="D60" t="s">
-        <v>8</v>
+        <v>114</v>
       </c>
       <c r="E60" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
+        <v>128</v>
+      </c>
+      <c r="B61" t="s">
         <v>129</v>
-      </c>
-      <c r="B61" t="s">
-        <v>130</v>
       </c>
       <c r="C61" t="s">
         <v>61</v>
@@ -2720,66 +2711,66 @@
         <v>114</v>
       </c>
       <c r="E61" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B62" t="s">
+        <v>131</v>
+      </c>
+      <c r="C62" t="s">
         <v>132</v>
-      </c>
-      <c r="C62" t="s">
-        <v>133</v>
       </c>
       <c r="D62" t="s">
         <v>4</v>
       </c>
       <c r="E62" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
+        <v>134</v>
+      </c>
+      <c r="B63" t="s">
         <v>135</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
         <v>136</v>
-      </c>
-      <c r="C63" t="s">
-        <v>137</v>
       </c>
       <c r="D63" t="s">
         <v>114</v>
       </c>
       <c r="E63" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
+        <v>224</v>
+      </c>
+      <c r="B64" t="s">
         <v>225</v>
       </c>
-      <c r="B64" t="s">
-        <v>226</v>
-      </c>
       <c r="C64" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D64" t="s">
         <v>114</v>
       </c>
       <c r="E64" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B65" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C65" t="s">
         <v>56</v>
@@ -2788,49 +2779,49 @@
         <v>114</v>
       </c>
       <c r="E65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
+        <v>140</v>
+      </c>
+      <c r="B66" t="s">
+        <v>163</v>
+      </c>
+      <c r="C66" t="s">
         <v>141</v>
-      </c>
-      <c r="B66" t="s">
-        <v>164</v>
-      </c>
-      <c r="C66" t="s">
-        <v>142</v>
       </c>
       <c r="D66" t="s">
         <v>114</v>
       </c>
       <c r="E66" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
+        <v>143</v>
+      </c>
+      <c r="B67" t="s">
         <v>144</v>
       </c>
-      <c r="B67" t="s">
-        <v>145</v>
-      </c>
       <c r="C67" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D67" t="s">
         <v>114</v>
       </c>
       <c r="E67" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B68" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C68" t="s">
         <v>56</v>
@@ -2839,15 +2830,15 @@
         <v>114</v>
       </c>
       <c r="E68" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
+        <v>147</v>
+      </c>
+      <c r="B69" t="s">
         <v>148</v>
-      </c>
-      <c r="B69" t="s">
-        <v>149</v>
       </c>
       <c r="C69" t="s">
         <v>3</v>
@@ -2856,15 +2847,15 @@
         <v>114</v>
       </c>
       <c r="E69" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B70" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C70" t="s">
         <v>67</v>
@@ -2873,7 +2864,7 @@
         <v>114</v>
       </c>
       <c r="E70" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="13.5" customHeight="1"/>

</xml_diff>

<commit_message>
suppression details calendrier + ajout doc sante
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="525" yWindow="30" windowWidth="20055" windowHeight="7950"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Calendrier" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="237">
   <si>
     <t>Date</t>
   </si>
@@ -523,9 +523,6 @@
     <t>marcaires</t>
   </si>
   <si>
-    <t>Gentlemen de Nommay (épreuve FFC ouverte aux FSGT - à confirmer)</t>
-  </si>
-  <si>
     <t>Cyclo-cross de Fesches le Châtel (à confirmer)</t>
   </si>
   <si>
@@ -682,9 +679,6 @@
     <t>Annulée</t>
   </si>
   <si>
-    <t>Annulé (routes impraticables)</t>
-  </si>
-  <si>
     <t>Sam 6 Novembre</t>
   </si>
   <si>
@@ -694,9 +688,6 @@
     <t>guebwiller</t>
   </si>
   <si>
-    <t>Ouvert aux FFC</t>
-  </si>
-  <si>
     <t>La Super cUp VTT</t>
   </si>
   <si>
@@ -715,9 +706,6 @@
     <t>3&lt;sup&gt;e&lt;/sup&gt; VTT Peugeot</t>
   </si>
   <si>
-    <t>Annulé (nouvelles restrictions sanitaires depuis le 9 Août)</t>
-  </si>
-  <si>
     <t>Prix Gekobike à Heimsbrunn</t>
   </si>
   <si>
@@ -731,6 +719,12 @@
   </si>
   <si>
     <t>Championnat d'Alsace FSGT. Ouvert aux FFC</t>
+  </si>
+  <si>
+    <t>https://www.ffc-bfc.fr/calendrier-resultats/gentlemen-de-nommay-2</t>
+  </si>
+  <si>
+    <t>Gentlemen de Nommay (épreuve FFC ouverte aux FSGT)</t>
   </si>
 </sst>
 </file>
@@ -1567,8 +1561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1609,7 +1603,7 @@
         <v>165</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1621,7 +1615,7 @@
         <v>149</v>
       </c>
       <c r="G2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1641,7 +1635,7 @@
         <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1661,7 +1655,7 @@
         <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1681,7 +1675,7 @@
         <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1701,7 +1695,7 @@
         <v>28</v>
       </c>
       <c r="G6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1709,7 +1703,7 @@
         <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C7" t="s">
         <v>30</v>
@@ -1721,7 +1715,7 @@
         <v>31</v>
       </c>
       <c r="G7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1741,7 +1735,7 @@
         <v>166</v>
       </c>
       <c r="G8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1749,7 +1743,7 @@
         <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
@@ -1761,7 +1755,7 @@
         <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1784,7 +1778,7 @@
         <v>168</v>
       </c>
       <c r="G10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1792,7 +1786,7 @@
         <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C11" t="s">
         <v>40</v>
@@ -1801,18 +1795,18 @@
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C12" t="s">
         <v>56</v>
@@ -1821,10 +1815,10 @@
         <v>4</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1832,7 +1826,7 @@
         <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
@@ -1849,7 +1843,7 @@
         <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C14" t="s">
         <v>44</v>
@@ -1892,7 +1886,7 @@
         <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1917,7 +1911,7 @@
         <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C18" t="s">
         <v>56</v>
@@ -1929,7 +1923,7 @@
         <v>57</v>
       </c>
       <c r="G18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1966,7 +1960,7 @@
         <v>62</v>
       </c>
       <c r="G20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1986,7 +1980,7 @@
         <v>63</v>
       </c>
       <c r="G21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1994,7 +1988,7 @@
         <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C22" t="s">
         <v>61</v>
@@ -2003,10 +1997,10 @@
         <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -2014,7 +2008,7 @@
         <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C23" t="s">
         <v>61</v>
@@ -2023,18 +2017,18 @@
         <v>4</v>
       </c>
       <c r="E23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
@@ -2043,7 +2037,7 @@
         <v>64</v>
       </c>
       <c r="G24" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -2051,7 +2045,7 @@
         <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C25" t="s">
         <v>20</v>
@@ -2102,7 +2096,7 @@
         <v>65</v>
       </c>
       <c r="B28" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C28" t="s">
         <v>11</v>
@@ -2136,7 +2130,7 @@
         <v>72</v>
       </c>
       <c r="B30" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C30" t="s">
         <v>13</v>
@@ -2145,7 +2139,7 @@
         <v>4</v>
       </c>
       <c r="E30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -2153,7 +2147,7 @@
         <v>72</v>
       </c>
       <c r="B31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C31" t="s">
         <v>75</v>
@@ -2165,7 +2159,7 @@
         <v>77</v>
       </c>
       <c r="G31" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -2190,7 +2184,7 @@
         <v>78</v>
       </c>
       <c r="B33" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C33" t="s">
         <v>79</v>
@@ -2202,7 +2196,7 @@
         <v>80</v>
       </c>
       <c r="G33" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -2239,41 +2233,41 @@
         <v>83</v>
       </c>
       <c r="G35" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
+        <v>215</v>
+      </c>
+      <c r="B36" t="s">
         <v>216</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>217</v>
-      </c>
-      <c r="C36" t="s">
-        <v>218</v>
       </c>
       <c r="D36" t="s">
         <v>45</v>
       </c>
       <c r="E36" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
+        <v>178</v>
+      </c>
+      <c r="B37" t="s">
         <v>179</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>180</v>
-      </c>
-      <c r="C37" t="s">
-        <v>181</v>
       </c>
       <c r="D37" t="s">
         <v>8</v>
       </c>
       <c r="E37" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -2295,21 +2289,18 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
+        <v>187</v>
+      </c>
+      <c r="B39" t="s">
+        <v>212</v>
+      </c>
+      <c r="C39" t="s">
         <v>188</v>
-      </c>
-      <c r="B39" t="s">
-        <v>213</v>
-      </c>
-      <c r="C39" t="s">
-        <v>189</v>
       </c>
       <c r="D39" t="s">
         <v>8</v>
       </c>
       <c r="E39" t="s">
-        <v>229</v>
-      </c>
-      <c r="G39" t="s">
         <v>226</v>
       </c>
     </row>
@@ -2318,7 +2309,7 @@
         <v>88</v>
       </c>
       <c r="B40" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C40" t="s">
         <v>89</v>
@@ -2330,7 +2321,7 @@
         <v>90</v>
       </c>
       <c r="G40" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -2350,7 +2341,7 @@
         <v>93</v>
       </c>
       <c r="G41" t="s">
-        <v>222</v>
+        <v>176</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -2367,10 +2358,10 @@
         <v>4</v>
       </c>
       <c r="E42" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G42" t="s">
-        <v>233</v>
+        <v>176</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -2378,7 +2369,7 @@
         <v>94</v>
       </c>
       <c r="B43" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C43" t="s">
         <v>17</v>
@@ -2390,7 +2381,7 @@
         <v>95</v>
       </c>
       <c r="G43" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -2427,7 +2418,7 @@
         <v>99</v>
       </c>
       <c r="G45" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -2435,7 +2426,7 @@
         <v>97</v>
       </c>
       <c r="B46" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C46" t="s">
         <v>103</v>
@@ -2464,7 +2455,7 @@
         <v>102</v>
       </c>
       <c r="G47" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -2472,7 +2463,7 @@
         <v>100</v>
       </c>
       <c r="B48" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C48" t="s">
         <v>56</v>
@@ -2481,7 +2472,7 @@
         <v>45</v>
       </c>
       <c r="E48" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -2506,7 +2497,7 @@
         <v>108</v>
       </c>
       <c r="B50" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C50" t="s">
         <v>109</v>
@@ -2518,7 +2509,7 @@
         <v>110</v>
       </c>
       <c r="G50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -2526,7 +2517,7 @@
         <v>108</v>
       </c>
       <c r="B51" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C51" t="s">
         <v>27</v>
@@ -2538,7 +2529,7 @@
         <v>111</v>
       </c>
       <c r="G51" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -2546,7 +2537,7 @@
         <v>112</v>
       </c>
       <c r="B52" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C52" t="s">
         <v>30</v>
@@ -2558,7 +2549,7 @@
         <v>31</v>
       </c>
       <c r="G52" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -2566,7 +2557,7 @@
         <v>116</v>
       </c>
       <c r="B53" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C53" t="s">
         <v>113</v>
@@ -2583,7 +2574,7 @@
         <v>117</v>
       </c>
       <c r="B54" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C54" t="s">
         <v>13</v>
@@ -2595,7 +2586,7 @@
         <v>14</v>
       </c>
       <c r="G54" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -2603,7 +2594,7 @@
         <v>117</v>
       </c>
       <c r="B55" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C55" t="s">
         <v>61</v>
@@ -2612,10 +2603,10 @@
         <v>4</v>
       </c>
       <c r="E55" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G55" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -2637,7 +2628,7 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B57" t="s">
         <v>23</v>
@@ -2671,10 +2662,10 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B59" t="s">
-        <v>169</v>
+        <v>236</v>
       </c>
       <c r="C59" t="s">
         <v>126</v>
@@ -2684,6 +2675,9 @@
       </c>
       <c r="E59" t="s">
         <v>127</v>
+      </c>
+      <c r="F59" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2756,10 +2750,10 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B64" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C64" t="s">
         <v>136</v>
@@ -2768,7 +2762,7 @@
         <v>114</v>
       </c>
       <c r="E64" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -2776,7 +2770,7 @@
         <v>138</v>
       </c>
       <c r="B65" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C65" t="s">
         <v>56</v>
@@ -2827,7 +2821,7 @@
         <v>143</v>
       </c>
       <c r="B68" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C68" t="s">
         <v>56</v>
@@ -2861,7 +2855,7 @@
         <v>150</v>
       </c>
       <c r="B70" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C70" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
2e en 3e cx
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="525" yWindow="30" windowWidth="20055" windowHeight="7950"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Calendrier" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -481,9 +481,6 @@
     <t xml:space="preserve">12&lt;sup&gt;e&lt;/sup&gt; Cyclo-cross de l'Amitié et de la Solidarité à Morschwiller le bas  </t>
   </si>
   <si>
-    <t xml:space="preserve">2&lt;sup&gt;e&lt;/sup&gt; cyclo-cross du Gloeckelsberg  </t>
-  </si>
-  <si>
     <t>https://www.cyclosportive-lesmarcaires.fr/</t>
   </si>
   <si>
@@ -749,6 +746,9 @@
   </si>
   <si>
     <t>Cyclo-cross de Dambelin  Championnat Bourgogne Franche-Comté</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3&lt;sup&gt;e&lt;/sup&gt; cyclo-cross du Gloeckelsberg  </t>
   </si>
 </sst>
 </file>
@@ -1586,7 +1586,7 @@
   <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1624,10 +1624,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1639,7 +1639,7 @@
         <v>142</v>
       </c>
       <c r="G2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1659,7 +1659,7 @@
         <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1679,7 +1679,7 @@
         <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1699,7 +1699,7 @@
         <v>27</v>
       </c>
       <c r="G5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1707,7 +1707,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
@@ -1719,7 +1719,7 @@
         <v>30</v>
       </c>
       <c r="G6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1736,10 +1736,10 @@
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1747,7 +1747,7 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C8" t="s">
         <v>26</v>
@@ -1759,7 +1759,7 @@
         <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1776,13 +1776,13 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1790,7 +1790,7 @@
         <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C10" t="s">
         <v>39</v>
@@ -1799,18 +1799,18 @@
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C11" t="s">
         <v>55</v>
@@ -1819,10 +1819,10 @@
         <v>4</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1830,7 +1830,7 @@
         <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
@@ -1847,7 +1847,7 @@
         <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C13" t="s">
         <v>43</v>
@@ -1890,7 +1890,7 @@
         <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1915,7 +1915,7 @@
         <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C17" t="s">
         <v>55</v>
@@ -1927,7 +1927,7 @@
         <v>56</v>
       </c>
       <c r="G17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1964,7 +1964,7 @@
         <v>61</v>
       </c>
       <c r="G19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1984,7 +1984,7 @@
         <v>62</v>
       </c>
       <c r="G20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1992,7 +1992,7 @@
         <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C21" t="s">
         <v>60</v>
@@ -2001,10 +2001,10 @@
         <v>4</v>
       </c>
       <c r="E21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2012,7 +2012,7 @@
         <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C22" t="s">
         <v>60</v>
@@ -2021,18 +2021,18 @@
         <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D23" t="s">
         <v>8</v>
@@ -2041,7 +2041,7 @@
         <v>63</v>
       </c>
       <c r="G23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -2049,7 +2049,7 @@
         <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C24" t="s">
         <v>20</v>
@@ -2100,7 +2100,7 @@
         <v>64</v>
       </c>
       <c r="B27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C27" t="s">
         <v>11</v>
@@ -2134,7 +2134,7 @@
         <v>71</v>
       </c>
       <c r="B29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C29" t="s">
         <v>13</v>
@@ -2143,7 +2143,7 @@
         <v>4</v>
       </c>
       <c r="E29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -2151,7 +2151,7 @@
         <v>71</v>
       </c>
       <c r="B30" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C30" t="s">
         <v>74</v>
@@ -2163,7 +2163,7 @@
         <v>76</v>
       </c>
       <c r="G30" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -2188,7 +2188,7 @@
         <v>77</v>
       </c>
       <c r="B32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C32" t="s">
         <v>78</v>
@@ -2200,7 +2200,7 @@
         <v>79</v>
       </c>
       <c r="G32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -2237,41 +2237,41 @@
         <v>82</v>
       </c>
       <c r="G34" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
+        <v>201</v>
+      </c>
+      <c r="B35" t="s">
         <v>202</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>203</v>
-      </c>
-      <c r="C35" t="s">
-        <v>204</v>
       </c>
       <c r="D35" t="s">
         <v>44</v>
       </c>
       <c r="E35" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
+        <v>166</v>
+      </c>
+      <c r="B36" t="s">
         <v>167</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>168</v>
-      </c>
-      <c r="C36" t="s">
-        <v>169</v>
       </c>
       <c r="D36" t="s">
         <v>8</v>
       </c>
       <c r="E36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2293,22 +2293,22 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
+        <v>175</v>
+      </c>
+      <c r="B38" t="s">
+        <v>198</v>
+      </c>
+      <c r="C38" t="s">
         <v>176</v>
-      </c>
-      <c r="B38" t="s">
-        <v>199</v>
-      </c>
-      <c r="C38" t="s">
-        <v>177</v>
       </c>
       <c r="D38" t="s">
         <v>8</v>
       </c>
       <c r="E38" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G38" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -2316,7 +2316,7 @@
         <v>87</v>
       </c>
       <c r="B39" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C39" t="s">
         <v>88</v>
@@ -2328,7 +2328,7 @@
         <v>89</v>
       </c>
       <c r="G39" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -2348,7 +2348,7 @@
         <v>92</v>
       </c>
       <c r="G40" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -2365,10 +2365,10 @@
         <v>4</v>
       </c>
       <c r="E41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G41" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -2376,7 +2376,7 @@
         <v>93</v>
       </c>
       <c r="B42" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C42" t="s">
         <v>17</v>
@@ -2388,7 +2388,7 @@
         <v>94</v>
       </c>
       <c r="G42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -2425,7 +2425,7 @@
         <v>98</v>
       </c>
       <c r="G44" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -2433,7 +2433,7 @@
         <v>96</v>
       </c>
       <c r="B45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C45" t="s">
         <v>101</v>
@@ -2450,7 +2450,7 @@
         <v>99</v>
       </c>
       <c r="B46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C46" t="s">
         <v>43</v>
@@ -2467,7 +2467,7 @@
         <v>99</v>
       </c>
       <c r="B47" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C47" t="s">
         <v>55</v>
@@ -2476,7 +2476,7 @@
         <v>44</v>
       </c>
       <c r="E47" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -2501,7 +2501,7 @@
         <v>106</v>
       </c>
       <c r="B49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C49" t="s">
         <v>107</v>
@@ -2513,7 +2513,7 @@
         <v>108</v>
       </c>
       <c r="G49" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -2521,7 +2521,7 @@
         <v>106</v>
       </c>
       <c r="B50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C50" t="s">
         <v>26</v>
@@ -2533,7 +2533,7 @@
         <v>109</v>
       </c>
       <c r="G50" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -2541,7 +2541,7 @@
         <v>110</v>
       </c>
       <c r="B51" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C51" t="s">
         <v>29</v>
@@ -2553,7 +2553,7 @@
         <v>30</v>
       </c>
       <c r="G51" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -2561,7 +2561,7 @@
         <v>114</v>
       </c>
       <c r="B52" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C52" t="s">
         <v>111</v>
@@ -2578,7 +2578,7 @@
         <v>115</v>
       </c>
       <c r="B53" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C53" t="s">
         <v>13</v>
@@ -2590,7 +2590,7 @@
         <v>14</v>
       </c>
       <c r="G53" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -2598,7 +2598,7 @@
         <v>115</v>
       </c>
       <c r="B54" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C54" t="s">
         <v>60</v>
@@ -2607,10 +2607,10 @@
         <v>4</v>
       </c>
       <c r="E54" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G54" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -2632,7 +2632,7 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B56" t="s">
         <v>22</v>
@@ -2647,7 +2647,7 @@
         <v>23</v>
       </c>
       <c r="G56" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2669,10 +2669,10 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B58" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C58" t="s">
         <v>124</v>
@@ -2681,10 +2681,10 @@
         <v>8</v>
       </c>
       <c r="E58" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G58" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -2709,7 +2709,7 @@
         <v>122</v>
       </c>
       <c r="B60" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C60" t="s">
         <v>78</v>
@@ -2718,7 +2718,7 @@
         <v>4</v>
       </c>
       <c r="E60" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -2740,10 +2740,10 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B62" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C62" t="s">
         <v>128</v>
@@ -2752,7 +2752,7 @@
         <v>4</v>
       </c>
       <c r="E62" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2774,10 +2774,10 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B64" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C64" t="s">
         <v>131</v>
@@ -2786,24 +2786,24 @@
         <v>112</v>
       </c>
       <c r="E64" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B65" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C65" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D65" t="s">
         <v>112</v>
       </c>
       <c r="E65" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -2811,7 +2811,7 @@
         <v>133</v>
       </c>
       <c r="B66" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C66" t="s">
         <v>55</v>
@@ -2828,7 +2828,7 @@
         <v>137</v>
       </c>
       <c r="B67" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C67" t="s">
         <v>131</v>
@@ -2845,7 +2845,7 @@
         <v>137</v>
       </c>
       <c r="B68" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C68" t="s">
         <v>131</v>
@@ -2854,7 +2854,7 @@
         <v>44</v>
       </c>
       <c r="E68" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -2862,7 +2862,7 @@
         <v>137</v>
       </c>
       <c r="B69" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C69" t="s">
         <v>55</v>
@@ -2891,15 +2891,15 @@
         <v>142</v>
       </c>
       <c r="G70" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B71" t="s">
-        <v>155</v>
+        <v>244</v>
       </c>
       <c r="C71" t="s">
         <v>135</v>
@@ -2913,10 +2913,10 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B72" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C72" t="s">
         <v>66</v>
@@ -2928,15 +2928,15 @@
         <v>143</v>
       </c>
       <c r="G72" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="13.5" customHeight="1">
       <c r="A73" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B73" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C73" t="s">
         <v>11</v>
@@ -2945,15 +2945,15 @@
         <v>112</v>
       </c>
       <c r="E73" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B74" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C74" t="s">
         <v>29</v>
@@ -2962,10 +2962,10 @@
         <v>112</v>
       </c>
       <c r="E74" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F74" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1e version classement national
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caroline\Documents\68-FSGT-Cyclisme-Alsace\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4669372D-D1A8-4813-9E76-682A643C2AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendrier" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="197">
   <si>
     <t>Date</t>
   </si>
@@ -301,9 +307,6 @@
     <t>montreux</t>
   </si>
   <si>
-    <t>https://www.fsgt.org/activites/velo/epreuves/cyclo-cross-championnat-national-fsgt-des-22-et-23-janvier-2022</t>
-  </si>
-  <si>
     <t>Cyclo-cross de Fesches le Châtel</t>
   </si>
   <si>
@@ -547,9 +550,6 @@
     <t xml:space="preserve"> Championnat de Bourgogne Franche-Comté</t>
   </si>
   <si>
-    <t>nationaux_vtt</t>
-  </si>
-  <si>
     <t>Cyclo-cross de Wattwiller</t>
   </si>
   <si>
@@ -608,13 +608,16 @@
   </si>
   <si>
     <t>VTT ELS Immo</t>
+  </si>
+  <si>
+    <t>nationaux</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1135,12 +1138,12 @@
     <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Commentaire" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Lien hypertexte" xfId="42" builtinId="8"/>
     <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -1208,7 +1211,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1240,9 +1243,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1274,6 +1295,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1449,14 +1488,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="67.42578125" customWidth="1"/>
@@ -1466,7 +1505,7 @@
     <col min="7" max="7" width="51.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1489,12 +1528,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
         <v>97</v>
-      </c>
-      <c r="B2" t="s">
-        <v>98</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -1506,12 +1545,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -1520,18 +1559,15 @@
         <v>64</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -1543,9 +1579,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
@@ -1560,12 +1596,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -1577,12 +1613,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" t="s">
         <v>103</v>
-      </c>
-      <c r="B7" t="s">
-        <v>104</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
@@ -1594,26 +1630,26 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" t="s">
         <v>105</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>106</v>
-      </c>
-      <c r="C8" t="s">
-        <v>107</v>
       </c>
       <c r="D8" t="s">
         <v>29</v>
       </c>
       <c r="E8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>109</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
@@ -1628,12 +1664,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" t="s">
         <v>110</v>
-      </c>
-      <c r="B10" t="s">
-        <v>111</v>
       </c>
       <c r="C10" t="s">
         <v>26</v>
@@ -1645,12 +1681,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" t="s">
         <v>180</v>
-      </c>
-      <c r="B11" t="s">
-        <v>182</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
@@ -1662,9 +1698,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -1676,15 +1712,15 @@
         <v>3</v>
       </c>
       <c r="E12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>113</v>
-      </c>
-      <c r="B13" t="s">
-        <v>114</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
@@ -1696,9 +1732,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B14" t="s">
         <v>24</v>
@@ -1713,12 +1749,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C15" t="s">
         <v>23</v>
@@ -1727,15 +1763,15 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>117</v>
-      </c>
       <c r="B16" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -1747,12 +1783,12 @@
         <v>40</v>
       </c>
       <c r="G16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B17" t="s">
         <v>88</v>
@@ -1764,15 +1800,15 @@
         <v>29</v>
       </c>
       <c r="E17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
-        <v>118</v>
-      </c>
-      <c r="B18" t="s">
-        <v>120</v>
       </c>
       <c r="C18" t="s">
         <v>20</v>
@@ -1781,12 +1817,12 @@
         <v>29</v>
       </c>
       <c r="E18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B19" t="s">
         <v>30</v>
@@ -1801,9 +1837,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B20" t="s">
         <v>89</v>
@@ -1818,15 +1854,15 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" t="s">
+        <v>174</v>
+      </c>
+      <c r="C21" t="s">
         <v>122</v>
-      </c>
-      <c r="B21" t="s">
-        <v>175</v>
-      </c>
-      <c r="C21" t="s">
-        <v>123</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
@@ -1835,29 +1871,29 @@
         <v>36</v>
       </c>
       <c r="G21" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D22" t="s">
         <v>6</v>
       </c>
       <c r="E22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
         <v>126</v>
-      </c>
-      <c r="B23" t="s">
-        <v>127</v>
       </c>
       <c r="C23" t="s">
         <v>33</v>
@@ -1869,9 +1905,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B24" t="s">
         <v>39</v>
@@ -1883,15 +1919,15 @@
         <v>29</v>
       </c>
       <c r="E24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
         <v>129</v>
-      </c>
-      <c r="B25" t="s">
-        <v>130</v>
       </c>
       <c r="C25" t="s">
         <v>10</v>
@@ -1903,9 +1939,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B26" t="s">
         <v>90</v>
@@ -1920,12 +1956,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>131</v>
+      </c>
+      <c r="B27" t="s">
         <v>132</v>
-      </c>
-      <c r="B27" t="s">
-        <v>133</v>
       </c>
       <c r="C27" t="s">
         <v>28</v>
@@ -1937,12 +1973,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C28" t="s">
         <v>85</v>
@@ -1951,12 +1987,12 @@
         <v>6</v>
       </c>
       <c r="E28" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" t="s">
-        <v>136</v>
       </c>
       <c r="B29" t="s">
         <v>47</v>
@@ -1971,29 +2007,29 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>191</v>
+      </c>
+      <c r="B30" t="s">
+        <v>192</v>
+      </c>
+      <c r="C30" t="s">
         <v>193</v>
-      </c>
-      <c r="B30" t="s">
-        <v>194</v>
-      </c>
-      <c r="C30" t="s">
-        <v>195</v>
       </c>
       <c r="D30" t="s">
         <v>6</v>
       </c>
       <c r="E30" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>136</v>
+      </c>
+      <c r="B31" t="s">
         <v>137</v>
-      </c>
-      <c r="B31" t="s">
-        <v>138</v>
       </c>
       <c r="C31" t="s">
         <v>25</v>
@@ -2005,12 +2041,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B32" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C32" t="s">
         <v>50</v>
@@ -2022,12 +2058,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>139</v>
+      </c>
+      <c r="B33" t="s">
         <v>140</v>
-      </c>
-      <c r="B33" t="s">
-        <v>141</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
@@ -2036,15 +2072,15 @@
         <v>6</v>
       </c>
       <c r="E33" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>53</v>
       </c>
       <c r="B34" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C34" t="s">
         <v>12</v>
@@ -2056,9 +2092,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B35" t="s">
         <v>55</v>
@@ -2073,12 +2109,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B36" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C36" t="s">
         <v>57</v>
@@ -2090,12 +2126,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B37" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C37" t="s">
         <v>59</v>
@@ -2107,9 +2143,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B38" t="s">
         <v>86</v>
@@ -2121,15 +2157,15 @@
         <v>3</v>
       </c>
       <c r="E38" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B39" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C39" t="s">
         <v>10</v>
@@ -2141,12 +2177,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>147</v>
+      </c>
+      <c r="B40" t="s">
         <v>148</v>
-      </c>
-      <c r="B40" t="s">
-        <v>149</v>
       </c>
       <c r="C40" t="s">
         <v>18</v>
@@ -2158,9 +2194,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B41" t="s">
         <v>32</v>
@@ -2175,12 +2211,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B42" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C42" t="s">
         <v>63</v>
@@ -2192,12 +2228,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B43" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C43" t="s">
         <v>2</v>
@@ -2206,12 +2242,12 @@
         <v>3</v>
       </c>
       <c r="E43" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" t="s">
-        <v>153</v>
       </c>
       <c r="B44" t="s">
         <v>66</v>
@@ -2226,12 +2262,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B45" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C45" t="s">
         <v>45</v>
@@ -2243,15 +2279,15 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>154</v>
+      </c>
+      <c r="B46" t="s">
+        <v>187</v>
+      </c>
+      <c r="C46" t="s">
         <v>155</v>
-      </c>
-      <c r="B46" t="s">
-        <v>189</v>
-      </c>
-      <c r="C46" t="s">
-        <v>156</v>
       </c>
       <c r="D46" t="s">
         <v>64</v>
@@ -2260,9 +2296,9 @@
         <v>93</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B47" t="s">
         <v>92</v>
@@ -2274,12 +2310,12 @@
         <v>6</v>
       </c>
       <c r="E47" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" t="s">
-        <v>158</v>
       </c>
       <c r="B48" t="s">
         <v>71</v>
@@ -2291,12 +2327,12 @@
         <v>64</v>
       </c>
       <c r="E48" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" t="s">
-        <v>160</v>
       </c>
       <c r="B49" t="s">
         <v>68</v>
@@ -2308,15 +2344,15 @@
         <v>64</v>
       </c>
       <c r="E49" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" t="s">
-        <v>162</v>
-      </c>
       <c r="B50" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C50" t="s">
         <v>35</v>
@@ -2328,12 +2364,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>162</v>
+      </c>
+      <c r="B51" t="s">
         <v>163</v>
-      </c>
-      <c r="B51" t="s">
-        <v>164</v>
       </c>
       <c r="C51" t="s">
         <v>35</v>
@@ -2345,12 +2381,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B52" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C52" t="s">
         <v>75</v>
@@ -2359,15 +2395,15 @@
         <v>64</v>
       </c>
       <c r="E52" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="53" spans="1:7">
-      <c r="A53" t="s">
+      <c r="B53" t="s">
         <v>167</v>
-      </c>
-      <c r="B53" t="s">
-        <v>168</v>
       </c>
       <c r="C53" t="s">
         <v>72</v>
@@ -2379,9 +2415,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B54" t="s">
         <v>77</v>
@@ -2396,12 +2432,12 @@
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B55" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C55" t="s">
         <v>72</v>
@@ -2413,14 +2449,14 @@
         <v>73</v>
       </c>
       <c r="G55" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="73" ht="13.5" customHeight="1"/>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="73" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
-    <hyperlink ref="E14" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId1" display="https://www.fsgt.org/activites/velo/epreuves/cyclo-cross-championnat-national-fsgt-des-22-et-23-janvier-2022" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId3"/>

</xml_diff>

<commit_message>
publis nationaux + membre + rector en larger
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caroline\Documents\68-FSGT-Cyclisme-Alsace\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6349E90-B7B9-40DE-84CF-F854B5BDFDE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendrier" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="199">
   <si>
     <t>Date</t>
   </si>
@@ -373,9 +379,6 @@
     <t>2 et 3 Juillet</t>
   </si>
   <si>
-    <t>nationaux_rte</t>
-  </si>
-  <si>
     <t>Dim 3 Juillet</t>
   </si>
   <si>
@@ -599,13 +602,28 @@
   </si>
   <si>
     <t>Jeu 12 Mai</t>
+  </si>
+  <si>
+    <t>9 et 10 Juillet</t>
+  </si>
+  <si>
+    <t>Championnat National à Le Mesnil-Réaume (Seine-Maritime)</t>
+  </si>
+  <si>
+    <t>Accro Bike 76</t>
+  </si>
+  <si>
+    <t>https://www.championnats-nationaux.fr/uploads/179/Plaquette%20du%20National%20VTT%202022%20avec%20reglements.pdf</t>
+  </si>
+  <si>
+    <t>https://www.championnats-nationaux.fr/uploads/177/Plaquette%20du%20National%20route%202022%20avec%20les%20reglements.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1126,12 +1144,12 @@
     <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Commentaire" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Lien hypertexte" xfId="42" builtinId="8"/>
     <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -1199,7 +1217,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1231,9 +1249,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1265,6 +1301,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1440,14 +1494,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="67.42578125" customWidth="1"/>
@@ -1457,7 +1511,7 @@
     <col min="7" max="7" width="51.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1480,7 +1534,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>94</v>
       </c>
@@ -1488,7 +1542,7 @@
         <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D2" t="s">
         <v>62</v>
@@ -1497,9 +1551,9 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B3" t="s">
         <v>96</v>
@@ -1511,15 +1565,15 @@
         <v>62</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>97</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -1531,10 +1585,10 @@
         <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>98</v>
       </c>
@@ -1542,7 +1596,7 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
@@ -1551,12 +1605,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -1568,10 +1622,10 @@
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>100</v>
       </c>
@@ -1588,10 +1642,10 @@
         <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>102</v>
       </c>
@@ -1608,9 +1662,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
@@ -1625,7 +1679,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>106</v>
       </c>
@@ -1642,15 +1696,15 @@
         <v>85</v>
       </c>
       <c r="G10" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -1662,15 +1716,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D12" t="s">
         <v>3</v>
@@ -1679,10 +1733,10 @@
         <v>108</v>
       </c>
       <c r="G12" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>109</v>
       </c>
@@ -1699,7 +1753,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>111</v>
       </c>
@@ -1716,12 +1770,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
@@ -1733,18 +1787,18 @@
         <v>112</v>
       </c>
       <c r="G15" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>113</v>
       </c>
       <c r="B16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
@@ -1753,10 +1807,10 @@
         <v>38</v>
       </c>
       <c r="G16" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>114</v>
       </c>
@@ -1773,7 +1827,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>114</v>
       </c>
@@ -1790,7 +1844,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>116</v>
       </c>
@@ -1807,12 +1861,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>116</v>
       </c>
       <c r="B20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C20" t="s">
         <v>117</v>
@@ -1824,29 +1878,29 @@
         <v>35</v>
       </c>
       <c r="G20" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>118</v>
       </c>
       <c r="B21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
       </c>
       <c r="E21" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>120</v>
-      </c>
-      <c r="B22" t="s">
-        <v>121</v>
       </c>
       <c r="C22" t="s">
         <v>32</v>
@@ -1858,15 +1912,15 @@
         <v>36</v>
       </c>
       <c r="G22" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" t="s">
         <v>122</v>
-      </c>
-      <c r="B23" t="s">
-        <v>123</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
@@ -1878,478 +1932,478 @@
         <v>39</v>
       </c>
       <c r="G23" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>124</v>
+        <v>194</v>
       </c>
       <c r="B24" t="s">
+        <v>195</v>
+      </c>
+      <c r="C24" t="s">
+        <v>196</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" t="s">
         <v>88</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>40</v>
-      </c>
-      <c r="D24" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>125</v>
-      </c>
-      <c r="B25" t="s">
-        <v>126</v>
-      </c>
-      <c r="C25" t="s">
-        <v>27</v>
       </c>
       <c r="D25" t="s">
         <v>41</v>
       </c>
       <c r="E25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="s">
-        <v>171</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>170</v>
+      </c>
+      <c r="B27" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" t="s">
         <v>127</v>
       </c>
-      <c r="C26" t="s">
-        <v>83</v>
-      </c>
-      <c r="D26" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" t="s">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" t="s">
-        <v>129</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>45</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>46</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>41</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E28" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
-      <c r="A28" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>182</v>
+      </c>
+      <c r="B29" t="s">
         <v>183</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C29" t="s">
         <v>184</v>
-      </c>
-      <c r="C28" t="s">
-        <v>185</v>
-      </c>
-      <c r="D28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" t="s">
-        <v>186</v>
-      </c>
-      <c r="G28" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" t="s">
-        <v>130</v>
-      </c>
-      <c r="B29" t="s">
-        <v>131</v>
-      </c>
-      <c r="C29" t="s">
-        <v>24</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>
       </c>
       <c r="E29" t="s">
+        <v>185</v>
+      </c>
+      <c r="G29" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" t="s">
+        <v>130</v>
+      </c>
+      <c r="C30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" t="s">
         <v>50</v>
       </c>
-      <c r="G29" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" t="s">
+      <c r="G30" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" t="s">
+        <v>174</v>
+      </c>
+      <c r="C31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>132</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
+        <v>133</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" t="s">
         <v>175</v>
       </c>
-      <c r="C30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D30" t="s">
-        <v>41</v>
-      </c>
-      <c r="E30" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" t="s">
-        <v>133</v>
-      </c>
-      <c r="B31" t="s">
-        <v>134</v>
-      </c>
-      <c r="C31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" t="s">
-        <v>51</v>
-      </c>
-      <c r="B32" t="s">
-        <v>176</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>11</v>
-      </c>
-      <c r="D32" t="s">
-        <v>3</v>
-      </c>
-      <c r="E32" t="s">
-        <v>52</v>
-      </c>
-      <c r="G32" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" t="s">
-        <v>136</v>
-      </c>
-      <c r="B33" t="s">
-        <v>53</v>
-      </c>
-      <c r="C33" t="s">
-        <v>48</v>
       </c>
       <c r="D33" t="s">
         <v>3</v>
       </c>
       <c r="E33" t="s">
+        <v>52</v>
+      </c>
+      <c r="G33" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" t="s">
         <v>54</v>
       </c>
-      <c r="G33" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" t="s">
+      <c r="G34" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" t="s">
+        <v>180</v>
+      </c>
+      <c r="C35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>136</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B36" t="s">
         <v>181</v>
       </c>
-      <c r="C34" t="s">
-        <v>55</v>
-      </c>
-      <c r="D34" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" t="s">
+      <c r="C36" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>137</v>
       </c>
-      <c r="B35" t="s">
-        <v>182</v>
-      </c>
-      <c r="C35" t="s">
-        <v>57</v>
-      </c>
-      <c r="D35" t="s">
-        <v>41</v>
-      </c>
-      <c r="E35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" t="s">
+      <c r="B37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" t="s">
         <v>138</v>
       </c>
-      <c r="B36" t="s">
-        <v>84</v>
-      </c>
-      <c r="C36" t="s">
-        <v>59</v>
-      </c>
-      <c r="D36" t="s">
-        <v>3</v>
-      </c>
-      <c r="E36" t="s">
-        <v>139</v>
-      </c>
-      <c r="G36" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" t="s">
-        <v>138</v>
-      </c>
-      <c r="B37" t="s">
-        <v>177</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="G37" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>137</v>
+      </c>
+      <c r="B38" t="s">
+        <v>176</v>
+      </c>
+      <c r="C38" t="s">
         <v>9</v>
-      </c>
-      <c r="D37" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" t="s">
-        <v>140</v>
-      </c>
-      <c r="B38" t="s">
-        <v>141</v>
-      </c>
-      <c r="C38" t="s">
-        <v>17</v>
       </c>
       <c r="D38" t="s">
         <v>6</v>
       </c>
       <c r="E38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>139</v>
+      </c>
+      <c r="B39" t="s">
+        <v>140</v>
+      </c>
+      <c r="C39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
-      <c r="A39" t="s">
-        <v>140</v>
-      </c>
-      <c r="B39" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>139</v>
+      </c>
+      <c r="B40" t="s">
         <v>31</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
+        <v>188</v>
+      </c>
+      <c r="D40" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>139</v>
+      </c>
+      <c r="B41" t="s">
+        <v>141</v>
+      </c>
+      <c r="C41" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>142</v>
+      </c>
+      <c r="B42" t="s">
+        <v>177</v>
+      </c>
+      <c r="C42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" t="s">
+        <v>143</v>
+      </c>
+      <c r="G42" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>144</v>
+      </c>
+      <c r="B43" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>41</v>
+      </c>
+      <c r="E43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>189</v>
       </c>
-      <c r="D39" t="s">
-        <v>3</v>
-      </c>
-      <c r="E39" t="s">
-        <v>8</v>
-      </c>
-      <c r="G39" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" t="s">
-        <v>140</v>
-      </c>
-      <c r="B40" t="s">
-        <v>142</v>
-      </c>
-      <c r="C40" t="s">
-        <v>61</v>
-      </c>
-      <c r="D40" t="s">
-        <v>62</v>
-      </c>
-      <c r="E40" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" t="s">
-        <v>143</v>
-      </c>
-      <c r="B41" t="s">
-        <v>178</v>
-      </c>
-      <c r="C41" t="s">
-        <v>2</v>
-      </c>
-      <c r="D41" t="s">
-        <v>3</v>
-      </c>
-      <c r="E41" t="s">
-        <v>144</v>
-      </c>
-      <c r="G41" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" t="s">
-        <v>145</v>
-      </c>
-      <c r="B42" t="s">
-        <v>64</v>
-      </c>
-      <c r="C42" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" t="s">
-        <v>41</v>
-      </c>
-      <c r="E42" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" t="s">
-        <v>190</v>
-      </c>
-      <c r="B43" t="s">
-        <v>180</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="B44" t="s">
+        <v>179</v>
+      </c>
+      <c r="C44" t="s">
         <v>73</v>
-      </c>
-      <c r="D43" t="s">
-        <v>62</v>
-      </c>
-      <c r="E43" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" t="s">
-        <v>146</v>
-      </c>
-      <c r="B44" t="s">
-        <v>169</v>
-      </c>
-      <c r="C44" t="s">
-        <v>43</v>
       </c>
       <c r="D44" t="s">
         <v>62</v>
       </c>
       <c r="E44" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B45" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C45" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="D45" t="s">
         <v>62</v>
       </c>
       <c r="E45" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>146</v>
+      </c>
+      <c r="B46" t="s">
+        <v>178</v>
+      </c>
+      <c r="C46" t="s">
+        <v>147</v>
+      </c>
+      <c r="D46" t="s">
+        <v>62</v>
+      </c>
+      <c r="E46" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
-      <c r="A46" t="s">
-        <v>147</v>
-      </c>
-      <c r="B46" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>146</v>
+      </c>
+      <c r="B47" t="s">
         <v>90</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>68</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>6</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E47" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" t="s">
-        <v>150</v>
-      </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>69</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>37</v>
-      </c>
-      <c r="D47" t="s">
-        <v>62</v>
-      </c>
-      <c r="E47" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" t="s">
-        <v>152</v>
-      </c>
-      <c r="B48" t="s">
-        <v>66</v>
-      </c>
-      <c r="C48" t="s">
-        <v>19</v>
       </c>
       <c r="D48" t="s">
         <v>62</v>
       </c>
       <c r="E48" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B49" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="C49" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D49" t="s">
         <v>62</v>
       </c>
       <c r="E49" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B50" t="s">
-        <v>156</v>
+        <v>93</v>
       </c>
       <c r="C50" t="s">
         <v>34</v>
@@ -2358,68 +2412,85 @@
         <v>62</v>
       </c>
       <c r="E50" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B51" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C51" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="D51" t="s">
         <v>62</v>
       </c>
       <c r="E51" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B52" t="s">
-        <v>75</v>
+        <v>158</v>
       </c>
       <c r="C52" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="D52" t="s">
         <v>62</v>
       </c>
       <c r="E52" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B53" t="s">
-        <v>168</v>
+        <v>75</v>
       </c>
       <c r="C53" t="s">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="D53" t="s">
         <v>62</v>
       </c>
       <c r="E53" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>160</v>
+      </c>
+      <c r="B54" t="s">
+        <v>167</v>
+      </c>
+      <c r="C54" t="s">
+        <v>70</v>
+      </c>
+      <c r="D54" t="s">
+        <v>62</v>
+      </c>
+      <c r="E54" t="s">
         <v>71</v>
       </c>
-      <c r="G53" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="71" ht="13.5" customHeight="1"/>
+      <c r="G54" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="72" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="https://www.fsgt.org/activites/velo/epreuves/cyclo-cross-championnat-national-fsgt-des-22-et-23-janvier-2022"/>
-    <hyperlink ref="E14" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId1" display="https://www.fsgt.org/activites/velo/epreuves/cyclo-cross-championnat-national-fsgt-des-22-et-23-janvier-2022" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId3"/>

</xml_diff>

<commit_message>
US to BC Giro
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caroline\Documents\68-FSGT-Cyclisme-Alsace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6349E90-B7B9-40DE-84CF-F854B5BDFDE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBB0E34-FA4A-4BF6-8488-903CDECB8B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -463,9 +463,6 @@
     <t>Dim 16 Octobre</t>
   </si>
   <si>
-    <t>US Giromagny VTT</t>
-  </si>
-  <si>
     <t>nommay</t>
   </si>
   <si>
@@ -617,6 +614,9 @@
   </si>
   <si>
     <t>https://www.championnats-nationaux.fr/uploads/177/Plaquette%20du%20National%20route%202022%20avec%20les%20reglements.pdf</t>
+  </si>
+  <si>
+    <t>Bike Club Giromagny</t>
   </si>
 </sst>
 </file>
@@ -1497,8 +1497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1542,7 +1542,7 @@
         <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D2" t="s">
         <v>62</v>
@@ -1553,7 +1553,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B3" t="s">
         <v>96</v>
@@ -1565,7 +1565,7 @@
         <v>62</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1573,7 +1573,7 @@
         <v>97</v>
       </c>
       <c r="B4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -1585,7 +1585,7 @@
         <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1596,7 +1596,7 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
@@ -1610,7 +1610,7 @@
         <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -1622,7 +1622,7 @@
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1642,7 +1642,7 @@
         <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1664,7 +1664,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
@@ -1696,15 +1696,15 @@
         <v>85</v>
       </c>
       <c r="G10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -1718,13 +1718,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D12" t="s">
         <v>3</v>
@@ -1733,7 +1733,7 @@
         <v>108</v>
       </c>
       <c r="G12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1772,10 +1772,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
@@ -1787,7 +1787,7 @@
         <v>112</v>
       </c>
       <c r="G15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1795,10 +1795,10 @@
         <v>113</v>
       </c>
       <c r="B16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
@@ -1807,7 +1807,7 @@
         <v>38</v>
       </c>
       <c r="G16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1866,7 +1866,7 @@
         <v>116</v>
       </c>
       <c r="B20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C20" t="s">
         <v>117</v>
@@ -1878,7 +1878,7 @@
         <v>35</v>
       </c>
       <c r="G20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1886,13 +1886,13 @@
         <v>118</v>
       </c>
       <c r="B21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1912,7 +1912,7 @@
         <v>36</v>
       </c>
       <c r="G22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1932,24 +1932,24 @@
         <v>39</v>
       </c>
       <c r="G23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>193</v>
+      </c>
+      <c r="B24" t="s">
         <v>194</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>195</v>
-      </c>
-      <c r="C24" t="s">
-        <v>196</v>
       </c>
       <c r="D24" t="s">
         <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1988,7 +1988,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B27" t="s">
         <v>126</v>
@@ -2022,22 +2022,22 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>181</v>
+      </c>
+      <c r="B29" t="s">
         <v>182</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>183</v>
-      </c>
-      <c r="C29" t="s">
-        <v>184</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2057,7 +2057,7 @@
         <v>50</v>
       </c>
       <c r="G30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2065,7 +2065,7 @@
         <v>131</v>
       </c>
       <c r="B31" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C31" t="s">
         <v>48</v>
@@ -2099,7 +2099,7 @@
         <v>51</v>
       </c>
       <c r="B33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
@@ -2111,7 +2111,7 @@
         <v>52</v>
       </c>
       <c r="G33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2131,7 +2131,7 @@
         <v>54</v>
       </c>
       <c r="G34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -2139,7 +2139,7 @@
         <v>135</v>
       </c>
       <c r="B35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C35" t="s">
         <v>55</v>
@@ -2156,7 +2156,7 @@
         <v>136</v>
       </c>
       <c r="B36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C36" t="s">
         <v>57</v>
@@ -2185,7 +2185,7 @@
         <v>138</v>
       </c>
       <c r="G37" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2193,7 +2193,7 @@
         <v>137</v>
       </c>
       <c r="B38" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C38" t="s">
         <v>9</v>
@@ -2230,7 +2230,7 @@
         <v>31</v>
       </c>
       <c r="C40" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D40" t="s">
         <v>3</v>
@@ -2239,7 +2239,7 @@
         <v>8</v>
       </c>
       <c r="G40" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2264,7 +2264,7 @@
         <v>142</v>
       </c>
       <c r="B42" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
@@ -2276,7 +2276,7 @@
         <v>143</v>
       </c>
       <c r="G42" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2298,10 +2298,10 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B44" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C44" t="s">
         <v>73</v>
@@ -2310,7 +2310,7 @@
         <v>62</v>
       </c>
       <c r="E44" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -2318,7 +2318,7 @@
         <v>145</v>
       </c>
       <c r="B45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C45" t="s">
         <v>43</v>
@@ -2335,10 +2335,10 @@
         <v>146</v>
       </c>
       <c r="B46" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C46" t="s">
-        <v>147</v>
+        <v>198</v>
       </c>
       <c r="D46" t="s">
         <v>62</v>
@@ -2361,12 +2361,12 @@
         <v>6</v>
       </c>
       <c r="E47" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B48" t="s">
         <v>69</v>
@@ -2378,12 +2378,12 @@
         <v>62</v>
       </c>
       <c r="E48" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B49" t="s">
         <v>66</v>
@@ -2395,12 +2395,12 @@
         <v>62</v>
       </c>
       <c r="E49" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B50" t="s">
         <v>93</v>
@@ -2417,10 +2417,10 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>153</v>
+      </c>
+      <c r="B51" t="s">
         <v>154</v>
-      </c>
-      <c r="B51" t="s">
-        <v>155</v>
       </c>
       <c r="C51" t="s">
         <v>34</v>
@@ -2434,10 +2434,10 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>156</v>
+      </c>
+      <c r="B52" t="s">
         <v>157</v>
-      </c>
-      <c r="B52" t="s">
-        <v>158</v>
       </c>
       <c r="C52" t="s">
         <v>70</v>
@@ -2451,7 +2451,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B53" t="s">
         <v>75</v>
@@ -2468,10 +2468,10 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B54" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C54" t="s">
         <v>70</v>
@@ -2483,7 +2483,7 @@
         <v>71</v>
       </c>
       <c r="G54" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="72" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
record heure et rando beaucourt
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caroline\Documents\68-FSGT-Cyclisme-Alsace\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521FBFC7-BA4B-4531-9F08-5BECF287BA95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendrier" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="216">
   <si>
     <t>Date</t>
   </si>
@@ -340,9 +346,6 @@
     <t>rando_vcscp</t>
   </si>
   <si>
-    <t>Dim 26 Juin</t>
-  </si>
-  <si>
     <t>2 et 3 Juillet</t>
   </si>
   <si>
@@ -656,13 +659,22 @@
   </si>
   <si>
     <t>Sam 17 Septembre</t>
+  </si>
+  <si>
+    <t>Tentative de record de l'heure de David Arnoux (Granges)</t>
+  </si>
+  <si>
+    <t>record_heure</t>
+  </si>
+  <si>
+    <t>Ven 24 Juin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1183,12 +1195,12 @@
     <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Commentaire" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Lien hypertexte" xfId="42" builtinId="8"/>
     <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -1256,7 +1268,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1288,9 +1300,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1322,6 +1352,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1497,14 +1545,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="67.42578125" customWidth="1"/>
@@ -1514,7 +1562,7 @@
     <col min="7" max="7" width="51.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1537,7 +1585,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>90</v>
       </c>
@@ -1545,7 +1593,7 @@
         <v>91</v>
       </c>
       <c r="C2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D2" t="s">
         <v>59</v>
@@ -1554,9 +1602,9 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s">
         <v>92</v>
@@ -1568,15 +1616,15 @@
         <v>59</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -1588,10 +1636,10 @@
         <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -1599,7 +1647,7 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
@@ -1608,12 +1656,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>95</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -1625,27 +1673,27 @@
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C7" t="s">
         <v>205</v>
-      </c>
-      <c r="B7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C7" t="s">
-        <v>206</v>
       </c>
       <c r="D7" t="s">
         <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>96</v>
       </c>
@@ -1662,12 +1710,12 @@
         <v>20</v>
       </c>
       <c r="G8" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
@@ -1682,7 +1730,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -1699,15 +1747,15 @@
         <v>82</v>
       </c>
       <c r="G10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -1719,15 +1767,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D12" t="s">
         <v>3</v>
@@ -1736,27 +1784,27 @@
         <v>100</v>
       </c>
       <c r="G12" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B13" t="s">
+        <v>193</v>
+      </c>
+      <c r="C13" t="s">
         <v>194</v>
-      </c>
-      <c r="C13" t="s">
-        <v>195</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>101</v>
       </c>
@@ -1773,12 +1821,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>101</v>
       </c>
       <c r="B15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C15" t="s">
         <v>36</v>
@@ -1787,13 +1835,13 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G15" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>103</v>
       </c>
@@ -1810,12 +1858,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C17" t="s">
         <v>22</v>
@@ -1827,15 +1875,15 @@
         <v>104</v>
       </c>
       <c r="G17" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C18" t="s">
         <v>34</v>
@@ -1844,18 +1892,18 @@
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>105</v>
       </c>
       <c r="B19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D19" t="s">
         <v>6</v>
@@ -1864,15 +1912,15 @@
         <v>37</v>
       </c>
       <c r="G19" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>106</v>
       </c>
       <c r="B20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C20" t="s">
         <v>27</v>
@@ -1884,7 +1932,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>106</v>
       </c>
@@ -1901,29 +1949,29 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>108</v>
+        <v>215</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>213</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>164</v>
       </c>
       <c r="D22" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C23" t="s">
         <v>32</v>
@@ -1932,15 +1980,15 @@
         <v>28</v>
       </c>
       <c r="E23" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C24" t="s">
         <v>32</v>
@@ -1949,32 +1997,32 @@
         <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G24" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D25" t="s">
         <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" t="s">
         <v>110</v>
-      </c>
-      <c r="B26" t="s">
-        <v>111</v>
       </c>
       <c r="C26" t="s">
         <v>32</v>
@@ -1986,15 +2034,15 @@
         <v>35</v>
       </c>
       <c r="G26" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C27" t="s">
         <v>32</v>
@@ -2003,35 +2051,32 @@
         <v>28</v>
       </c>
       <c r="E27" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B28" t="s">
-        <v>200</v>
+        <v>83</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="E28" t="s">
-        <v>38</v>
-      </c>
-      <c r="G28" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B29" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
@@ -2040,330 +2085,345 @@
         <v>3</v>
       </c>
       <c r="E29" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" t="s">
         <v>202</v>
       </c>
-      <c r="G29" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>175</v>
+        <v>111</v>
       </c>
       <c r="B30" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="C30" t="s">
-        <v>177</v>
+        <v>9</v>
       </c>
       <c r="D30" t="s">
         <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>201</v>
+      </c>
+      <c r="G30" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>174</v>
       </c>
       <c r="B31" t="s">
+        <v>175</v>
+      </c>
+      <c r="C31" t="s">
+        <v>176</v>
+      </c>
+      <c r="D31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32" t="s">
         <v>84</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>39</v>
-      </c>
-      <c r="D31" t="s">
-        <v>40</v>
-      </c>
-      <c r="E31" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" t="s">
-        <v>114</v>
-      </c>
-      <c r="B32" t="s">
-        <v>115</v>
-      </c>
-      <c r="C32" t="s">
-        <v>27</v>
       </c>
       <c r="D32" t="s">
         <v>40</v>
       </c>
       <c r="E32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" t="s">
+        <v>114</v>
+      </c>
+      <c r="C33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
-      <c r="A33" t="s">
-        <v>154</v>
-      </c>
-      <c r="B33" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>153</v>
+      </c>
+      <c r="B34" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
         <v>116</v>
       </c>
-      <c r="C33" t="s">
-        <v>80</v>
-      </c>
-      <c r="D33" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" t="s">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" t="s">
-        <v>118</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>44</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>45</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>40</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
-      <c r="A35" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>162</v>
+      </c>
+      <c r="B36" t="s">
         <v>163</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C36" t="s">
         <v>164</v>
-      </c>
-      <c r="C35" t="s">
-        <v>165</v>
-      </c>
-      <c r="D35" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" t="s">
-        <v>166</v>
-      </c>
-      <c r="G35" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" t="s">
-        <v>119</v>
-      </c>
-      <c r="B36" t="s">
-        <v>120</v>
-      </c>
-      <c r="C36" t="s">
-        <v>24</v>
       </c>
       <c r="D36" t="s">
         <v>6</v>
       </c>
       <c r="E36" t="s">
+        <v>165</v>
+      </c>
+      <c r="G36" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" t="s">
         <v>49</v>
       </c>
-      <c r="G36" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" t="s">
+      <c r="G37" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>120</v>
+      </c>
+      <c r="B38" t="s">
+        <v>156</v>
+      </c>
+      <c r="C38" t="s">
+        <v>47</v>
+      </c>
+      <c r="D38" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" t="s">
+        <v>180</v>
+      </c>
+      <c r="C39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" t="s">
+        <v>50</v>
+      </c>
+      <c r="G39" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>121</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B40" t="s">
+        <v>122</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>124</v>
+      </c>
+      <c r="B41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" t="s">
+        <v>52</v>
+      </c>
+      <c r="G41" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>124</v>
+      </c>
+      <c r="B42" t="s">
+        <v>160</v>
+      </c>
+      <c r="C42" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>125</v>
+      </c>
+      <c r="B43" t="s">
+        <v>161</v>
+      </c>
+      <c r="C43" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>126</v>
+      </c>
+      <c r="B44" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" t="s">
+        <v>57</v>
+      </c>
+      <c r="D44" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" t="s">
+        <v>127</v>
+      </c>
+      <c r="G44" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>126</v>
+      </c>
+      <c r="B45" t="s">
         <v>157</v>
       </c>
-      <c r="C37" t="s">
-        <v>47</v>
-      </c>
-      <c r="D37" t="s">
-        <v>40</v>
-      </c>
-      <c r="E37" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A38" t="s">
-        <v>121</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="C45" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>212</v>
+      </c>
+      <c r="B46" t="s">
+        <v>129</v>
+      </c>
+      <c r="C46" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46" t="s">
+        <v>59</v>
+      </c>
+      <c r="E46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>128</v>
+      </c>
+      <c r="B47" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47" t="s">
+        <v>168</v>
+      </c>
+      <c r="D47" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47" t="s">
+        <v>8</v>
+      </c>
+      <c r="G47" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>181</v>
       </c>
-      <c r="C38" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" t="s">
-        <v>3</v>
-      </c>
-      <c r="E38" t="s">
-        <v>50</v>
-      </c>
-      <c r="G38" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" t="s">
-        <v>122</v>
-      </c>
-      <c r="B39" t="s">
-        <v>123</v>
-      </c>
-      <c r="C39" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" t="s">
-        <v>6</v>
-      </c>
-      <c r="E39" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" t="s">
-        <v>125</v>
-      </c>
-      <c r="B40" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40" t="s">
-        <v>47</v>
-      </c>
-      <c r="D40" t="s">
-        <v>3</v>
-      </c>
-      <c r="E40" t="s">
-        <v>52</v>
-      </c>
-      <c r="G40" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" t="s">
-        <v>125</v>
-      </c>
-      <c r="B41" t="s">
-        <v>161</v>
-      </c>
-      <c r="C41" t="s">
-        <v>53</v>
-      </c>
-      <c r="D41" t="s">
-        <v>6</v>
-      </c>
-      <c r="E41" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" t="s">
-        <v>126</v>
-      </c>
-      <c r="B42" t="s">
-        <v>162</v>
-      </c>
-      <c r="C42" t="s">
-        <v>55</v>
-      </c>
-      <c r="D42" t="s">
-        <v>40</v>
-      </c>
-      <c r="E42" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" t="s">
-        <v>127</v>
-      </c>
-      <c r="B43" t="s">
-        <v>81</v>
-      </c>
-      <c r="C43" t="s">
-        <v>57</v>
-      </c>
-      <c r="D43" t="s">
-        <v>3</v>
-      </c>
-      <c r="E43" t="s">
-        <v>128</v>
-      </c>
-      <c r="G43" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" t="s">
-        <v>127</v>
-      </c>
-      <c r="B44" t="s">
-        <v>158</v>
-      </c>
-      <c r="C44" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" t="s">
-        <v>6</v>
-      </c>
-      <c r="E44" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" t="s">
-        <v>213</v>
-      </c>
-      <c r="B45" t="s">
-        <v>130</v>
-      </c>
-      <c r="C45" t="s">
-        <v>58</v>
-      </c>
-      <c r="D45" t="s">
-        <v>59</v>
-      </c>
-      <c r="E45" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" t="s">
-        <v>129</v>
-      </c>
-      <c r="B46" t="s">
-        <v>31</v>
-      </c>
-      <c r="C46" t="s">
-        <v>169</v>
-      </c>
-      <c r="D46" t="s">
-        <v>3</v>
-      </c>
-      <c r="E46" t="s">
-        <v>8</v>
-      </c>
-      <c r="G46" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" t="s">
+      <c r="B48" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" t="s">
-        <v>131</v>
-      </c>
-      <c r="B48" t="s">
-        <v>183</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
@@ -2372,15 +2432,15 @@
         <v>3</v>
       </c>
       <c r="E48" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G48" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>170</v>
+        <v>130</v>
       </c>
       <c r="B49" t="s">
         <v>61</v>
@@ -2395,12 +2455,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>132</v>
+        <v>169</v>
       </c>
       <c r="B50" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C50" t="s">
         <v>70</v>
@@ -2409,15 +2469,15 @@
         <v>59</v>
       </c>
       <c r="E50" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B51" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C51" t="s">
         <v>42</v>
@@ -2429,15 +2489,15 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B52" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C52" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D52" t="s">
         <v>59</v>
@@ -2446,9 +2506,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B53" t="s">
         <v>86</v>
@@ -2460,12 +2520,12 @@
         <v>6</v>
       </c>
       <c r="E53" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
-      <c r="A54" t="s">
-        <v>137</v>
       </c>
       <c r="B54" t="s">
         <v>66</v>
@@ -2477,12 +2537,12 @@
         <v>59</v>
       </c>
       <c r="E54" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>136</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="A55" t="s">
-        <v>139</v>
       </c>
       <c r="B55" t="s">
         <v>63</v>
@@ -2494,12 +2554,12 @@
         <v>59</v>
       </c>
       <c r="E55" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>138</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
-      <c r="A56" t="s">
-        <v>140</v>
       </c>
       <c r="B56" t="s">
         <v>89</v>
@@ -2514,12 +2574,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B57" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C57" t="s">
         <v>34</v>
@@ -2531,12 +2591,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B58" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C58" t="s">
         <v>67</v>
@@ -2548,9 +2608,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B59" t="s">
         <v>72</v>
@@ -2565,9 +2625,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>145</v>
+      </c>
       <c r="B60" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C60" t="s">
         <v>67</v>
@@ -2579,14 +2642,14 @@
         <v>68</v>
       </c>
       <c r="G60" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="78" ht="13.5" customHeight="1"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="78" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="https://www.fsgt.org/activites/velo/epreuves/cyclo-cross-championnat-national-fsgt-des-22-et-23-janvier-2022"/>
-    <hyperlink ref="E16" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId1" display="https://www.fsgt.org/activites/velo/epreuves/cyclo-cross-championnat-national-fsgt-des-22-et-23-janvier-2022" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId3"/>

</xml_diff>

<commit_message>
classements divers en ligne
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caroline\Documents\68-FSGT-Cyclisme-Alsace\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56FBCAA-355E-47ED-9869-F9B46AA43BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendrier" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="224">
   <si>
     <t>Date</t>
   </si>
@@ -680,13 +686,19 @@
   </si>
   <si>
     <t>champduf_marathon</t>
+  </si>
+  <si>
+    <t>https://www.sporkrono.fr/2022-resultats-champduf/</t>
+  </si>
+  <si>
+    <t>https://www.tempustiming.fr/resultats-juillet-2022/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1175,9 +1187,10 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1207,12 +1220,12 @@
     <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Commentaire" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Lien hypertexte" xfId="42" builtinId="8"/>
     <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -1280,7 +1293,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1312,9 +1325,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1346,6 +1377,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1521,14 +1570,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="67.42578125" customWidth="1"/>
@@ -1538,7 +1587,7 @@
     <col min="7" max="7" width="51.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1561,7 +1610,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>90</v>
       </c>
@@ -1578,7 +1627,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>146</v>
       </c>
@@ -1595,7 +1644,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -1615,7 +1664,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -1632,7 +1681,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -1652,7 +1701,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>202</v>
       </c>
@@ -1669,7 +1718,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>96</v>
       </c>
@@ -1689,7 +1738,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>173</v>
       </c>
@@ -1706,7 +1755,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -1726,7 +1775,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>152</v>
       </c>
@@ -1743,7 +1792,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>152</v>
       </c>
@@ -1763,7 +1812,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>152</v>
       </c>
@@ -1780,7 +1829,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>101</v>
       </c>
@@ -1797,7 +1846,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>101</v>
       </c>
@@ -1817,7 +1866,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>103</v>
       </c>
@@ -1837,7 +1886,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>172</v>
       </c>
@@ -1857,7 +1906,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>172</v>
       </c>
@@ -1874,7 +1923,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>105</v>
       </c>
@@ -1894,7 +1943,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>106</v>
       </c>
@@ -1911,7 +1960,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>106</v>
       </c>
@@ -1928,7 +1977,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>212</v>
       </c>
@@ -1945,7 +1994,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>183</v>
       </c>
@@ -1962,7 +2011,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>183</v>
       </c>
@@ -1975,14 +2024,17 @@
       <c r="D24" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="2" t="s">
         <v>221</v>
+      </c>
+      <c r="F24" t="s">
+        <v>222</v>
       </c>
       <c r="G24" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>108</v>
       </c>
@@ -1995,8 +2047,11 @@
       <c r="E25" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="F25" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>109</v>
       </c>
@@ -2016,7 +2071,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>109</v>
       </c>
@@ -2033,7 +2088,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>109</v>
       </c>
@@ -2050,7 +2105,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>111</v>
       </c>
@@ -2070,7 +2125,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>111</v>
       </c>
@@ -2090,7 +2145,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>174</v>
       </c>
@@ -2107,7 +2162,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>112</v>
       </c>
@@ -2127,7 +2182,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>113</v>
       </c>
@@ -2147,7 +2202,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>153</v>
       </c>
@@ -2164,7 +2219,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>117</v>
       </c>
@@ -2181,7 +2236,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>162</v>
       </c>
@@ -2201,7 +2256,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>118</v>
       </c>
@@ -2221,7 +2276,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>120</v>
       </c>
@@ -2238,7 +2293,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="14.25" customHeight="1">
+    <row r="39" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>120</v>
       </c>
@@ -2258,7 +2313,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>121</v>
       </c>
@@ -2275,7 +2330,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>124</v>
       </c>
@@ -2295,7 +2350,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>124</v>
       </c>
@@ -2312,7 +2367,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>219</v>
       </c>
@@ -2329,7 +2384,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>125</v>
       </c>
@@ -2346,7 +2401,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>126</v>
       </c>
@@ -2366,7 +2421,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>126</v>
       </c>
@@ -2383,7 +2438,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>210</v>
       </c>
@@ -2400,7 +2455,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>128</v>
       </c>
@@ -2420,7 +2475,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>180</v>
       </c>
@@ -2440,7 +2495,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>130</v>
       </c>
@@ -2457,7 +2512,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>169</v>
       </c>
@@ -2474,7 +2529,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>131</v>
       </c>
@@ -2491,7 +2546,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>132</v>
       </c>
@@ -2508,7 +2563,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>132</v>
       </c>
@@ -2525,7 +2580,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>134</v>
       </c>
@@ -2542,7 +2597,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>136</v>
       </c>
@@ -2559,7 +2614,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>138</v>
       </c>
@@ -2576,7 +2631,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>139</v>
       </c>
@@ -2593,7 +2648,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>142</v>
       </c>
@@ -2610,7 +2665,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>144</v>
       </c>
@@ -2627,7 +2682,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>145</v>
       </c>
@@ -2647,14 +2702,13 @@
         <v>147</v>
       </c>
     </row>
-    <row r="79" ht="13.5" customHeight="1"/>
+    <row r="79" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="https://www.fsgt.org/activites/velo/epreuves/cyclo-cross-championnat-national-fsgt-des-22-et-23-janvier-2022"/>
-    <hyperlink ref="E16" r:id="rId2"/>
-    <hyperlink ref="E24" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId1" display="https://www.fsgt.org/activites/velo/epreuves/cyclo-cross-championnat-national-fsgt-des-22-et-23-janvier-2022" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
retour du classement du marathon
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caroline\Documents\68-FSGT-Cyclisme-Alsace\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEFDB2D-FA5C-4A5F-BC2B-B4F6B409A1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendrier" sheetId="1" r:id="rId1"/>
@@ -685,8 +691,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1207,12 +1213,12 @@
     <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Commentaire" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Lien hypertexte" xfId="42" builtinId="8"/>
     <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -1280,7 +1286,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1312,9 +1318,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1346,6 +1370,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1521,14 +1563,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="67.42578125" customWidth="1"/>
@@ -1538,7 +1580,7 @@
     <col min="7" max="7" width="51.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1561,7 +1603,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>90</v>
       </c>
@@ -1578,7 +1620,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>146</v>
       </c>
@@ -1595,7 +1637,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -1615,7 +1657,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -1632,7 +1674,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -1652,7 +1694,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>202</v>
       </c>
@@ -1669,7 +1711,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>96</v>
       </c>
@@ -1689,7 +1731,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>173</v>
       </c>
@@ -1706,7 +1748,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -1726,7 +1768,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>152</v>
       </c>
@@ -1743,7 +1785,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>152</v>
       </c>
@@ -1763,7 +1805,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>152</v>
       </c>
@@ -1780,7 +1822,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>101</v>
       </c>
@@ -1797,7 +1839,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>101</v>
       </c>
@@ -1817,7 +1859,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>103</v>
       </c>
@@ -1837,7 +1879,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>172</v>
       </c>
@@ -1857,7 +1899,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>172</v>
       </c>
@@ -1874,7 +1916,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>105</v>
       </c>
@@ -1894,7 +1936,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>106</v>
       </c>
@@ -1911,7 +1953,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>106</v>
       </c>
@@ -1928,7 +1970,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>212</v>
       </c>
@@ -1945,7 +1987,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>183</v>
       </c>
@@ -1962,7 +2004,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>183</v>
       </c>
@@ -1975,14 +2017,14 @@
       <c r="D24" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>221</v>
       </c>
       <c r="G24" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>108</v>
       </c>
@@ -1996,7 +2038,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>109</v>
       </c>
@@ -2016,7 +2058,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>109</v>
       </c>
@@ -2033,7 +2075,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>109</v>
       </c>
@@ -2050,7 +2092,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>111</v>
       </c>
@@ -2070,7 +2112,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>111</v>
       </c>
@@ -2090,7 +2132,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>174</v>
       </c>
@@ -2107,7 +2149,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>112</v>
       </c>
@@ -2127,7 +2169,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>113</v>
       </c>
@@ -2147,7 +2189,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>153</v>
       </c>
@@ -2164,7 +2206,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>117</v>
       </c>
@@ -2181,7 +2223,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>162</v>
       </c>
@@ -2201,7 +2243,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>118</v>
       </c>
@@ -2221,7 +2263,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>120</v>
       </c>
@@ -2238,7 +2280,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="14.25" customHeight="1">
+    <row r="39" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>120</v>
       </c>
@@ -2258,7 +2300,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>121</v>
       </c>
@@ -2275,7 +2317,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>124</v>
       </c>
@@ -2295,7 +2337,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>124</v>
       </c>
@@ -2312,7 +2354,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>219</v>
       </c>
@@ -2329,7 +2371,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>125</v>
       </c>
@@ -2346,7 +2388,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>126</v>
       </c>
@@ -2366,7 +2408,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>126</v>
       </c>
@@ -2383,7 +2425,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>210</v>
       </c>
@@ -2400,7 +2442,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>128</v>
       </c>
@@ -2420,7 +2462,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>180</v>
       </c>
@@ -2440,7 +2482,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>130</v>
       </c>
@@ -2457,7 +2499,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>169</v>
       </c>
@@ -2474,7 +2516,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>131</v>
       </c>
@@ -2491,7 +2533,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>132</v>
       </c>
@@ -2508,7 +2550,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>132</v>
       </c>
@@ -2525,7 +2567,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>134</v>
       </c>
@@ -2542,7 +2584,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>136</v>
       </c>
@@ -2559,7 +2601,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>138</v>
       </c>
@@ -2576,7 +2618,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>139</v>
       </c>
@@ -2593,7 +2635,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>142</v>
       </c>
@@ -2610,7 +2652,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>144</v>
       </c>
@@ -2627,7 +2669,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>145</v>
       </c>
@@ -2647,12 +2689,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="79" ht="13.5" customHeight="1"/>
+    <row r="79" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="https://www.fsgt.org/activites/velo/epreuves/cyclo-cross-championnat-national-fsgt-des-22-et-23-janvier-2022"/>
-    <hyperlink ref="E16" r:id="rId2"/>
-    <hyperlink ref="E24" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId1" display="https://www.fsgt.org/activites/velo/epreuves/cyclo-cross-championnat-national-fsgt-des-22-et-23-janvier-2022" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F24" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId4"/>

</xml_diff>

<commit_message>
Classements 3h vtt altkirch
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caroline\Documents\68-FSGT-Cyclisme-Alsace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D18B98-5A7B-4A2F-9BCF-D80A4D427436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2736414-76B4-439C-8DFA-A46DB5709D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="196">
   <si>
     <t>Date</t>
   </si>
@@ -1488,8 +1488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2104,9 +2104,6 @@
       <c r="D33" t="s">
         <v>38</v>
       </c>
-      <c r="E33" t="s">
-        <v>192</v>
-      </c>
       <c r="G33" t="s">
         <v>181</v>
       </c>

</xml_diff>

<commit_message>
cyclotour alsace et bernwiller
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caroline\Documents\68-FSGT-Cyclisme-Alsace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4643A38-9297-46EE-BA87-1A2EEFA49050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D64EEB-4B96-426B-9DF6-433622A4D743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="202">
   <si>
     <t>Date</t>
   </si>
@@ -611,6 +611,21 @@
   </si>
   <si>
     <t>waldbach</t>
+  </si>
+  <si>
+    <t>bernwiller</t>
+  </si>
+  <si>
+    <t>L'étape Cyclo du Tour</t>
+  </si>
+  <si>
+    <t>Tour Alsace &amp; FSGT</t>
+  </si>
+  <si>
+    <t>cyclotouralsace</t>
+  </si>
+  <si>
+    <t>Sam 30 Juillet</t>
   </si>
 </sst>
 </file>
@@ -1489,10 +1504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2130,130 +2145,127 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>96</v>
+        <v>201</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>198</v>
       </c>
       <c r="C35" t="s">
-        <v>41</v>
+        <v>199</v>
       </c>
       <c r="D35" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="E35" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>134</v>
+        <v>96</v>
       </c>
       <c r="B36" t="s">
-        <v>135</v>
+        <v>40</v>
       </c>
       <c r="C36" t="s">
-        <v>136</v>
+        <v>41</v>
       </c>
       <c r="D36" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="E36" t="s">
-        <v>191</v>
-      </c>
-      <c r="G36" t="s">
-        <v>142</v>
+        <v>196</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>97</v>
+        <v>134</v>
       </c>
       <c r="B37" t="s">
-        <v>98</v>
+        <v>135</v>
       </c>
       <c r="C37" t="s">
-        <v>23</v>
+        <v>136</v>
       </c>
       <c r="D37" t="s">
         <v>6</v>
       </c>
       <c r="E37" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="G37" t="s">
-        <v>185</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B38" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="C38" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D38" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="E38" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+      <c r="G38" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>99</v>
       </c>
       <c r="B39" t="s">
+        <v>129</v>
+      </c>
+      <c r="C39" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>99</v>
+      </c>
+      <c r="B40" t="s">
         <v>149</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>10</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>3</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G40" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>100</v>
-      </c>
-      <c r="B40" t="s">
-        <v>101</v>
-      </c>
-      <c r="C40" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" t="s">
-        <v>6</v>
-      </c>
-      <c r="E40" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>101</v>
       </c>
       <c r="C41" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E41" t="s">
         <v>191</v>
-      </c>
-      <c r="G41" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2261,27 +2273,30 @@
         <v>102</v>
       </c>
       <c r="B42" t="s">
-        <v>132</v>
+        <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D42" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E42" t="s">
         <v>191</v>
       </c>
+      <c r="G42" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>187</v>
+        <v>102</v>
       </c>
       <c r="B43" t="s">
-        <v>186</v>
+        <v>132</v>
       </c>
       <c r="C43" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="D43" t="s">
         <v>6</v>
@@ -2292,16 +2307,16 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>103</v>
+        <v>187</v>
       </c>
       <c r="B44" t="s">
-        <v>133</v>
+        <v>186</v>
       </c>
       <c r="C44" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="D44" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="E44" t="s">
         <v>191</v>
@@ -2309,127 +2324,127 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B45" t="s">
-        <v>63</v>
+        <v>133</v>
       </c>
       <c r="C45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D45" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="E45" t="s">
         <v>191</v>
       </c>
-      <c r="G45" t="s">
-        <v>185</v>
-      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>179</v>
+        <v>104</v>
       </c>
       <c r="B46" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="C46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D46" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="E46" t="s">
         <v>191</v>
       </c>
+      <c r="G46" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>105</v>
+        <v>179</v>
       </c>
       <c r="B47" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
       <c r="C47" t="s">
-        <v>139</v>
+        <v>47</v>
       </c>
       <c r="D47" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="E47" t="s">
         <v>191</v>
       </c>
-      <c r="G47" t="s">
-        <v>141</v>
-      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>190</v>
+        <v>105</v>
       </c>
       <c r="B48" t="s">
-        <v>192</v>
+        <v>29</v>
       </c>
       <c r="C48" t="s">
-        <v>8</v>
+        <v>139</v>
       </c>
       <c r="D48" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E48" t="s">
         <v>191</v>
       </c>
+      <c r="G48" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>150</v>
+        <v>190</v>
       </c>
       <c r="B49" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="C49" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D49" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E49" t="s">
         <v>191</v>
       </c>
-      <c r="G49" t="s">
-        <v>141</v>
-      </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>107</v>
+        <v>150</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
+        <v>151</v>
       </c>
       <c r="C50" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D50" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E50" t="s">
         <v>191</v>
       </c>
+      <c r="G50" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>140</v>
+        <v>107</v>
       </c>
       <c r="B51" t="s">
-        <v>131</v>
+        <v>49</v>
       </c>
       <c r="C51" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="D51" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E51" t="s">
         <v>191</v>
@@ -2437,13 +2452,13 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="B52" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="C52" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="D52" t="s">
         <v>48</v>
@@ -2454,13 +2469,13 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B53" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C53" t="s">
-        <v>148</v>
+        <v>39</v>
       </c>
       <c r="D53" t="s">
         <v>48</v>
@@ -2474,41 +2489,41 @@
         <v>109</v>
       </c>
       <c r="B54" t="s">
-        <v>67</v>
+        <v>130</v>
       </c>
       <c r="C54" t="s">
-        <v>51</v>
+        <v>148</v>
       </c>
       <c r="D54" t="s">
-        <v>6</v>
+        <v>48</v>
+      </c>
+      <c r="E54" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B55" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="C55" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="D55" t="s">
-        <v>48</v>
-      </c>
-      <c r="E55" t="s">
-        <v>191</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B56" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C56" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D56" t="s">
         <v>48</v>
@@ -2519,13 +2534,13 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B57" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="C57" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="D57" t="s">
         <v>48</v>
@@ -2536,10 +2551,10 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B58" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C58" t="s">
         <v>32</v>
@@ -2553,13 +2568,13 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B59" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C59" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="D59" t="s">
         <v>48</v>
@@ -2570,13 +2585,13 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B60" t="s">
-        <v>55</v>
+        <v>116</v>
       </c>
       <c r="C60" t="s">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="D60" t="s">
         <v>48</v>
@@ -2587,13 +2602,13 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B61" t="s">
-        <v>123</v>
+        <v>55</v>
       </c>
       <c r="C61" t="s">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="D61" t="s">
         <v>48</v>
@@ -2601,11 +2616,28 @@
       <c r="E61" t="s">
         <v>191</v>
       </c>
-      <c r="G61" t="s">
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>118</v>
+      </c>
+      <c r="B62" t="s">
+        <v>123</v>
+      </c>
+      <c r="C62" t="s">
+        <v>53</v>
+      </c>
+      <c r="D62" t="s">
+        <v>48</v>
+      </c>
+      <c r="E62" t="s">
+        <v>191</v>
+      </c>
+      <c r="G62" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="79" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" display="https://www.fsgt.org/activites/velo/epreuves/cyclo-cross-championnat-national-fsgt-des-22-et-23-janvier-2022" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
avec la bonne modif excel
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caroline\Documents\68-FSGT-Cyclisme-Alsace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE689C71-08A0-484C-BBEE-AB1775C1290C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62FB681-E7D3-4B47-AB24-B4E2956D30F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1518,8 +1518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="C33" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2504,7 +2504,7 @@
       <c r="D53" t="s">
         <v>6</v>
       </c>
-      <c r="E53" t="s">
+      <c r="G53" t="s">
         <v>176</v>
       </c>
     </row>

</xml_diff>

<commit_message>
un tas de nouveau classement depuis autre pc
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FlorianKohler\Desktop\PRIVE\Sites\68-FSGT-Cyclisme-Alsace\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038A3056-D82C-4896-834C-2B180929DDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendrier" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="218">
   <si>
     <t>Date</t>
   </si>
@@ -647,13 +653,34 @@
   </si>
   <si>
     <t>morschwiller</t>
+  </si>
+  <si>
+    <t>morschwiller_vtt</t>
+  </si>
+  <si>
+    <t>heimsbrunn_cx</t>
+  </si>
+  <si>
+    <t>wittenheim</t>
+  </si>
+  <si>
+    <t>blaesheim</t>
+  </si>
+  <si>
+    <t>technochape</t>
+  </si>
+  <si>
+    <t>boron</t>
+  </si>
+  <si>
+    <t>Frotey_clm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1174,12 +1201,12 @@
     <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Commentaire" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Lien hypertexte" xfId="42" builtinId="8"/>
     <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -1247,7 +1274,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1279,9 +1306,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1313,6 +1358,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1488,24 +1551,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="67.42578125" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.81640625" customWidth="1"/>
+    <col min="2" max="2" width="67.453125" customWidth="1"/>
+    <col min="3" max="3" width="24.26953125" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="42.7109375" customWidth="1"/>
-    <col min="7" max="7" width="51.85546875" customWidth="1"/>
+    <col min="6" max="6" width="42.7265625" customWidth="1"/>
+    <col min="7" max="7" width="51.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1528,7 +1591,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -1545,7 +1608,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -1562,7 +1625,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>71</v>
       </c>
@@ -1582,7 +1645,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>72</v>
       </c>
@@ -1599,7 +1662,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -1619,7 +1682,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>161</v>
       </c>
@@ -1636,7 +1699,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>74</v>
       </c>
@@ -1656,7 +1719,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>136</v>
       </c>
@@ -1673,7 +1736,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>76</v>
       </c>
@@ -1693,7 +1756,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -1710,7 +1773,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>118</v>
       </c>
@@ -1730,7 +1793,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -1747,7 +1810,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -1764,7 +1827,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>79</v>
       </c>
@@ -1784,7 +1847,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -1804,7 +1867,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>135</v>
       </c>
@@ -1824,7 +1887,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>135</v>
       </c>
@@ -1841,7 +1904,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -1861,7 +1924,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>84</v>
       </c>
@@ -1878,7 +1941,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>84</v>
       </c>
@@ -1895,7 +1958,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>171</v>
       </c>
@@ -1912,7 +1975,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>142</v>
       </c>
@@ -1929,7 +1992,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>142</v>
       </c>
@@ -1949,7 +2012,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>86</v>
       </c>
@@ -1963,7 +2026,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>87</v>
       </c>
@@ -1983,7 +2046,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>87</v>
       </c>
@@ -2000,7 +2063,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>87</v>
       </c>
@@ -2017,7 +2080,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>89</v>
       </c>
@@ -2037,7 +2100,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>89</v>
       </c>
@@ -2057,7 +2120,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>137</v>
       </c>
@@ -2074,7 +2137,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>90</v>
       </c>
@@ -2094,7 +2157,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>91</v>
       </c>
@@ -2111,7 +2174,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>119</v>
       </c>
@@ -2128,7 +2191,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>191</v>
       </c>
@@ -2145,7 +2208,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>94</v>
       </c>
@@ -2162,7 +2225,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>126</v>
       </c>
@@ -2182,7 +2245,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>95</v>
       </c>
@@ -2202,7 +2265,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>97</v>
       </c>
@@ -2222,7 +2285,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="14.25" customHeight="1">
+    <row r="40" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>97</v>
       </c>
@@ -2239,7 +2302,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -2256,7 +2319,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>100</v>
       </c>
@@ -2273,7 +2336,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>100</v>
       </c>
@@ -2287,10 +2350,10 @@
         <v>6</v>
       </c>
       <c r="E43" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>177</v>
       </c>
@@ -2310,7 +2373,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>177</v>
       </c>
@@ -2324,10 +2387,10 @@
         <v>6</v>
       </c>
       <c r="E45" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>101</v>
       </c>
@@ -2344,7 +2407,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>169</v>
       </c>
@@ -2358,13 +2421,13 @@
         <v>47</v>
       </c>
       <c r="E47" t="s">
-        <v>181</v>
+        <v>213</v>
       </c>
       <c r="G47" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>102</v>
       </c>
@@ -2378,13 +2441,13 @@
         <v>3</v>
       </c>
       <c r="E48" t="s">
-        <v>181</v>
+        <v>215</v>
       </c>
       <c r="G48" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>180</v>
       </c>
@@ -2404,7 +2467,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>140</v>
       </c>
@@ -2424,7 +2487,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>103</v>
       </c>
@@ -2444,7 +2507,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>132</v>
       </c>
@@ -2458,13 +2521,13 @@
         <v>47</v>
       </c>
       <c r="E52" t="s">
-        <v>181</v>
+        <v>214</v>
       </c>
       <c r="G52" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>199</v>
       </c>
@@ -2481,7 +2544,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>203</v>
       </c>
@@ -2498,7 +2561,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>203</v>
       </c>
@@ -2512,10 +2575,10 @@
         <v>3</v>
       </c>
       <c r="E55" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>209</v>
       </c>
@@ -2529,10 +2592,10 @@
         <v>47</v>
       </c>
       <c r="E56" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>104</v>
       </c>
@@ -2549,7 +2612,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>206</v>
       </c>
@@ -2569,7 +2632,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>105</v>
       </c>
@@ -2586,7 +2649,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>106</v>
       </c>
@@ -2603,7 +2666,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>108</v>
       </c>
@@ -2623,7 +2686,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>110</v>
       </c>
@@ -2640,7 +2703,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>111</v>
       </c>
@@ -2660,12 +2723,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="81" ht="13.5" customHeight="1"/>
+    <row r="81" ht="13.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="https://www.fsgt.org/activites/velo/epreuves/cyclo-cross-championnat-national-fsgt-des-22-et-23-janvier-2022"/>
-    <hyperlink ref="E16" r:id="rId2"/>
-    <hyperlink ref="F24" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId1" display="https://www.fsgt.org/activites/velo/epreuves/cyclo-cross-championnat-national-fsgt-des-22-et-23-janvier-2022" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F24" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId4"/>

</xml_diff>

<commit_message>
2023 remplace par 2023*
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\Documents\68-FSGT-Cyclisme-Alsace\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8DCD70-2F46-4E3F-A6FD-0EC95CF06AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendrier" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="146">
   <si>
     <t>Date</t>
   </si>
@@ -405,9 +411,6 @@
     <t>Reiningue</t>
   </si>
   <si>
-    <t>Critérium National VTT Cross-Country Marathon, La Champduf 2022 (Belmont)</t>
-  </si>
-  <si>
     <t>La Champduf 2023 (Belmont)</t>
   </si>
   <si>
@@ -454,13 +457,19 @@
   </si>
   <si>
     <t>VC Ste Marie aux Mines</t>
+  </si>
+  <si>
+    <t>frotey</t>
+  </si>
+  <si>
+    <t>Critérium National VTT Cross-Country Marathon, La Champduf 2023 (Belmont)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -808,33 +817,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="67.42578125" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="67.44140625" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="42.7109375" customWidth="1"/>
-    <col min="7" max="7" width="51.7109375" customWidth="1"/>
-    <col min="8" max="1025" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="42.6640625" customWidth="1"/>
+    <col min="7" max="7" width="51.6640625" customWidth="1"/>
+    <col min="8" max="1025" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -857,21 +866,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" t="s">
         <v>132</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>133</v>
-      </c>
-      <c r="C2" t="s">
-        <v>134</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -888,7 +897,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -902,7 +911,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -919,7 +928,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -936,7 +945,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>77</v>
       </c>
@@ -950,7 +959,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -964,7 +973,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>81</v>
       </c>
@@ -978,7 +987,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>82</v>
       </c>
@@ -995,12 +1004,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>83</v>
       </c>
       <c r="B11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C11" t="s">
         <v>23</v>
@@ -1009,10 +1018,10 @@
         <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>84</v>
       </c>
@@ -1029,7 +1038,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>85</v>
       </c>
@@ -1049,7 +1058,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>124</v>
       </c>
@@ -1066,12 +1075,12 @@
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>87</v>
       </c>
       <c r="B15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
@@ -1083,7 +1092,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>88</v>
       </c>
@@ -1100,23 +1109,23 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17" t="s">
         <v>135</v>
-      </c>
-      <c r="B17" t="s">
-        <v>136</v>
       </c>
       <c r="D17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>89</v>
       </c>
       <c r="B18" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="C18" t="s">
         <v>36</v>
@@ -1126,12 +1135,12 @@
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>90</v>
       </c>
       <c r="B19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C19" t="s">
         <v>36</v>
@@ -1140,7 +1149,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>126</v>
       </c>
@@ -1154,18 +1163,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>92</v>
       </c>
       <c r="B21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>91</v>
       </c>
@@ -1179,7 +1188,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>93</v>
       </c>
@@ -1196,7 +1205,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -1213,7 +1222,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="14.25" customHeight="1">
+    <row r="25" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>96</v>
       </c>
@@ -1221,13 +1230,13 @@
         <v>97</v>
       </c>
       <c r="C25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D25" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -1244,7 +1253,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -1261,7 +1270,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -1278,7 +1287,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>103</v>
       </c>
@@ -1295,12 +1304,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>104</v>
       </c>
       <c r="B30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
@@ -1312,21 +1321,21 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B31" t="s">
         <v>105</v>
       </c>
       <c r="C31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D31" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>106</v>
       </c>
@@ -1343,7 +1352,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>108</v>
       </c>
@@ -1360,12 +1369,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>109</v>
       </c>
       <c r="B34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C34" t="s">
         <v>57</v>
@@ -1377,7 +1386,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>110</v>
       </c>
@@ -1394,7 +1403,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>111</v>
       </c>
@@ -1411,7 +1420,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>112</v>
       </c>
@@ -1428,12 +1437,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>113</v>
       </c>
       <c r="B38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C38" t="s">
         <v>28</v>
@@ -1442,7 +1451,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>114</v>
       </c>
@@ -1459,7 +1468,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>115</v>
       </c>
@@ -1473,9 +1482,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B41" t="s">
         <v>63</v>
@@ -1490,7 +1499,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>118</v>
       </c>
@@ -1510,7 +1519,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>121</v>
       </c>
@@ -1524,7 +1533,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>120</v>
       </c>
@@ -1538,7 +1547,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" ht="13.5" customHeight="1"/>
+    <row r="61" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Maj reglement 2023 et randos
</commit_message>
<xml_diff>
--- a/Calendrier.xlsx
+++ b/Calendrier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\Documents\68-FSGT-Cyclisme-Alsace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E38FE26-25CE-4AB8-808F-B031A740A963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41C9C9A-A944-46D6-9F66-A145177BB200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="159">
   <si>
     <t>Date</t>
   </si>
@@ -487,6 +487,21 @@
   </si>
   <si>
     <t>seppois</t>
+  </si>
+  <si>
+    <t>8&lt;sup&gt;e&lt;/sup&gt; Rando Tour Wagner &amp; Associés</t>
+  </si>
+  <si>
+    <t>VC Sainte-Croix-en-Plaine</t>
+  </si>
+  <si>
+    <t>rando_vcscp</t>
+  </si>
+  <si>
+    <t>challengeballons</t>
+  </si>
+  <si>
+    <t>Petit Ballon Challenges</t>
   </si>
 </sst>
 </file>
@@ -849,10 +864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1192,39 +1207,38 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>125</v>
+        <v>81</v>
       </c>
       <c r="B20" t="s">
-        <v>126</v>
+        <v>154</v>
+      </c>
+      <c r="C20" t="s">
+        <v>155</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="E20" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="B21" t="s">
-        <v>136</v>
-      </c>
-      <c r="C21" t="s">
-        <v>32</v>
+        <v>126</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="1"/>
-      <c r="G21" t="s">
-        <v>140</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B22" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C22" t="s">
         <v>32</v>
@@ -1232,22 +1246,23 @@
       <c r="D22" t="s">
         <v>11</v>
       </c>
+      <c r="F22" s="1"/>
       <c r="G22" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>118</v>
+        <v>83</v>
       </c>
       <c r="B23" t="s">
-        <v>119</v>
+        <v>148</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G23" t="s">
         <v>140</v>
@@ -1255,304 +1270,307 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B24" t="s">
-        <v>130</v>
+        <v>158</v>
+      </c>
+      <c r="C24" t="s">
+        <v>155</v>
       </c>
       <c r="D24" t="s">
         <v>17</v>
       </c>
+      <c r="E24" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>119</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="D25" t="s">
         <v>13</v>
       </c>
+      <c r="G25" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>137</v>
+        <v>85</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
-      </c>
-      <c r="C26" t="s">
-        <v>16</v>
+        <v>130</v>
       </c>
       <c r="D26" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D27" t="s">
         <v>13</v>
       </c>
-      <c r="E27" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>137</v>
       </c>
       <c r="B28" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="D28" t="s">
         <v>13</v>
       </c>
       <c r="E28" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B29" t="s">
-        <v>90</v>
+        <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>129</v>
+        <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="E29" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B30" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C30" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D30" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="E30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B31" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="C31" t="s">
-        <v>7</v>
+        <v>129</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
       </c>
-      <c r="E31" t="s">
-        <v>48</v>
-      </c>
-      <c r="G31" t="s">
-        <v>140</v>
-      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D32" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="E32" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B33" t="s">
-        <v>121</v>
+        <v>47</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E33" t="s">
-        <v>41</v>
+        <v>48</v>
+      </c>
+      <c r="G33" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="B34" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="C34" t="s">
-        <v>134</v>
+        <v>45</v>
       </c>
       <c r="D34" t="s">
-        <v>33</v>
+        <v>8</v>
+      </c>
+      <c r="E34" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B35" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="C35" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D35" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E35" t="s">
-        <v>50</v>
-      </c>
-      <c r="G35" t="s">
-        <v>140</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="B36" t="s">
-        <v>51</v>
+        <v>97</v>
       </c>
       <c r="C36" t="s">
-        <v>29</v>
+        <v>134</v>
       </c>
       <c r="D36" t="s">
         <v>33</v>
       </c>
-      <c r="E36" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B37" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="C37" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E37" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="G37" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B38" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C38" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="D38" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="E38" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B39" t="s">
-        <v>58</v>
+        <v>128</v>
       </c>
       <c r="C39" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="D39" t="s">
         <v>8</v>
       </c>
       <c r="E39" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B40" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C40" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="D40" t="s">
         <v>8</v>
       </c>
       <c r="E40" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B41" t="s">
-        <v>132</v>
+        <v>58</v>
       </c>
       <c r="C41" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D41" t="s">
         <v>8</v>
       </c>
+      <c r="E41" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C42" t="s">
         <v>25</v>
@@ -1561,18 +1579,18 @@
         <v>8</v>
       </c>
       <c r="E42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B43" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="C43" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="D43" t="s">
         <v>8</v>
@@ -1580,70 +1598,101 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="B44" t="s">
-        <v>152</v>
+        <v>60</v>
       </c>
       <c r="C44" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D44" t="s">
         <v>8</v>
       </c>
       <c r="E44" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B45" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="C45" t="s">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="D45" t="s">
         <v>8</v>
       </c>
-      <c r="E45" t="s">
-        <v>67</v>
-      </c>
-      <c r="G45" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="B46" t="s">
-        <v>114</v>
+        <v>152</v>
       </c>
       <c r="C46" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="D46" t="s">
         <v>8</v>
       </c>
+      <c r="E46" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C47" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D47" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="64" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="E47" t="s">
+        <v>67</v>
+      </c>
+      <c r="G47" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" t="s">
+        <v>29</v>
+      </c>
+      <c r="D48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>112</v>
+      </c>
+      <c r="B49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>